<commit_message>
Added, updated and cleaned up translations
</commit_message>
<xml_diff>
--- a/assets/Localizations.xlsx
+++ b/assets/Localizations.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Grade.ly\Grade.ly - Flutter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Grade.ly\Grade.ly - Flutter\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9887EA5-C60A-477A-B09C-5B3A8F4E4967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73089631-C2B8-47C9-82A2-E2565FCDE833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -736,18 +736,6 @@
     <t>note_text</t>
   </si>
   <si>
-    <t>You can always edit your subjects in the settings later</t>
-  </si>
-  <si>
-    <t>Vous pouvez toujours modifier vos matières dans les paramètres ultérieurement</t>
-  </si>
-  <si>
-    <t>Sie können Ihre Fächer später immer noch in den Einstellungen bearbeiten</t>
-  </si>
-  <si>
-    <t>Dir kënnt är Fächer spéider ëmmer nach an den Astellungen beaarbechten</t>
-  </si>
-  <si>
     <t>open</t>
   </si>
   <si>
@@ -1400,6 +1388,18 @@
   </si>
   <si>
     <t>Ok</t>
+  </si>
+  <si>
+    <t>You can always edit your subjects and other options in the settings later</t>
+  </si>
+  <si>
+    <t>Vous pouvez toujours modifier vos matières et les autres options dans les paramètres plus tard</t>
+  </si>
+  <si>
+    <t>Sie können Ihre Fächer und andere Optionen später immer noch in den Einstellungen bearbeiten</t>
+  </si>
+  <si>
+    <t>Dir kënnt är Fächer an aner Optiounen spéider ëmmer nach an den Astellungen beaarbechten</t>
   </si>
 </sst>
 </file>
@@ -1767,8 +1767,8 @@
   </sheetPr>
   <dimension ref="A1:E113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="A77" sqref="A77"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="D76" sqref="D76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1799,19 +1799,19 @@
     </row>
     <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="B2" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="C2" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="D2" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E2" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2003,19 +2003,19 @@
     </row>
     <row r="14" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="B14" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="C14" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="D14" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="E14" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2054,53 +2054,53 @@
     </row>
     <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="B17" t="s">
+        <v>406</v>
+      </c>
+      <c r="C17" t="s">
         <v>410</v>
       </c>
-      <c r="C17" t="s">
-        <v>414</v>
-      </c>
       <c r="D17" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="E17" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>443</v>
+      </c>
+      <c r="B18" t="s">
+        <v>445</v>
+      </c>
+      <c r="C18" t="s">
+        <v>446</v>
+      </c>
+      <c r="D18" t="s">
+        <v>448</v>
+      </c>
+      <c r="E18" t="s">
         <v>447</v>
-      </c>
-      <c r="B18" t="s">
-        <v>449</v>
-      </c>
-      <c r="C18" t="s">
-        <v>450</v>
-      </c>
-      <c r="D18" t="s">
-        <v>452</v>
-      </c>
-      <c r="E18" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="B19" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="C19" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="D19" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="E19" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2139,19 +2139,19 @@
     </row>
     <row r="22" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="B22" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="C22" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="D22" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="E22" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2292,19 +2292,19 @@
     </row>
     <row r="31" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="B31" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="C31" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="D31" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="E31" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2377,19 +2377,19 @@
     </row>
     <row r="36" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="B36" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="C36" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="D36" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="E36" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2513,36 +2513,36 @@
     </row>
     <row r="44" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>364</v>
+      </c>
+      <c r="B44" t="s">
+        <v>365</v>
+      </c>
+      <c r="C44" t="s">
+        <v>366</v>
+      </c>
+      <c r="D44" t="s">
+        <v>367</v>
+      </c>
+      <c r="E44" t="s">
         <v>368</v>
-      </c>
-      <c r="B44" t="s">
-        <v>369</v>
-      </c>
-      <c r="C44" t="s">
-        <v>370</v>
-      </c>
-      <c r="D44" t="s">
-        <v>371</v>
-      </c>
-      <c r="E44" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="B45" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="C45" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="D45" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="E45" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2564,19 +2564,19 @@
     </row>
     <row r="47" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="B47" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="C47" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="D47" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="E47" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2768,19 +2768,19 @@
     </row>
     <row r="59" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="B59" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="C59" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="D59" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="E59" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2921,19 +2921,19 @@
     </row>
     <row r="68" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="B68" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="C68" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="D68" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="E68" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2955,36 +2955,36 @@
     </row>
     <row r="70" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>375</v>
+      </c>
+      <c r="B70" t="s">
+        <v>376</v>
+      </c>
+      <c r="C70" t="s">
+        <v>377</v>
+      </c>
+      <c r="D70" t="s">
+        <v>378</v>
+      </c>
+      <c r="E70" t="s">
         <v>379</v>
-      </c>
-      <c r="B70" t="s">
-        <v>380</v>
-      </c>
-      <c r="C70" t="s">
-        <v>381</v>
-      </c>
-      <c r="D70" t="s">
-        <v>382</v>
-      </c>
-      <c r="E70" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="B71" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="C71" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="D71" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="E71" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3006,36 +3006,36 @@
     </row>
     <row r="73" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>434</v>
+      </c>
+      <c r="B73" t="s">
+        <v>436</v>
+      </c>
+      <c r="C73" t="s">
         <v>438</v>
       </c>
-      <c r="B73" t="s">
+      <c r="D73" t="s">
         <v>440</v>
       </c>
-      <c r="C73" t="s">
+      <c r="E73" t="s">
         <v>442</v>
-      </c>
-      <c r="D73" t="s">
-        <v>444</v>
-      </c>
-      <c r="E73" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>380</v>
+      </c>
+      <c r="B74" t="s">
+        <v>381</v>
+      </c>
+      <c r="C74" t="s">
+        <v>382</v>
+      </c>
+      <c r="D74" t="s">
+        <v>383</v>
+      </c>
+      <c r="E74" t="s">
         <v>384</v>
-      </c>
-      <c r="B74" t="s">
-        <v>385</v>
-      </c>
-      <c r="C74" t="s">
-        <v>386</v>
-      </c>
-      <c r="D74" t="s">
-        <v>387</v>
-      </c>
-      <c r="E74" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3060,33 +3060,33 @@
         <v>236</v>
       </c>
       <c r="B76" t="s">
-        <v>237</v>
+        <v>455</v>
       </c>
       <c r="C76" t="s">
-        <v>238</v>
+        <v>456</v>
       </c>
       <c r="D76" t="s">
-        <v>239</v>
+        <v>457</v>
       </c>
       <c r="E76" t="s">
-        <v>240</v>
+        <v>458</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="B77" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="C77" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="D77" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="E77" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3108,36 +3108,36 @@
     </row>
     <row r="79" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B79" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C79" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="D79" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="E79" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>241</v>
+      </c>
+      <c r="B80" t="s">
+        <v>242</v>
+      </c>
+      <c r="C80" t="s">
+        <v>243</v>
+      </c>
+      <c r="D80" t="s">
+        <v>244</v>
+      </c>
+      <c r="E80" t="s">
         <v>245</v>
-      </c>
-      <c r="B80" t="s">
-        <v>246</v>
-      </c>
-      <c r="C80" t="s">
-        <v>247</v>
-      </c>
-      <c r="D80" t="s">
-        <v>248</v>
-      </c>
-      <c r="E80" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3159,240 +3159,240 @@
     </row>
     <row r="82" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>246</v>
+      </c>
+      <c r="B82" t="s">
+        <v>247</v>
+      </c>
+      <c r="C82" t="s">
+        <v>248</v>
+      </c>
+      <c r="D82" t="s">
+        <v>249</v>
+      </c>
+      <c r="E82" t="s">
         <v>250</v>
-      </c>
-      <c r="B82" t="s">
-        <v>251</v>
-      </c>
-      <c r="C82" t="s">
-        <v>252</v>
-      </c>
-      <c r="D82" t="s">
-        <v>253</v>
-      </c>
-      <c r="E82" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
+        <v>251</v>
+      </c>
+      <c r="B83" t="s">
+        <v>252</v>
+      </c>
+      <c r="C83" t="s">
+        <v>253</v>
+      </c>
+      <c r="D83" t="s">
+        <v>254</v>
+      </c>
+      <c r="E83" t="s">
         <v>255</v>
-      </c>
-      <c r="B83" t="s">
-        <v>256</v>
-      </c>
-      <c r="C83" t="s">
-        <v>257</v>
-      </c>
-      <c r="D83" t="s">
-        <v>258</v>
-      </c>
-      <c r="E83" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
+        <v>256</v>
+      </c>
+      <c r="B84" t="s">
+        <v>257</v>
+      </c>
+      <c r="C84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D84" t="s">
+        <v>259</v>
+      </c>
+      <c r="E84" t="s">
         <v>260</v>
-      </c>
-      <c r="B84" t="s">
-        <v>261</v>
-      </c>
-      <c r="C84" t="s">
-        <v>262</v>
-      </c>
-      <c r="D84" t="s">
-        <v>263</v>
-      </c>
-      <c r="E84" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
+        <v>261</v>
+      </c>
+      <c r="B85" t="s">
+        <v>262</v>
+      </c>
+      <c r="C85" t="s">
+        <v>263</v>
+      </c>
+      <c r="D85" t="s">
+        <v>264</v>
+      </c>
+      <c r="E85" t="s">
         <v>265</v>
-      </c>
-      <c r="B85" t="s">
-        <v>266</v>
-      </c>
-      <c r="C85" t="s">
-        <v>267</v>
-      </c>
-      <c r="D85" t="s">
-        <v>268</v>
-      </c>
-      <c r="E85" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
+        <v>266</v>
+      </c>
+      <c r="B86" t="s">
+        <v>267</v>
+      </c>
+      <c r="C86" t="s">
+        <v>268</v>
+      </c>
+      <c r="D86" t="s">
+        <v>269</v>
+      </c>
+      <c r="E86" t="s">
         <v>270</v>
-      </c>
-      <c r="B86" t="s">
-        <v>271</v>
-      </c>
-      <c r="C86" t="s">
-        <v>272</v>
-      </c>
-      <c r="D86" t="s">
-        <v>273</v>
-      </c>
-      <c r="E86" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
+        <v>271</v>
+      </c>
+      <c r="B87" t="s">
+        <v>272</v>
+      </c>
+      <c r="C87" t="s">
+        <v>273</v>
+      </c>
+      <c r="D87" t="s">
+        <v>274</v>
+      </c>
+      <c r="E87" t="s">
         <v>275</v>
-      </c>
-      <c r="B87" t="s">
-        <v>276</v>
-      </c>
-      <c r="C87" t="s">
-        <v>277</v>
-      </c>
-      <c r="D87" t="s">
-        <v>278</v>
-      </c>
-      <c r="E87" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
+        <v>276</v>
+      </c>
+      <c r="B88" t="s">
+        <v>277</v>
+      </c>
+      <c r="C88" t="s">
+        <v>278</v>
+      </c>
+      <c r="D88" t="s">
+        <v>279</v>
+      </c>
+      <c r="E88" t="s">
         <v>280</v>
-      </c>
-      <c r="B88" t="s">
-        <v>281</v>
-      </c>
-      <c r="C88" t="s">
-        <v>282</v>
-      </c>
-      <c r="D88" t="s">
-        <v>283</v>
-      </c>
-      <c r="E88" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="B89" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="C89" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="D89" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="E89" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
+        <v>281</v>
+      </c>
+      <c r="B90" t="s">
+        <v>282</v>
+      </c>
+      <c r="C90" t="s">
+        <v>283</v>
+      </c>
+      <c r="D90" t="s">
+        <v>284</v>
+      </c>
+      <c r="E90" t="s">
         <v>285</v>
-      </c>
-      <c r="B90" t="s">
-        <v>286</v>
-      </c>
-      <c r="C90" t="s">
-        <v>287</v>
-      </c>
-      <c r="D90" t="s">
-        <v>288</v>
-      </c>
-      <c r="E90" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="B91" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="C91" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="D91" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="E91" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B92" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="C92" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="D92" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="E92" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B93" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C93" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D93" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="E93" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
+        <v>296</v>
+      </c>
+      <c r="B94" t="s">
+        <v>297</v>
+      </c>
+      <c r="C94" t="s">
+        <v>298</v>
+      </c>
+      <c r="D94" t="s">
+        <v>299</v>
+      </c>
+      <c r="E94" t="s">
         <v>300</v>
-      </c>
-      <c r="B94" t="s">
-        <v>301</v>
-      </c>
-      <c r="C94" t="s">
-        <v>302</v>
-      </c>
-      <c r="D94" t="s">
-        <v>303</v>
-      </c>
-      <c r="E94" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
+        <v>301</v>
+      </c>
+      <c r="B95" t="s">
+        <v>302</v>
+      </c>
+      <c r="C95" t="s">
+        <v>303</v>
+      </c>
+      <c r="D95" t="s">
+        <v>304</v>
+      </c>
+      <c r="E95" t="s">
         <v>305</v>
-      </c>
-      <c r="B95" t="s">
-        <v>306</v>
-      </c>
-      <c r="C95" t="s">
-        <v>307</v>
-      </c>
-      <c r="D95" t="s">
-        <v>308</v>
-      </c>
-      <c r="E95" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -3414,274 +3414,274 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
+        <v>306</v>
+      </c>
+      <c r="B97" t="s">
+        <v>307</v>
+      </c>
+      <c r="C97" t="s">
+        <v>308</v>
+      </c>
+      <c r="D97" t="s">
+        <v>309</v>
+      </c>
+      <c r="E97" t="s">
         <v>310</v>
-      </c>
-      <c r="B97" t="s">
-        <v>311</v>
-      </c>
-      <c r="C97" t="s">
-        <v>312</v>
-      </c>
-      <c r="D97" t="s">
-        <v>313</v>
-      </c>
-      <c r="E97" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="B98" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="C98" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="D98" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="E98" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="B99" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="C99" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="D99" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E99" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B100" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="C100" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="D100" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="E100" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="B101" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C101" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D101" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="E101" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
+        <v>323</v>
+      </c>
+      <c r="B102" t="s">
+        <v>324</v>
+      </c>
+      <c r="C102" t="s">
+        <v>325</v>
+      </c>
+      <c r="D102" t="s">
+        <v>326</v>
+      </c>
+      <c r="E102" t="s">
         <v>327</v>
-      </c>
-      <c r="B102" t="s">
-        <v>328</v>
-      </c>
-      <c r="C102" t="s">
-        <v>329</v>
-      </c>
-      <c r="D102" t="s">
-        <v>330</v>
-      </c>
-      <c r="E102" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
+        <v>328</v>
+      </c>
+      <c r="B103" t="s">
+        <v>329</v>
+      </c>
+      <c r="C103" t="s">
+        <v>330</v>
+      </c>
+      <c r="D103" t="s">
+        <v>331</v>
+      </c>
+      <c r="E103" t="s">
         <v>332</v>
-      </c>
-      <c r="B103" t="s">
-        <v>333</v>
-      </c>
-      <c r="C103" t="s">
-        <v>334</v>
-      </c>
-      <c r="D103" t="s">
-        <v>335</v>
-      </c>
-      <c r="E103" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
+        <v>333</v>
+      </c>
+      <c r="B104" t="s">
+        <v>334</v>
+      </c>
+      <c r="C104" t="s">
+        <v>335</v>
+      </c>
+      <c r="D104" t="s">
+        <v>336</v>
+      </c>
+      <c r="E104" t="s">
         <v>337</v>
-      </c>
-      <c r="B104" t="s">
-        <v>338</v>
-      </c>
-      <c r="C104" t="s">
-        <v>339</v>
-      </c>
-      <c r="D104" t="s">
-        <v>340</v>
-      </c>
-      <c r="E104" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="B105" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="C105" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="D105" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="E105" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="B106" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="C106" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="D106" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="E106" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="B107" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="C107" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="D107" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="E107" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="B108" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="C108" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="D108" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="E108" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
+        <v>351</v>
+      </c>
+      <c r="B109" t="s">
+        <v>352</v>
+      </c>
+      <c r="C109" t="s">
+        <v>353</v>
+      </c>
+      <c r="D109" t="s">
+        <v>354</v>
+      </c>
+      <c r="E109" t="s">
         <v>355</v>
-      </c>
-      <c r="B109" t="s">
-        <v>356</v>
-      </c>
-      <c r="C109" t="s">
-        <v>357</v>
-      </c>
-      <c r="D109" t="s">
-        <v>358</v>
-      </c>
-      <c r="E109" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="B110" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="C110" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="D110" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="E110" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
+        <v>359</v>
+      </c>
+      <c r="B111" t="s">
+        <v>360</v>
+      </c>
+      <c r="C111" t="s">
+        <v>361</v>
+      </c>
+      <c r="D111" t="s">
+        <v>362</v>
+      </c>
+      <c r="E111" t="s">
         <v>363</v>
-      </c>
-      <c r="B111" t="s">
-        <v>364</v>
-      </c>
-      <c r="C111" t="s">
-        <v>365</v>
-      </c>
-      <c r="D111" t="s">
-        <v>366</v>
-      </c>
-      <c r="E111" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
+        <v>433</v>
+      </c>
+      <c r="B112" t="s">
+        <v>435</v>
+      </c>
+      <c r="C112" t="s">
         <v>437</v>
       </c>
-      <c r="B112" t="s">
+      <c r="D112" t="s">
         <v>439</v>
       </c>
-      <c r="C112" t="s">
+      <c r="E112" t="s">
         <v>441</v>
-      </c>
-      <c r="D112" t="s">
-        <v>443</v>
-      </c>
-      <c r="E112" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixed some invalid characters
</commit_message>
<xml_diff>
--- a/assets/Localizations.xlsx
+++ b/assets/Localizations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Grade.ly\Grade.ly - Flutter\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73089631-C2B8-47C9-82A2-E2565FCDE833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35CAF98F-1A71-428C-9EEE-D5FFE3F2CE7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -223,9 +223,6 @@
     <t>App version</t>
   </si>
   <si>
-    <t>Version de l\'application</t>
-  </si>
-  <si>
     <t>App-Version</t>
   </si>
   <si>
@@ -517,9 +514,6 @@
     <t>Klicken Sie um Ihre Fächer zu bearbeiten</t>
   </si>
   <si>
-    <t>Klickt fir är Fächer ze beaarbechten</t>
-  </si>
-  <si>
     <t>edit_test</t>
   </si>
   <si>
@@ -814,15 +808,9 @@
     <t>Delete all saved grades and reset app</t>
   </si>
   <si>
-    <t>Supprimer toutes les notes enregistrées et réinitialiser l\'application</t>
-  </si>
-  <si>
     <t>Alle gespeicherten Noten löschen und App zurücksetzen</t>
   </si>
   <si>
-    <t>All gespäichert Notten läschen an d\'App zeréckzesetzen</t>
-  </si>
-  <si>
     <t>round_to</t>
   </si>
   <si>
@@ -1030,9 +1018,6 @@
     <t>To integer</t>
   </si>
   <si>
-    <t>A l\'entier</t>
-  </si>
-  <si>
     <t>Zu Ganzzahl</t>
   </si>
   <si>
@@ -1309,9 +1294,6 @@
     <t>F - Musek</t>
   </si>
   <si>
-    <t>G - Mënschlech an sozial Wëssenschaften</t>
-  </si>
-  <si>
     <t>I - Informatik &amp; Kommunikatioun</t>
   </si>
   <si>
@@ -1381,9 +1363,6 @@
     <t>Klicken Sie um Ihre aktuelle Klasse zu ändern. Alle gespeicherten Noten werden dabei gelöscht.</t>
   </si>
   <si>
-    <t>Klickt fir är aktuell Klass ze änneren. All gespäichert Notten ginn dobäi geläscht.</t>
-  </si>
-  <si>
     <t>ok</t>
   </si>
   <si>
@@ -1399,7 +1378,28 @@
     <t>Sie können Ihre Fächer und andere Optionen später immer noch in den Einstellungen bearbeiten</t>
   </si>
   <si>
-    <t>Dir kënnt är Fächer an aner Optiounen spéider ëmmer nach an den Astellungen beaarbechten</t>
+    <t>Version de l'application</t>
+  </si>
+  <si>
+    <t>Supprimer toutes les notes enregistrées et réinitialiser l'application</t>
+  </si>
+  <si>
+    <t>A l'entier</t>
+  </si>
+  <si>
+    <t>Klickt fir är aktuell Klass ze änneren. All gespäichert Notten ginn dobäi geläscht.</t>
+  </si>
+  <si>
+    <t>Klickt fir är Fächer ze beaarbechten</t>
+  </si>
+  <si>
+    <t>G - Mënschlech an sozial Wëssenschaften</t>
+  </si>
+  <si>
+    <t>Dir kënnt är Fächer an aner Optiounen spéider ëmmer nach an den Astellungen beaarbechten</t>
+  </si>
+  <si>
+    <t>All gespäichert Notten läschen an d'App zeréckzesetzen</t>
   </si>
 </sst>
 </file>
@@ -1767,8 +1767,8 @@
   </sheetPr>
   <dimension ref="A1:E113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="D76" sqref="D76"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1799,19 +1799,19 @@
     </row>
     <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="B2" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="C2" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="D2" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="E2" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1941,47 +1941,47 @@
         <v>65</v>
       </c>
       <c r="C10" t="s">
+        <v>451</v>
+      </c>
+      <c r="D10" t="s">
         <v>66</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>67</v>
-      </c>
-      <c r="E10" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" t="s">
         <v>69</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>70</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>71</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>72</v>
-      </c>
-      <c r="E11" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" t="s">
         <v>74</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>75</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>76</v>
       </c>
-      <c r="D12" t="s">
-        <v>77</v>
-      </c>
       <c r="E12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2003,478 +2003,478 @@
     </row>
     <row r="14" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="B14" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="C14" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="D14" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="E14" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" t="s">
         <v>78</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>79</v>
       </c>
-      <c r="C15" t="s">
-        <v>80</v>
-      </c>
       <c r="D15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>80</v>
+      </c>
+      <c r="B16" t="s">
         <v>81</v>
       </c>
-      <c r="B16" t="s">
-        <v>82</v>
-      </c>
       <c r="C16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="B17" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="C17" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="D17" t="s">
+        <v>414</v>
+      </c>
+      <c r="E17" t="s">
         <v>419</v>
-      </c>
-      <c r="E17" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
       <c r="B18" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
       <c r="C18" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
       <c r="D18" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="E18" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>438</v>
+      </c>
+      <c r="B19" t="s">
         <v>444</v>
       </c>
-      <c r="B19" t="s">
-        <v>450</v>
-      </c>
       <c r="C19" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="D19" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
       <c r="E19" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" t="s">
         <v>83</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>84</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>85</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>86</v>
-      </c>
-      <c r="E20" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>87</v>
+      </c>
+      <c r="B21" t="s">
         <v>88</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>89</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>90</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>91</v>
-      </c>
-      <c r="E21" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="B22" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="C22" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="D22" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="E22" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>92</v>
+      </c>
+      <c r="B23" t="s">
         <v>93</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
+        <v>93</v>
+      </c>
+      <c r="D23" t="s">
         <v>94</v>
       </c>
-      <c r="C23" t="s">
+      <c r="E23" t="s">
         <v>94</v>
-      </c>
-      <c r="D23" t="s">
-        <v>95</v>
-      </c>
-      <c r="E23" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>95</v>
+      </c>
+      <c r="B24" t="s">
         <v>96</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
+        <v>96</v>
+      </c>
+      <c r="D24" t="s">
         <v>97</v>
       </c>
-      <c r="C24" t="s">
+      <c r="E24" t="s">
         <v>97</v>
-      </c>
-      <c r="D24" t="s">
-        <v>98</v>
-      </c>
-      <c r="E24" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>98</v>
+      </c>
+      <c r="B25" t="s">
         <v>99</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
+        <v>99</v>
+      </c>
+      <c r="D25" t="s">
         <v>100</v>
       </c>
-      <c r="C25" t="s">
-        <v>100</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>101</v>
-      </c>
-      <c r="E25" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>102</v>
+      </c>
+      <c r="B26" t="s">
         <v>103</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>104</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>105</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>106</v>
-      </c>
-      <c r="E26" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>107</v>
+      </c>
+      <c r="B27" t="s">
         <v>108</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>109</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>110</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>111</v>
-      </c>
-      <c r="E27" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>112</v>
+      </c>
+      <c r="B28" t="s">
         <v>113</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>114</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>115</v>
       </c>
-      <c r="D28" t="s">
-        <v>116</v>
-      </c>
       <c r="E28" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>116</v>
+      </c>
+      <c r="B29" t="s">
         <v>117</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>118</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>119</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>120</v>
-      </c>
-      <c r="E29" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>121</v>
+      </c>
+      <c r="B30" t="s">
         <v>122</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>123</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>124</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>125</v>
-      </c>
-      <c r="E30" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="B31" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="C31" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="D31" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="E31" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>126</v>
+      </c>
+      <c r="B32" t="s">
         <v>127</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>128</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>129</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>130</v>
-      </c>
-      <c r="E32" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>131</v>
+      </c>
+      <c r="B33" t="s">
         <v>132</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>133</v>
       </c>
-      <c r="C33" t="s">
-        <v>134</v>
-      </c>
       <c r="D33" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E33" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>134</v>
+      </c>
+      <c r="B34" t="s">
         <v>135</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>136</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>137</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>138</v>
-      </c>
-      <c r="E34" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>139</v>
+      </c>
+      <c r="B35" t="s">
         <v>140</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>141</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>142</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>143</v>
-      </c>
-      <c r="E35" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="B36" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="C36" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="D36" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="E36" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>144</v>
+      </c>
+      <c r="B37" t="s">
         <v>145</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>146</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>147</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>148</v>
-      </c>
-      <c r="E37" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>149</v>
+      </c>
+      <c r="B38" t="s">
         <v>150</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>151</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>152</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>153</v>
-      </c>
-      <c r="E38" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>154</v>
+      </c>
+      <c r="B39" t="s">
         <v>155</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>156</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>157</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>158</v>
-      </c>
-      <c r="E39" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>159</v>
+      </c>
+      <c r="B40" t="s">
         <v>160</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
         <v>161</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>162</v>
       </c>
-      <c r="D40" t="s">
-        <v>163</v>
-      </c>
       <c r="E40" t="s">
-        <v>164</v>
+        <v>455</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>163</v>
+      </c>
+      <c r="B41" t="s">
+        <v>164</v>
+      </c>
+      <c r="C41" t="s">
         <v>165</v>
       </c>
-      <c r="B41" t="s">
+      <c r="D41" t="s">
         <v>166</v>
       </c>
-      <c r="C41" t="s">
+      <c r="E41" t="s">
         <v>167</v>
-      </c>
-      <c r="D41" t="s">
-        <v>168</v>
-      </c>
-      <c r="E41" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2513,36 +2513,36 @@
     </row>
     <row r="44" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="B44" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="C44" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="D44" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="E44" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>393</v>
+      </c>
+      <c r="B45" t="s">
         <v>398</v>
       </c>
-      <c r="B45" t="s">
-        <v>403</v>
-      </c>
       <c r="C45" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="D45" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="E45" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2564,36 +2564,36 @@
     </row>
     <row r="47" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="B47" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="C47" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="D47" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="E47" t="s">
-        <v>428</v>
+        <v>456</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>168</v>
+      </c>
+      <c r="B48" t="s">
+        <v>169</v>
+      </c>
+      <c r="C48" t="s">
         <v>170</v>
       </c>
-      <c r="B48" t="s">
+      <c r="D48" t="s">
         <v>171</v>
       </c>
-      <c r="C48" t="s">
+      <c r="E48" t="s">
         <v>172</v>
-      </c>
-      <c r="D48" t="s">
-        <v>173</v>
-      </c>
-      <c r="E48" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2615,19 +2615,19 @@
     </row>
     <row r="50" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>173</v>
+      </c>
+      <c r="B50" t="s">
+        <v>174</v>
+      </c>
+      <c r="C50" t="s">
         <v>175</v>
       </c>
-      <c r="B50" t="s">
+      <c r="D50" t="s">
         <v>176</v>
       </c>
-      <c r="C50" t="s">
-        <v>177</v>
-      </c>
-      <c r="D50" t="s">
-        <v>178</v>
-      </c>
       <c r="E50" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2649,19 +2649,19 @@
     </row>
     <row r="52" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>177</v>
+      </c>
+      <c r="B52" t="s">
+        <v>178</v>
+      </c>
+      <c r="C52" t="s">
         <v>179</v>
       </c>
-      <c r="B52" t="s">
+      <c r="D52" t="s">
+        <v>179</v>
+      </c>
+      <c r="E52" t="s">
         <v>180</v>
-      </c>
-      <c r="C52" t="s">
-        <v>181</v>
-      </c>
-      <c r="D52" t="s">
-        <v>181</v>
-      </c>
-      <c r="E52" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2717,189 +2717,189 @@
     </row>
     <row r="56" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>181</v>
+      </c>
+      <c r="B56" t="s">
+        <v>182</v>
+      </c>
+      <c r="C56" t="s">
         <v>183</v>
       </c>
-      <c r="B56" t="s">
+      <c r="D56" t="s">
         <v>184</v>
       </c>
-      <c r="C56" t="s">
+      <c r="E56" t="s">
         <v>185</v>
-      </c>
-      <c r="D56" t="s">
-        <v>186</v>
-      </c>
-      <c r="E56" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>186</v>
+      </c>
+      <c r="B57" t="s">
+        <v>187</v>
+      </c>
+      <c r="C57" t="s">
         <v>188</v>
       </c>
-      <c r="B57" t="s">
+      <c r="D57" t="s">
         <v>189</v>
       </c>
-      <c r="C57" t="s">
+      <c r="E57" t="s">
         <v>190</v>
-      </c>
-      <c r="D57" t="s">
-        <v>191</v>
-      </c>
-      <c r="E57" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>191</v>
+      </c>
+      <c r="B58" t="s">
+        <v>192</v>
+      </c>
+      <c r="C58" t="s">
         <v>193</v>
       </c>
-      <c r="B58" t="s">
+      <c r="D58" t="s">
         <v>194</v>
       </c>
-      <c r="C58" t="s">
+      <c r="E58" t="s">
         <v>195</v>
-      </c>
-      <c r="D58" t="s">
-        <v>196</v>
-      </c>
-      <c r="E58" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="B59" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="C59" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="D59" t="s">
+        <v>418</v>
+      </c>
+      <c r="E59" t="s">
         <v>423</v>
-      </c>
-      <c r="E59" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>196</v>
+      </c>
+      <c r="B60" t="s">
+        <v>197</v>
+      </c>
+      <c r="C60" t="s">
         <v>198</v>
       </c>
-      <c r="B60" t="s">
+      <c r="D60" t="s">
         <v>199</v>
       </c>
-      <c r="C60" t="s">
+      <c r="E60" t="s">
         <v>200</v>
-      </c>
-      <c r="D60" t="s">
-        <v>201</v>
-      </c>
-      <c r="E60" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>201</v>
+      </c>
+      <c r="B61" t="s">
+        <v>202</v>
+      </c>
+      <c r="C61" t="s">
+        <v>202</v>
+      </c>
+      <c r="D61" t="s">
         <v>203</v>
       </c>
-      <c r="B61" t="s">
+      <c r="E61" t="s">
         <v>204</v>
-      </c>
-      <c r="C61" t="s">
-        <v>204</v>
-      </c>
-      <c r="D61" t="s">
-        <v>205</v>
-      </c>
-      <c r="E61" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>205</v>
+      </c>
+      <c r="B62" t="s">
+        <v>206</v>
+      </c>
+      <c r="C62" t="s">
+        <v>206</v>
+      </c>
+      <c r="D62" t="s">
         <v>207</v>
       </c>
-      <c r="B62" t="s">
-        <v>208</v>
-      </c>
-      <c r="C62" t="s">
-        <v>208</v>
-      </c>
-      <c r="D62" t="s">
-        <v>209</v>
-      </c>
       <c r="E62" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>208</v>
+      </c>
+      <c r="B63" t="s">
+        <v>209</v>
+      </c>
+      <c r="C63" t="s">
         <v>210</v>
       </c>
-      <c r="B63" t="s">
+      <c r="D63" t="s">
         <v>211</v>
       </c>
-      <c r="C63" t="s">
+      <c r="E63" t="s">
         <v>212</v>
-      </c>
-      <c r="D63" t="s">
-        <v>213</v>
-      </c>
-      <c r="E63" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>213</v>
+      </c>
+      <c r="B64" t="s">
+        <v>214</v>
+      </c>
+      <c r="C64" t="s">
+        <v>214</v>
+      </c>
+      <c r="D64" t="s">
         <v>215</v>
       </c>
-      <c r="B64" t="s">
-        <v>216</v>
-      </c>
-      <c r="C64" t="s">
-        <v>216</v>
-      </c>
-      <c r="D64" t="s">
-        <v>217</v>
-      </c>
       <c r="E64" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>216</v>
+      </c>
+      <c r="B65" t="s">
+        <v>217</v>
+      </c>
+      <c r="C65" t="s">
+        <v>217</v>
+      </c>
+      <c r="D65" t="s">
         <v>218</v>
       </c>
-      <c r="B65" t="s">
+      <c r="E65" t="s">
         <v>219</v>
-      </c>
-      <c r="C65" t="s">
-        <v>219</v>
-      </c>
-      <c r="D65" t="s">
-        <v>220</v>
-      </c>
-      <c r="E65" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>220</v>
+      </c>
+      <c r="B66" t="s">
+        <v>221</v>
+      </c>
+      <c r="C66" t="s">
         <v>222</v>
       </c>
-      <c r="B66" t="s">
+      <c r="D66" t="s">
         <v>223</v>
       </c>
-      <c r="C66" t="s">
+      <c r="E66" t="s">
         <v>224</v>
-      </c>
-      <c r="D66" t="s">
-        <v>225</v>
-      </c>
-      <c r="E66" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2921,19 +2921,19 @@
     </row>
     <row r="68" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="B68" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="C68" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="D68" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="E68" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2955,138 +2955,138 @@
     </row>
     <row r="70" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="B70" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="C70" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="D70" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="E70" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="B71" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="C71" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="D71" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="E71" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>225</v>
+      </c>
+      <c r="B72" t="s">
+        <v>226</v>
+      </c>
+      <c r="C72" t="s">
         <v>227</v>
       </c>
-      <c r="B72" t="s">
+      <c r="D72" t="s">
         <v>228</v>
       </c>
-      <c r="C72" t="s">
+      <c r="E72" t="s">
         <v>229</v>
-      </c>
-      <c r="D72" t="s">
-        <v>230</v>
-      </c>
-      <c r="E72" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>428</v>
+      </c>
+      <c r="B73" t="s">
+        <v>430</v>
+      </c>
+      <c r="C73" t="s">
+        <v>432</v>
+      </c>
+      <c r="D73" t="s">
         <v>434</v>
       </c>
-      <c r="B73" t="s">
+      <c r="E73" t="s">
         <v>436</v>
-      </c>
-      <c r="C73" t="s">
-        <v>438</v>
-      </c>
-      <c r="D73" t="s">
-        <v>440</v>
-      </c>
-      <c r="E73" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="B74" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="C74" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="D74" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="E74" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
+        <v>230</v>
+      </c>
+      <c r="B75" t="s">
+        <v>231</v>
+      </c>
+      <c r="C75" t="s">
+        <v>231</v>
+      </c>
+      <c r="D75" t="s">
         <v>232</v>
       </c>
-      <c r="B75" t="s">
+      <c r="E75" t="s">
         <v>233</v>
-      </c>
-      <c r="C75" t="s">
-        <v>233</v>
-      </c>
-      <c r="D75" t="s">
-        <v>234</v>
-      </c>
-      <c r="E75" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B76" t="s">
-        <v>455</v>
+        <v>448</v>
       </c>
       <c r="C76" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="D76" t="s">
+        <v>450</v>
+      </c>
+      <c r="E76" t="s">
         <v>457</v>
-      </c>
-      <c r="E76" t="s">
-        <v>458</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
       <c r="B77" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
       <c r="C77" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
       <c r="D77" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
       <c r="E77" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3108,36 +3108,36 @@
     </row>
     <row r="79" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
+        <v>235</v>
+      </c>
+      <c r="B79" t="s">
+        <v>236</v>
+      </c>
+      <c r="C79" t="s">
         <v>237</v>
       </c>
-      <c r="B79" t="s">
+      <c r="D79" t="s">
         <v>238</v>
       </c>
-      <c r="C79" t="s">
-        <v>239</v>
-      </c>
-      <c r="D79" t="s">
-        <v>240</v>
-      </c>
       <c r="E79" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>239</v>
+      </c>
+      <c r="B80" t="s">
+        <v>240</v>
+      </c>
+      <c r="C80" t="s">
         <v>241</v>
       </c>
-      <c r="B80" t="s">
+      <c r="D80" t="s">
         <v>242</v>
       </c>
-      <c r="C80" t="s">
+      <c r="E80" t="s">
         <v>243</v>
-      </c>
-      <c r="D80" t="s">
-        <v>244</v>
-      </c>
-      <c r="E80" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3159,240 +3159,240 @@
     </row>
     <row r="82" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>244</v>
+      </c>
+      <c r="B82" t="s">
+        <v>245</v>
+      </c>
+      <c r="C82" t="s">
         <v>246</v>
       </c>
-      <c r="B82" t="s">
+      <c r="D82" t="s">
         <v>247</v>
       </c>
-      <c r="C82" t="s">
+      <c r="E82" t="s">
         <v>248</v>
-      </c>
-      <c r="D82" t="s">
-        <v>249</v>
-      </c>
-      <c r="E82" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
+        <v>249</v>
+      </c>
+      <c r="B83" t="s">
+        <v>250</v>
+      </c>
+      <c r="C83" t="s">
         <v>251</v>
       </c>
-      <c r="B83" t="s">
+      <c r="D83" t="s">
         <v>252</v>
       </c>
-      <c r="C83" t="s">
+      <c r="E83" t="s">
         <v>253</v>
-      </c>
-      <c r="D83" t="s">
-        <v>254</v>
-      </c>
-      <c r="E83" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
+        <v>254</v>
+      </c>
+      <c r="B84" t="s">
+        <v>255</v>
+      </c>
+      <c r="C84" t="s">
         <v>256</v>
       </c>
-      <c r="B84" t="s">
+      <c r="D84" t="s">
         <v>257</v>
       </c>
-      <c r="C84" t="s">
+      <c r="E84" t="s">
         <v>258</v>
-      </c>
-      <c r="D84" t="s">
-        <v>259</v>
-      </c>
-      <c r="E84" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
+        <v>259</v>
+      </c>
+      <c r="B85" t="s">
+        <v>260</v>
+      </c>
+      <c r="C85" t="s">
+        <v>452</v>
+      </c>
+      <c r="D85" t="s">
         <v>261</v>
       </c>
-      <c r="B85" t="s">
-        <v>262</v>
-      </c>
-      <c r="C85" t="s">
-        <v>263</v>
-      </c>
-      <c r="D85" t="s">
-        <v>264</v>
-      </c>
       <c r="E85" t="s">
-        <v>265</v>
+        <v>458</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
+        <v>262</v>
+      </c>
+      <c r="B86" t="s">
+        <v>263</v>
+      </c>
+      <c r="C86" t="s">
+        <v>264</v>
+      </c>
+      <c r="D86" t="s">
+        <v>265</v>
+      </c>
+      <c r="E86" t="s">
         <v>266</v>
-      </c>
-      <c r="B86" t="s">
-        <v>267</v>
-      </c>
-      <c r="C86" t="s">
-        <v>268</v>
-      </c>
-      <c r="D86" t="s">
-        <v>269</v>
-      </c>
-      <c r="E86" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
+        <v>267</v>
+      </c>
+      <c r="B87" t="s">
+        <v>268</v>
+      </c>
+      <c r="C87" t="s">
+        <v>269</v>
+      </c>
+      <c r="D87" t="s">
+        <v>270</v>
+      </c>
+      <c r="E87" t="s">
         <v>271</v>
-      </c>
-      <c r="B87" t="s">
-        <v>272</v>
-      </c>
-      <c r="C87" t="s">
-        <v>273</v>
-      </c>
-      <c r="D87" t="s">
-        <v>274</v>
-      </c>
-      <c r="E87" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
+        <v>272</v>
+      </c>
+      <c r="B88" t="s">
+        <v>273</v>
+      </c>
+      <c r="C88" t="s">
+        <v>274</v>
+      </c>
+      <c r="D88" t="s">
+        <v>275</v>
+      </c>
+      <c r="E88" t="s">
         <v>276</v>
-      </c>
-      <c r="B88" t="s">
-        <v>277</v>
-      </c>
-      <c r="C88" t="s">
-        <v>278</v>
-      </c>
-      <c r="D88" t="s">
-        <v>279</v>
-      </c>
-      <c r="E88" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="B89" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="C89" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="D89" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="E89" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
+        <v>277</v>
+      </c>
+      <c r="B90" t="s">
+        <v>278</v>
+      </c>
+      <c r="C90" t="s">
+        <v>279</v>
+      </c>
+      <c r="D90" t="s">
+        <v>280</v>
+      </c>
+      <c r="E90" t="s">
         <v>281</v>
-      </c>
-      <c r="B90" t="s">
-        <v>282</v>
-      </c>
-      <c r="C90" t="s">
-        <v>283</v>
-      </c>
-      <c r="D90" t="s">
-        <v>284</v>
-      </c>
-      <c r="E90" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B91" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="C91" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="D91" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="E91" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="B92" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="C92" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="D92" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="E92" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B93" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C93" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D93" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="E93" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
+        <v>292</v>
+      </c>
+      <c r="B94" t="s">
+        <v>293</v>
+      </c>
+      <c r="C94" t="s">
+        <v>294</v>
+      </c>
+      <c r="D94" t="s">
+        <v>295</v>
+      </c>
+      <c r="E94" t="s">
         <v>296</v>
-      </c>
-      <c r="B94" t="s">
-        <v>297</v>
-      </c>
-      <c r="C94" t="s">
-        <v>298</v>
-      </c>
-      <c r="D94" t="s">
-        <v>299</v>
-      </c>
-      <c r="E94" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
+        <v>297</v>
+      </c>
+      <c r="B95" t="s">
+        <v>298</v>
+      </c>
+      <c r="C95" t="s">
+        <v>299</v>
+      </c>
+      <c r="D95" t="s">
+        <v>300</v>
+      </c>
+      <c r="E95" t="s">
         <v>301</v>
-      </c>
-      <c r="B95" t="s">
-        <v>302</v>
-      </c>
-      <c r="C95" t="s">
-        <v>303</v>
-      </c>
-      <c r="D95" t="s">
-        <v>304</v>
-      </c>
-      <c r="E95" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -3414,274 +3414,274 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
+        <v>302</v>
+      </c>
+      <c r="B97" t="s">
+        <v>303</v>
+      </c>
+      <c r="C97" t="s">
+        <v>304</v>
+      </c>
+      <c r="D97" t="s">
+        <v>305</v>
+      </c>
+      <c r="E97" t="s">
         <v>306</v>
-      </c>
-      <c r="B97" t="s">
-        <v>307</v>
-      </c>
-      <c r="C97" t="s">
-        <v>308</v>
-      </c>
-      <c r="D97" t="s">
-        <v>309</v>
-      </c>
-      <c r="E97" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="B98" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="C98" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="D98" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="E98" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
       <c r="B99" t="s">
-        <v>431</v>
+        <v>425</v>
       </c>
       <c r="C99" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
       <c r="D99" t="s">
-        <v>431</v>
+        <v>425</v>
       </c>
       <c r="E99" t="s">
-        <v>431</v>
+        <v>425</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="B100" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="C100" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="D100" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="E100" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B101" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="C101" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="D101" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="E101" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
+        <v>319</v>
+      </c>
+      <c r="B102" t="s">
+        <v>320</v>
+      </c>
+      <c r="C102" t="s">
+        <v>321</v>
+      </c>
+      <c r="D102" t="s">
+        <v>322</v>
+      </c>
+      <c r="E102" t="s">
         <v>323</v>
-      </c>
-      <c r="B102" t="s">
-        <v>324</v>
-      </c>
-      <c r="C102" t="s">
-        <v>325</v>
-      </c>
-      <c r="D102" t="s">
-        <v>326</v>
-      </c>
-      <c r="E102" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
+        <v>324</v>
+      </c>
+      <c r="B103" t="s">
+        <v>325</v>
+      </c>
+      <c r="C103" t="s">
+        <v>326</v>
+      </c>
+      <c r="D103" t="s">
+        <v>327</v>
+      </c>
+      <c r="E103" t="s">
         <v>328</v>
-      </c>
-      <c r="B103" t="s">
-        <v>329</v>
-      </c>
-      <c r="C103" t="s">
-        <v>330</v>
-      </c>
-      <c r="D103" t="s">
-        <v>331</v>
-      </c>
-      <c r="E103" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="B104" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="C104" t="s">
-        <v>335</v>
+        <v>453</v>
       </c>
       <c r="D104" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="E104" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="B105" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="C105" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="D105" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="E105" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="B106" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="C106" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="D106" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="E106" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="B107" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="C107" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="D107" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="E107" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="B108" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="C108" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="D108" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="E108" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="B109" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="C109" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="D109" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="E109" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="B110" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="C110" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="D110" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="E110" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="B111" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="C111" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="D111" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="E111" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
+        <v>427</v>
+      </c>
+      <c r="B112" t="s">
+        <v>429</v>
+      </c>
+      <c r="C112" t="s">
+        <v>431</v>
+      </c>
+      <c r="D112" t="s">
         <v>433</v>
       </c>
-      <c r="B112" t="s">
+      <c r="E112" t="s">
         <v>435</v>
-      </c>
-      <c r="C112" t="s">
-        <v>437</v>
-      </c>
-      <c r="D112" t="s">
-        <v>439</v>
-      </c>
-      <c r="E112" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixed german rounding translations
</commit_message>
<xml_diff>
--- a/assets/Localizations.xlsx
+++ b/assets/Localizations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Grade.ly\Grade.ly - Flutter\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7230E82-1F66-4F0A-A4D7-44E54BA3DB88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE5685FD-4919-461F-831F-8343859A861E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="458">
   <si>
     <t>keys</t>
   </si>
@@ -940,9 +940,6 @@
     <t>Au 100ème</t>
   </si>
   <si>
-    <t>Zum 100-ten</t>
-  </si>
-  <si>
     <t>Zum 100-tel</t>
   </si>
   <si>
@@ -955,9 +952,6 @@
     <t>Au 10ème</t>
   </si>
   <si>
-    <t>Zum 10-ten</t>
-  </si>
-  <si>
     <t>Zum 10-tel</t>
   </si>
   <si>
@@ -967,9 +961,6 @@
     <t>To integer</t>
   </si>
   <si>
-    <t>Zu Ganzzahl</t>
-  </si>
-  <si>
     <t>Zur Ganzzuel</t>
   </si>
   <si>
@@ -1403,6 +1394,9 @@
   </si>
   <si>
     <t>section_classic_i</t>
+  </si>
+  <si>
+    <t>Zur Ganzzahl</t>
   </si>
 </sst>
 </file>
@@ -1770,8 +1764,8 @@
   </sheetPr>
   <dimension ref="A1:E113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="D104" sqref="D104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1802,19 +1796,19 @@
     </row>
     <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="B2" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="C2" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="D2" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="E2" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1944,7 +1938,7 @@
         <v>65</v>
       </c>
       <c r="C10" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="D10" t="s">
         <v>66</v>
@@ -2006,19 +2000,19 @@
     </row>
     <row r="14" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="B14" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="C14" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="D14" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="E14" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2057,53 +2051,53 @@
     </row>
     <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="B17" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="C17" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="D17" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="E17" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>409</v>
+      </c>
+      <c r="B18" t="s">
+        <v>411</v>
+      </c>
+      <c r="C18" t="s">
         <v>412</v>
       </c>
-      <c r="B18" t="s">
+      <c r="D18" t="s">
         <v>414</v>
       </c>
-      <c r="C18" t="s">
-        <v>415</v>
-      </c>
-      <c r="D18" t="s">
-        <v>417</v>
-      </c>
       <c r="E18" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="B19" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="C19" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="D19" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="E19" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2142,19 +2136,19 @@
     </row>
     <row r="22" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>360</v>
+      </c>
+      <c r="B22" t="s">
+        <v>361</v>
+      </c>
+      <c r="C22" t="s">
+        <v>362</v>
+      </c>
+      <c r="D22" t="s">
         <v>363</v>
       </c>
-      <c r="B22" t="s">
-        <v>364</v>
-      </c>
-      <c r="C22" t="s">
-        <v>365</v>
-      </c>
-      <c r="D22" t="s">
-        <v>366</v>
-      </c>
       <c r="E22" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2295,19 +2289,19 @@
     </row>
     <row r="31" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="B31" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="C31" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="D31" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="E31" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2363,19 +2357,19 @@
     </row>
     <row r="35" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="B35" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="C35" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="D35" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="E35" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2443,7 +2437,7 @@
         <v>157</v>
       </c>
       <c r="E39" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2499,36 +2493,36 @@
     </row>
     <row r="43" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>339</v>
+      </c>
+      <c r="B43" t="s">
+        <v>340</v>
+      </c>
+      <c r="C43" t="s">
+        <v>341</v>
+      </c>
+      <c r="D43" t="s">
         <v>342</v>
       </c>
-      <c r="B43" t="s">
+      <c r="E43" t="s">
         <v>343</v>
-      </c>
-      <c r="C43" t="s">
-        <v>344</v>
-      </c>
-      <c r="D43" t="s">
-        <v>345</v>
-      </c>
-      <c r="E43" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="B44" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="C44" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="D44" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="E44" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2550,19 +2544,19 @@
     </row>
     <row r="46" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="B46" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="C46" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="D46" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="E46" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2754,19 +2748,19 @@
     </row>
     <row r="58" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="B58" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="C58" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D58" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="E58" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2856,19 +2850,19 @@
     </row>
     <row r="64" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B64" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="C64" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="D64" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="E64" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2890,36 +2884,36 @@
     </row>
     <row r="66" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>350</v>
+      </c>
+      <c r="B66" t="s">
+        <v>351</v>
+      </c>
+      <c r="C66" t="s">
+        <v>352</v>
+      </c>
+      <c r="D66" t="s">
         <v>353</v>
       </c>
-      <c r="B66" t="s">
+      <c r="E66" t="s">
         <v>354</v>
-      </c>
-      <c r="C66" t="s">
-        <v>355</v>
-      </c>
-      <c r="D66" t="s">
-        <v>356</v>
-      </c>
-      <c r="E66" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>344</v>
+      </c>
+      <c r="B67" t="s">
+        <v>345</v>
+      </c>
+      <c r="C67" t="s">
+        <v>346</v>
+      </c>
+      <c r="D67" t="s">
+        <v>345</v>
+      </c>
+      <c r="E67" t="s">
         <v>347</v>
-      </c>
-      <c r="B67" t="s">
-        <v>348</v>
-      </c>
-      <c r="C67" t="s">
-        <v>349</v>
-      </c>
-      <c r="D67" t="s">
-        <v>348</v>
-      </c>
-      <c r="E67" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2941,36 +2935,36 @@
     </row>
     <row r="69" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="B69" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="C69" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="D69" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="E69" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>355</v>
+      </c>
+      <c r="B70" t="s">
+        <v>356</v>
+      </c>
+      <c r="C70" t="s">
+        <v>357</v>
+      </c>
+      <c r="D70" t="s">
         <v>358</v>
       </c>
-      <c r="B70" t="s">
+      <c r="E70" t="s">
         <v>359</v>
-      </c>
-      <c r="C70" t="s">
-        <v>360</v>
-      </c>
-      <c r="D70" t="s">
-        <v>361</v>
-      </c>
-      <c r="E70" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2995,33 +2989,33 @@
         <v>217</v>
       </c>
       <c r="B72" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C72" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="D72" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="E72" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="B73" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="C73" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="D73" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="E73" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3151,13 +3145,13 @@
         <v>243</v>
       </c>
       <c r="C81" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="D81" t="s">
         <v>244</v>
       </c>
       <c r="E81" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3213,19 +3207,19 @@
     </row>
     <row r="85" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="B85" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="C85" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="D85" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="E85" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3383,19 +3377,19 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="B95" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="C95" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="D95" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="E95" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -3434,70 +3428,70 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
+        <v>445</v>
+      </c>
+      <c r="B98" t="s">
+        <v>446</v>
+      </c>
+      <c r="C98" t="s">
+        <v>447</v>
+      </c>
+      <c r="D98" t="s">
         <v>448</v>
       </c>
-      <c r="B98" t="s">
-        <v>449</v>
-      </c>
-      <c r="C98" t="s">
-        <v>450</v>
-      </c>
-      <c r="D98" t="s">
-        <v>451</v>
-      </c>
       <c r="E98" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="B99" t="s">
+        <v>441</v>
+      </c>
+      <c r="C99" t="s">
+        <v>442</v>
+      </c>
+      <c r="D99" t="s">
+        <v>443</v>
+      </c>
+      <c r="E99" t="s">
         <v>444</v>
-      </c>
-      <c r="C99" t="s">
-        <v>445</v>
-      </c>
-      <c r="D99" t="s">
-        <v>446</v>
-      </c>
-      <c r="E99" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="B100" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="C100" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="D100" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="E100" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
+        <v>434</v>
+      </c>
+      <c r="B101" t="s">
+        <v>433</v>
+      </c>
+      <c r="C101" t="s">
+        <v>435</v>
+      </c>
+      <c r="D101" t="s">
+        <v>436</v>
+      </c>
+      <c r="E101" t="s">
         <v>437</v>
-      </c>
-      <c r="B101" t="s">
-        <v>436</v>
-      </c>
-      <c r="C101" t="s">
-        <v>438</v>
-      </c>
-      <c r="D101" t="s">
-        <v>439</v>
-      </c>
-      <c r="E101" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -3514,177 +3508,177 @@
         <v>305</v>
       </c>
       <c r="E102" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
+        <v>306</v>
+      </c>
+      <c r="B103" t="s">
         <v>307</v>
       </c>
-      <c r="B103" t="s">
+      <c r="C103" t="s">
         <v>308</v>
       </c>
-      <c r="C103" t="s">
+      <c r="D103" t="s">
         <v>309</v>
       </c>
-      <c r="D103" t="s">
-        <v>310</v>
-      </c>
       <c r="E103" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
+        <v>310</v>
+      </c>
+      <c r="B104" t="s">
+        <v>311</v>
+      </c>
+      <c r="C104" t="s">
+        <v>425</v>
+      </c>
+      <c r="D104" t="s">
+        <v>457</v>
+      </c>
+      <c r="E104" t="s">
         <v>312</v>
-      </c>
-      <c r="B104" t="s">
-        <v>313</v>
-      </c>
-      <c r="C104" t="s">
-        <v>428</v>
-      </c>
-      <c r="D104" t="s">
-        <v>314</v>
-      </c>
-      <c r="E104" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B105" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C105" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="D105" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="E105" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B106" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C106" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D106" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E106" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="B107" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C107" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="D107" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="E107" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
+        <v>322</v>
+      </c>
+      <c r="B108" t="s">
+        <v>323</v>
+      </c>
+      <c r="C108" t="s">
+        <v>324</v>
+      </c>
+      <c r="D108" t="s">
         <v>325</v>
       </c>
-      <c r="B108" t="s">
-        <v>326</v>
-      </c>
-      <c r="C108" t="s">
-        <v>327</v>
-      </c>
-      <c r="D108" t="s">
-        <v>328</v>
-      </c>
       <c r="E108" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
+        <v>326</v>
+      </c>
+      <c r="B109" t="s">
+        <v>327</v>
+      </c>
+      <c r="C109" t="s">
+        <v>328</v>
+      </c>
+      <c r="D109" t="s">
         <v>329</v>
       </c>
-      <c r="B109" t="s">
+      <c r="E109" t="s">
         <v>330</v>
-      </c>
-      <c r="C109" t="s">
-        <v>331</v>
-      </c>
-      <c r="D109" t="s">
-        <v>332</v>
-      </c>
-      <c r="E109" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B110" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="C110" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="D110" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="E110" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
+        <v>334</v>
+      </c>
+      <c r="B111" t="s">
+        <v>335</v>
+      </c>
+      <c r="C111" t="s">
+        <v>336</v>
+      </c>
+      <c r="D111" t="s">
         <v>337</v>
       </c>
-      <c r="B111" t="s">
+      <c r="E111" t="s">
         <v>338</v>
-      </c>
-      <c r="C111" t="s">
-        <v>339</v>
-      </c>
-      <c r="D111" t="s">
-        <v>340</v>
-      </c>
-      <c r="E111" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="B112" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="C112" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="D112" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="E112" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Improved text validation, Restructured project, Fixed Warnings
</commit_message>
<xml_diff>
--- a/assets/Localizations.xlsx
+++ b/assets/Localizations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Grade.ly\Grade.ly - Flutter\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE5685FD-4919-461F-831F-8343859A861E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A3596C3-6BE8-45EC-B41E-E74B53ACECBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="string" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0">string!$A$1:$B$113</definedName>
+    <definedName name="ExternalData_1" localSheetId="0">string!$A$1:$B$105</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="442">
   <si>
     <t>keys</t>
   </si>
@@ -46,51 +46,6 @@
     <t>Grade.ly</t>
   </si>
   <si>
-    <t>grade_sample1</t>
-  </si>
-  <si>
-    <t>01</t>
-  </si>
-  <si>
-    <t>grade_sample2</t>
-  </si>
-  <si>
-    <t>01/60</t>
-  </si>
-  <si>
-    <t>grade_sample3</t>
-  </si>
-  <si>
-    <t>60</t>
-  </si>
-  <si>
-    <t>slash</t>
-  </si>
-  <si>
-    <t>/</t>
-  </si>
-  <si>
-    <t>zero</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>plus</t>
-  </si>
-  <si>
-    <t>+</t>
-  </si>
-  <si>
-    <t>minus</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>az</t>
   </si>
   <si>
@@ -103,9 +58,6 @@
     <t>NightDream Games - FauconSpartiate\nVisual identity - Ellia Walrave\nTesting - AigleSpartiate</t>
   </si>
   <si>
-    <t>one</t>
-  </si>
-  <si>
     <t>github_summary</t>
   </si>
   <si>
@@ -1042,21 +994,6 @@
     <t>Joer</t>
   </si>
   <si>
-    <t>enter_valid_number</t>
-  </si>
-  <si>
-    <t>Enter a valid number</t>
-  </si>
-  <si>
-    <t>Entrez un nombre valide</t>
-  </si>
-  <si>
-    <t>Geben Sie eine gültige Nummer ein</t>
-  </si>
-  <si>
-    <t>Gidd eng gëlteg Nummer an</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -1147,9 +1084,6 @@
     <t>C - Natural sciences</t>
   </si>
   <si>
-    <t>I - Informatics</t>
-  </si>
-  <si>
     <t>A - Langues</t>
   </si>
   <si>
@@ -1397,6 +1331,24 @@
   </si>
   <si>
     <t>Zur Ganzzahl</t>
+  </si>
+  <si>
+    <t>Invalid</t>
+  </si>
+  <si>
+    <t>invalid</t>
+  </si>
+  <si>
+    <t>Invalide</t>
+  </si>
+  <si>
+    <t>Ungültig</t>
+  </si>
+  <si>
+    <t>Ongëlteg</t>
+  </si>
+  <si>
+    <t>I - Informatics &amp; Communication</t>
   </si>
 </sst>
 </file>
@@ -1458,10 +1410,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="string" displayName="string" ref="A1:E113" totalsRowShown="0">
-  <autoFilter ref="A1:E113" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E113">
-    <sortCondition ref="A1:A113"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="string" displayName="string" ref="A1:E105" totalsRowShown="0">
+  <autoFilter ref="A1:E105" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E105">
+    <sortCondition ref="A1:A105"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="keys"/>
@@ -1762,10 +1714,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E113"/>
+  <dimension ref="A1:E105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="D104" sqref="D104"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47:E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1796,1906 +1748,1770 @@
     </row>
     <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>449</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>367</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>375</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>383</v>
+        <v>26</v>
       </c>
       <c r="E2" t="s">
-        <v>392</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>43</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="E5" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="D7" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="E7" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>62</v>
+        <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>63</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>49</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>401</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="E9" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="B10" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="C10" t="s">
-        <v>423</v>
+        <v>54</v>
       </c>
       <c r="D10" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="E10" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C11" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="D11" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="E11" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>74</v>
+        <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>75</v>
+        <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>76</v>
+        <v>8</v>
       </c>
       <c r="E12" t="s">
-        <v>75</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>61</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="D13" t="s">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="E13" t="s">
-        <v>23</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>451</v>
+        <v>64</v>
       </c>
       <c r="B14" t="s">
-        <v>368</v>
+        <v>65</v>
       </c>
       <c r="C14" t="s">
-        <v>376</v>
+        <v>65</v>
       </c>
       <c r="D14" t="s">
-        <v>384</v>
+        <v>65</v>
       </c>
       <c r="E14" t="s">
-        <v>384</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>77</v>
+        <v>387</v>
       </c>
       <c r="B15" t="s">
-        <v>78</v>
+        <v>389</v>
       </c>
       <c r="C15" t="s">
-        <v>79</v>
+        <v>390</v>
       </c>
       <c r="D15" t="s">
-        <v>78</v>
+        <v>392</v>
       </c>
       <c r="E15" t="s">
-        <v>78</v>
+        <v>391</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>80</v>
+        <v>388</v>
       </c>
       <c r="B16" t="s">
-        <v>81</v>
+        <v>394</v>
       </c>
       <c r="C16" t="s">
-        <v>81</v>
+        <v>393</v>
       </c>
       <c r="D16" t="s">
-        <v>81</v>
+        <v>395</v>
       </c>
       <c r="E16" t="s">
-        <v>81</v>
+        <v>404</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>450</v>
+        <v>66</v>
       </c>
       <c r="B17" t="s">
-        <v>373</v>
+        <v>67</v>
       </c>
       <c r="C17" t="s">
-        <v>377</v>
+        <v>68</v>
       </c>
       <c r="D17" t="s">
-        <v>386</v>
+        <v>69</v>
       </c>
       <c r="E17" t="s">
-        <v>391</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>409</v>
+        <v>71</v>
       </c>
       <c r="B18" t="s">
-        <v>411</v>
+        <v>72</v>
       </c>
       <c r="C18" t="s">
-        <v>412</v>
+        <v>73</v>
       </c>
       <c r="D18" t="s">
-        <v>414</v>
+        <v>74</v>
       </c>
       <c r="E18" t="s">
-        <v>413</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>410</v>
+        <v>339</v>
       </c>
       <c r="B19" t="s">
-        <v>416</v>
+        <v>340</v>
       </c>
       <c r="C19" t="s">
-        <v>415</v>
+        <v>341</v>
       </c>
       <c r="D19" t="s">
-        <v>417</v>
+        <v>342</v>
       </c>
       <c r="E19" t="s">
-        <v>426</v>
+        <v>342</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B20" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C20" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D20" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="E20" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B21" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="C21" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="D21" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="E21" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>360</v>
+        <v>82</v>
       </c>
       <c r="B22" t="s">
-        <v>361</v>
+        <v>83</v>
       </c>
       <c r="C22" t="s">
-        <v>362</v>
+        <v>83</v>
       </c>
       <c r="D22" t="s">
-        <v>363</v>
+        <v>84</v>
       </c>
       <c r="E22" t="s">
-        <v>363</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B23" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C23" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D23" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E23" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>91</v>
+      </c>
+      <c r="B24" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24" t="s">
+        <v>93</v>
+      </c>
+      <c r="D24" t="s">
+        <v>94</v>
+      </c>
+      <c r="E24" t="s">
         <v>95</v>
-      </c>
-      <c r="B24" t="s">
-        <v>96</v>
-      </c>
-      <c r="C24" t="s">
-        <v>96</v>
-      </c>
-      <c r="D24" t="s">
-        <v>97</v>
-      </c>
-      <c r="E24" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>96</v>
+      </c>
+      <c r="B25" t="s">
+        <v>97</v>
+      </c>
+      <c r="C25" t="s">
         <v>98</v>
       </c>
-      <c r="B25" t="s">
+      <c r="D25" t="s">
         <v>99</v>
       </c>
-      <c r="C25" t="s">
+      <c r="E25" t="s">
         <v>99</v>
-      </c>
-      <c r="D25" t="s">
-        <v>100</v>
-      </c>
-      <c r="E25" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>100</v>
+      </c>
+      <c r="B26" t="s">
+        <v>101</v>
+      </c>
+      <c r="C26" t="s">
         <v>102</v>
       </c>
-      <c r="B26" t="s">
+      <c r="D26" t="s">
         <v>103</v>
       </c>
-      <c r="C26" t="s">
+      <c r="E26" t="s">
         <v>104</v>
-      </c>
-      <c r="D26" t="s">
-        <v>105</v>
-      </c>
-      <c r="E26" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>105</v>
+      </c>
+      <c r="B27" t="s">
+        <v>106</v>
+      </c>
+      <c r="C27" t="s">
         <v>107</v>
       </c>
-      <c r="B27" t="s">
+      <c r="D27" t="s">
         <v>108</v>
       </c>
-      <c r="C27" t="s">
+      <c r="E27" t="s">
         <v>109</v>
-      </c>
-      <c r="D27" t="s">
-        <v>110</v>
-      </c>
-      <c r="E27" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>110</v>
+      </c>
+      <c r="B28" t="s">
+        <v>111</v>
+      </c>
+      <c r="C28" t="s">
         <v>112</v>
       </c>
-      <c r="B28" t="s">
-        <v>113</v>
-      </c>
-      <c r="C28" t="s">
-        <v>114</v>
-      </c>
       <c r="D28" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E28" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>113</v>
+      </c>
+      <c r="B29" t="s">
+        <v>114</v>
+      </c>
+      <c r="C29" t="s">
+        <v>115</v>
+      </c>
+      <c r="D29" t="s">
         <v>116</v>
       </c>
-      <c r="B29" t="s">
+      <c r="E29" t="s">
         <v>117</v>
-      </c>
-      <c r="C29" t="s">
-        <v>118</v>
-      </c>
-      <c r="D29" t="s">
-        <v>119</v>
-      </c>
-      <c r="E29" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>118</v>
+      </c>
+      <c r="B30" t="s">
+        <v>119</v>
+      </c>
+      <c r="C30" t="s">
+        <v>120</v>
+      </c>
+      <c r="D30" t="s">
         <v>121</v>
       </c>
-      <c r="B30" t="s">
+      <c r="E30" t="s">
         <v>122</v>
-      </c>
-      <c r="C30" t="s">
-        <v>123</v>
-      </c>
-      <c r="D30" t="s">
-        <v>124</v>
-      </c>
-      <c r="E30" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>452</v>
+        <v>123</v>
       </c>
       <c r="B31" t="s">
-        <v>371</v>
+        <v>124</v>
       </c>
       <c r="C31" t="s">
-        <v>378</v>
+        <v>125</v>
       </c>
       <c r="D31" t="s">
-        <v>387</v>
+        <v>126</v>
       </c>
       <c r="E31" t="s">
-        <v>387</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B32" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C32" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D32" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="E32" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B33" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C33" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="D33" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="E33" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="B34" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="C34" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="D34" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="E34" t="s">
-        <v>138</v>
+        <v>405</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>453</v>
+        <v>142</v>
       </c>
       <c r="B35" t="s">
-        <v>369</v>
+        <v>143</v>
       </c>
       <c r="C35" t="s">
-        <v>379</v>
+        <v>144</v>
       </c>
       <c r="D35" t="s">
-        <v>385</v>
+        <v>145</v>
       </c>
       <c r="E35" t="s">
-        <v>393</v>
+        <v>146</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>139</v>
+        <v>21</v>
       </c>
       <c r="B36" t="s">
-        <v>140</v>
+        <v>22</v>
       </c>
       <c r="C36" t="s">
-        <v>141</v>
+        <v>22</v>
       </c>
       <c r="D36" t="s">
-        <v>142</v>
+        <v>22</v>
       </c>
       <c r="E36" t="s">
-        <v>143</v>
+        <v>22</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>144</v>
+        <v>13</v>
       </c>
       <c r="B37" t="s">
-        <v>145</v>
+        <v>14</v>
       </c>
       <c r="C37" t="s">
-        <v>146</v>
+        <v>14</v>
       </c>
       <c r="D37" t="s">
-        <v>147</v>
+        <v>14</v>
       </c>
       <c r="E37" t="s">
-        <v>148</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>149</v>
+        <v>17</v>
       </c>
       <c r="B38" t="s">
-        <v>150</v>
+        <v>18</v>
       </c>
       <c r="C38" t="s">
-        <v>151</v>
+        <v>18</v>
       </c>
       <c r="D38" t="s">
-        <v>152</v>
+        <v>18</v>
       </c>
       <c r="E38" t="s">
-        <v>153</v>
+        <v>18</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="B39" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="C39" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="D39" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="E39" t="s">
-        <v>427</v>
+        <v>151</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>158</v>
+        <v>15</v>
       </c>
       <c r="B40" t="s">
-        <v>159</v>
+        <v>16</v>
       </c>
       <c r="C40" t="s">
-        <v>160</v>
+        <v>16</v>
       </c>
       <c r="D40" t="s">
-        <v>161</v>
+        <v>16</v>
       </c>
       <c r="E40" t="s">
-        <v>162</v>
+        <v>16</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>37</v>
+        <v>152</v>
       </c>
       <c r="B41" t="s">
-        <v>38</v>
+        <v>153</v>
       </c>
       <c r="C41" t="s">
-        <v>38</v>
+        <v>154</v>
       </c>
       <c r="D41" t="s">
-        <v>38</v>
+        <v>155</v>
       </c>
       <c r="E41" t="s">
-        <v>38</v>
+        <v>155</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="B42" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="C42" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="D42" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="E42" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>339</v>
+        <v>156</v>
       </c>
       <c r="B43" t="s">
-        <v>340</v>
+        <v>157</v>
       </c>
       <c r="C43" t="s">
-        <v>341</v>
+        <v>158</v>
       </c>
       <c r="D43" t="s">
-        <v>342</v>
+        <v>158</v>
       </c>
       <c r="E43" t="s">
-        <v>343</v>
+        <v>159</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>454</v>
+        <v>160</v>
       </c>
       <c r="B44" t="s">
-        <v>370</v>
+        <v>161</v>
       </c>
       <c r="C44" t="s">
-        <v>380</v>
+        <v>162</v>
       </c>
       <c r="D44" t="s">
-        <v>388</v>
+        <v>163</v>
       </c>
       <c r="E44" t="s">
-        <v>394</v>
+        <v>164</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>33</v>
+        <v>165</v>
       </c>
       <c r="B45" t="s">
-        <v>34</v>
+        <v>166</v>
       </c>
       <c r="C45" t="s">
-        <v>34</v>
+        <v>167</v>
       </c>
       <c r="D45" t="s">
-        <v>34</v>
+        <v>168</v>
       </c>
       <c r="E45" t="s">
-        <v>34</v>
+        <v>169</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>455</v>
+        <v>170</v>
       </c>
       <c r="B46" t="s">
-        <v>372</v>
+        <v>171</v>
       </c>
       <c r="C46" t="s">
-        <v>381</v>
+        <v>172</v>
       </c>
       <c r="D46" t="s">
-        <v>389</v>
+        <v>173</v>
       </c>
       <c r="E46" t="s">
-        <v>428</v>
+        <v>174</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>163</v>
+        <v>437</v>
       </c>
       <c r="B47" t="s">
-        <v>164</v>
+        <v>436</v>
       </c>
       <c r="C47" t="s">
-        <v>165</v>
+        <v>438</v>
       </c>
       <c r="D47" t="s">
-        <v>166</v>
+        <v>439</v>
       </c>
       <c r="E47" t="s">
-        <v>167</v>
+        <v>440</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>31</v>
+        <v>175</v>
       </c>
       <c r="B48" t="s">
-        <v>32</v>
+        <v>176</v>
       </c>
       <c r="C48" t="s">
-        <v>32</v>
+        <v>177</v>
       </c>
       <c r="D48" t="s">
-        <v>32</v>
+        <v>178</v>
       </c>
       <c r="E48" t="s">
-        <v>32</v>
+        <v>179</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>168</v>
+        <v>180</v>
       </c>
       <c r="B49" t="s">
-        <v>169</v>
+        <v>181</v>
       </c>
       <c r="C49" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="D49" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="E49" t="s">
-        <v>171</v>
+        <v>183</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>27</v>
+        <v>184</v>
       </c>
       <c r="B50" t="s">
-        <v>28</v>
+        <v>185</v>
       </c>
       <c r="C50" t="s">
-        <v>28</v>
+        <v>185</v>
       </c>
       <c r="D50" t="s">
-        <v>28</v>
+        <v>186</v>
       </c>
       <c r="E50" t="s">
-        <v>28</v>
+        <v>186</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>172</v>
+        <v>187</v>
       </c>
       <c r="B51" t="s">
-        <v>173</v>
+        <v>188</v>
       </c>
       <c r="C51" t="s">
-        <v>174</v>
+        <v>189</v>
       </c>
       <c r="D51" t="s">
-        <v>174</v>
+        <v>190</v>
       </c>
       <c r="E51" t="s">
-        <v>175</v>
+        <v>191</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="B52" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C52" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="D52" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E52" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>9</v>
+        <v>327</v>
       </c>
       <c r="B53" t="s">
-        <v>10</v>
+        <v>328</v>
       </c>
       <c r="C53" t="s">
-        <v>10</v>
+        <v>328</v>
       </c>
       <c r="D53" t="s">
-        <v>10</v>
+        <v>328</v>
       </c>
       <c r="E53" t="s">
-        <v>10</v>
+        <v>328</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>11</v>
+        <v>329</v>
       </c>
       <c r="B54" t="s">
-        <v>12</v>
+        <v>330</v>
       </c>
       <c r="C54" t="s">
-        <v>12</v>
+        <v>331</v>
       </c>
       <c r="D54" t="s">
-        <v>12</v>
+        <v>332</v>
       </c>
       <c r="E54" t="s">
-        <v>12</v>
+        <v>333</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>176</v>
+        <v>323</v>
       </c>
       <c r="B55" t="s">
-        <v>177</v>
+        <v>324</v>
       </c>
       <c r="C55" t="s">
-        <v>178</v>
+        <v>325</v>
       </c>
       <c r="D55" t="s">
-        <v>179</v>
+        <v>324</v>
       </c>
       <c r="E55" t="s">
-        <v>180</v>
+        <v>326</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>181</v>
+        <v>192</v>
       </c>
       <c r="B56" t="s">
-        <v>182</v>
+        <v>193</v>
       </c>
       <c r="C56" t="s">
-        <v>183</v>
+        <v>194</v>
       </c>
       <c r="D56" t="s">
-        <v>184</v>
+        <v>195</v>
       </c>
       <c r="E56" t="s">
-        <v>185</v>
+        <v>196</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>186</v>
+        <v>378</v>
       </c>
       <c r="B57" t="s">
-        <v>187</v>
+        <v>380</v>
       </c>
       <c r="C57" t="s">
-        <v>188</v>
+        <v>382</v>
       </c>
       <c r="D57" t="s">
-        <v>189</v>
+        <v>384</v>
       </c>
       <c r="E57" t="s">
-        <v>190</v>
+        <v>386</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>456</v>
+        <v>334</v>
       </c>
       <c r="B58" t="s">
-        <v>374</v>
+        <v>335</v>
       </c>
       <c r="C58" t="s">
-        <v>382</v>
+        <v>336</v>
       </c>
       <c r="D58" t="s">
-        <v>390</v>
+        <v>337</v>
       </c>
       <c r="E58" t="s">
-        <v>395</v>
+        <v>338</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="B59" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="C59" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="D59" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="E59" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="B60" t="s">
-        <v>197</v>
+        <v>398</v>
       </c>
       <c r="C60" t="s">
-        <v>197</v>
+        <v>399</v>
       </c>
       <c r="D60" t="s">
-        <v>198</v>
+        <v>400</v>
       </c>
       <c r="E60" t="s">
-        <v>199</v>
+        <v>407</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>200</v>
+        <v>396</v>
       </c>
       <c r="B61" t="s">
-        <v>201</v>
+        <v>397</v>
       </c>
       <c r="C61" t="s">
-        <v>201</v>
+        <v>397</v>
       </c>
       <c r="D61" t="s">
-        <v>202</v>
+        <v>397</v>
       </c>
       <c r="E61" t="s">
-        <v>202</v>
+        <v>397</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>202</v>
+      </c>
+      <c r="B62" t="s">
         <v>203</v>
       </c>
-      <c r="B62" t="s">
+      <c r="C62" t="s">
         <v>204</v>
       </c>
-      <c r="C62" t="s">
+      <c r="D62" t="s">
         <v>205</v>
       </c>
-      <c r="D62" t="s">
-        <v>206</v>
-      </c>
       <c r="E62" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>35</v>
+        <v>206</v>
       </c>
       <c r="B63" t="s">
-        <v>36</v>
+        <v>207</v>
       </c>
       <c r="C63" t="s">
-        <v>36</v>
+        <v>208</v>
       </c>
       <c r="D63" t="s">
-        <v>36</v>
+        <v>209</v>
       </c>
       <c r="E63" t="s">
-        <v>36</v>
+        <v>210</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>348</v>
+        <v>211</v>
       </c>
       <c r="B64" t="s">
-        <v>349</v>
+        <v>212</v>
       </c>
       <c r="C64" t="s">
-        <v>349</v>
+        <v>213</v>
       </c>
       <c r="D64" t="s">
-        <v>349</v>
+        <v>214</v>
       </c>
       <c r="E64" t="s">
-        <v>349</v>
+        <v>215</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>20</v>
+        <v>216</v>
       </c>
       <c r="B65" t="s">
-        <v>21</v>
+        <v>217</v>
       </c>
       <c r="C65" t="s">
-        <v>21</v>
+        <v>218</v>
       </c>
       <c r="D65" t="s">
-        <v>21</v>
+        <v>219</v>
       </c>
       <c r="E65" t="s">
-        <v>21</v>
+        <v>220</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>350</v>
+        <v>221</v>
       </c>
       <c r="B66" t="s">
-        <v>351</v>
+        <v>222</v>
       </c>
       <c r="C66" t="s">
-        <v>352</v>
+        <v>223</v>
       </c>
       <c r="D66" t="s">
-        <v>353</v>
+        <v>224</v>
       </c>
       <c r="E66" t="s">
-        <v>354</v>
+        <v>225</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>344</v>
+        <v>226</v>
       </c>
       <c r="B67" t="s">
-        <v>345</v>
+        <v>227</v>
       </c>
       <c r="C67" t="s">
-        <v>346</v>
+        <v>402</v>
       </c>
       <c r="D67" t="s">
-        <v>345</v>
+        <v>228</v>
       </c>
       <c r="E67" t="s">
-        <v>347</v>
+        <v>408</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>208</v>
+        <v>229</v>
       </c>
       <c r="B68" t="s">
-        <v>209</v>
+        <v>230</v>
       </c>
       <c r="C68" t="s">
-        <v>210</v>
+        <v>231</v>
       </c>
       <c r="D68" t="s">
-        <v>211</v>
+        <v>232</v>
       </c>
       <c r="E68" t="s">
-        <v>212</v>
+        <v>233</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>400</v>
+        <v>234</v>
       </c>
       <c r="B69" t="s">
-        <v>402</v>
+        <v>235</v>
       </c>
       <c r="C69" t="s">
-        <v>404</v>
+        <v>236</v>
       </c>
       <c r="D69" t="s">
-        <v>406</v>
+        <v>237</v>
       </c>
       <c r="E69" t="s">
-        <v>408</v>
+        <v>238</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>355</v>
+        <v>239</v>
       </c>
       <c r="B70" t="s">
-        <v>356</v>
+        <v>240</v>
       </c>
       <c r="C70" t="s">
-        <v>357</v>
+        <v>241</v>
       </c>
       <c r="D70" t="s">
-        <v>358</v>
+        <v>242</v>
       </c>
       <c r="E70" t="s">
-        <v>359</v>
+        <v>243</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>213</v>
+        <v>343</v>
       </c>
       <c r="B71" t="s">
-        <v>214</v>
+        <v>344</v>
       </c>
       <c r="C71" t="s">
-        <v>214</v>
+        <v>344</v>
       </c>
       <c r="D71" t="s">
-        <v>215</v>
+        <v>344</v>
       </c>
       <c r="E71" t="s">
-        <v>216</v>
+        <v>345</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>217</v>
+        <v>427</v>
       </c>
       <c r="B72" t="s">
-        <v>420</v>
+        <v>346</v>
       </c>
       <c r="C72" t="s">
-        <v>421</v>
+        <v>353</v>
       </c>
       <c r="D72" t="s">
-        <v>422</v>
+        <v>361</v>
       </c>
       <c r="E72" t="s">
-        <v>429</v>
+        <v>370</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>418</v>
+        <v>429</v>
       </c>
       <c r="B73" t="s">
-        <v>419</v>
+        <v>347</v>
       </c>
       <c r="C73" t="s">
-        <v>419</v>
+        <v>354</v>
       </c>
       <c r="D73" t="s">
-        <v>419</v>
+        <v>362</v>
       </c>
       <c r="E73" t="s">
-        <v>419</v>
+        <v>362</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>26</v>
+        <v>428</v>
       </c>
       <c r="B74" t="s">
-        <v>17</v>
+        <v>352</v>
       </c>
       <c r="C74" t="s">
-        <v>17</v>
+        <v>355</v>
       </c>
       <c r="D74" t="s">
-        <v>17</v>
+        <v>364</v>
       </c>
       <c r="E74" t="s">
-        <v>17</v>
+        <v>369</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>218</v>
+        <v>430</v>
       </c>
       <c r="B75" t="s">
-        <v>219</v>
+        <v>350</v>
       </c>
       <c r="C75" t="s">
-        <v>220</v>
+        <v>356</v>
       </c>
       <c r="D75" t="s">
-        <v>221</v>
+        <v>365</v>
       </c>
       <c r="E75" t="s">
-        <v>221</v>
+        <v>365</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>222</v>
+        <v>431</v>
       </c>
       <c r="B76" t="s">
-        <v>223</v>
+        <v>348</v>
       </c>
       <c r="C76" t="s">
-        <v>224</v>
+        <v>357</v>
       </c>
       <c r="D76" t="s">
-        <v>225</v>
+        <v>363</v>
       </c>
       <c r="E76" t="s">
-        <v>226</v>
+        <v>371</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>18</v>
+        <v>432</v>
       </c>
       <c r="B77" t="s">
-        <v>19</v>
+        <v>349</v>
       </c>
       <c r="C77" t="s">
-        <v>19</v>
+        <v>358</v>
       </c>
       <c r="D77" t="s">
-        <v>19</v>
+        <v>366</v>
       </c>
       <c r="E77" t="s">
-        <v>19</v>
+        <v>372</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>227</v>
+        <v>433</v>
       </c>
       <c r="B78" t="s">
-        <v>228</v>
+        <v>351</v>
       </c>
       <c r="C78" t="s">
-        <v>229</v>
+        <v>359</v>
       </c>
       <c r="D78" t="s">
-        <v>230</v>
+        <v>367</v>
       </c>
       <c r="E78" t="s">
-        <v>231</v>
+        <v>406</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>232</v>
+        <v>434</v>
       </c>
       <c r="B79" t="s">
-        <v>233</v>
+        <v>441</v>
       </c>
       <c r="C79" t="s">
-        <v>234</v>
+        <v>360</v>
       </c>
       <c r="D79" t="s">
-        <v>235</v>
+        <v>368</v>
       </c>
       <c r="E79" t="s">
-        <v>236</v>
+        <v>373</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="B80" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="C80" t="s">
-        <v>239</v>
+        <v>246</v>
       </c>
       <c r="D80" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
       <c r="E80" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>242</v>
+        <v>249</v>
       </c>
       <c r="B81" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
       <c r="C81" t="s">
-        <v>424</v>
+        <v>251</v>
       </c>
       <c r="D81" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="E81" t="s">
-        <v>430</v>
+        <v>250</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
       <c r="B82" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="C82" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
       <c r="D82" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="E82" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="B83" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="C83" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="D83" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="E83" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="B84" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="C84" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="D84" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="E84" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>364</v>
+        <v>264</v>
       </c>
       <c r="B85" t="s">
-        <v>365</v>
+        <v>265</v>
       </c>
       <c r="C85" t="s">
-        <v>365</v>
+        <v>266</v>
       </c>
       <c r="D85" t="s">
-        <v>365</v>
+        <v>267</v>
       </c>
       <c r="E85" t="s">
-        <v>366</v>
+        <v>268</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>260</v>
+        <v>269</v>
       </c>
       <c r="B86" t="s">
-        <v>261</v>
+        <v>270</v>
       </c>
       <c r="C86" t="s">
-        <v>262</v>
+        <v>271</v>
       </c>
       <c r="D86" t="s">
-        <v>263</v>
+        <v>272</v>
       </c>
       <c r="E86" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>265</v>
+        <v>274</v>
       </c>
       <c r="B87" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
       <c r="C87" t="s">
-        <v>267</v>
+        <v>276</v>
       </c>
       <c r="D87" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
       <c r="E87" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>268</v>
+        <v>374</v>
       </c>
       <c r="B88" t="s">
-        <v>269</v>
+        <v>375</v>
       </c>
       <c r="C88" t="s">
-        <v>270</v>
+        <v>376</v>
       </c>
       <c r="D88" t="s">
-        <v>269</v>
+        <v>375</v>
       </c>
       <c r="E88" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>271</v>
+        <v>278</v>
       </c>
       <c r="B89" t="s">
-        <v>272</v>
+        <v>279</v>
       </c>
       <c r="C89" t="s">
-        <v>273</v>
+        <v>280</v>
       </c>
       <c r="D89" t="s">
-        <v>274</v>
+        <v>281</v>
       </c>
       <c r="E89" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>275</v>
+        <v>282</v>
       </c>
       <c r="B90" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="C90" t="s">
-        <v>277</v>
+        <v>284</v>
       </c>
       <c r="D90" t="s">
-        <v>278</v>
+        <v>285</v>
       </c>
       <c r="E90" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>280</v>
+        <v>423</v>
       </c>
       <c r="B91" t="s">
-        <v>281</v>
+        <v>424</v>
       </c>
       <c r="C91" t="s">
-        <v>282</v>
+        <v>425</v>
       </c>
       <c r="D91" t="s">
-        <v>283</v>
+        <v>426</v>
       </c>
       <c r="E91" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>13</v>
+        <v>410</v>
       </c>
       <c r="B92" t="s">
-        <v>14</v>
+        <v>419</v>
       </c>
       <c r="C92" t="s">
-        <v>14</v>
+        <v>420</v>
       </c>
       <c r="D92" t="s">
-        <v>14</v>
+        <v>421</v>
       </c>
       <c r="E92" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>285</v>
+        <v>409</v>
       </c>
       <c r="B93" t="s">
-        <v>286</v>
+        <v>416</v>
       </c>
       <c r="C93" t="s">
-        <v>287</v>
+        <v>417</v>
       </c>
       <c r="D93" t="s">
-        <v>288</v>
+        <v>418</v>
       </c>
       <c r="E93" t="s">
-        <v>289</v>
+        <v>418</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>290</v>
+        <v>412</v>
       </c>
       <c r="B94" t="s">
-        <v>291</v>
+        <v>411</v>
       </c>
       <c r="C94" t="s">
-        <v>292</v>
+        <v>413</v>
       </c>
       <c r="D94" t="s">
-        <v>293</v>
+        <v>414</v>
       </c>
       <c r="E94" t="s">
-        <v>293</v>
+        <v>415</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>396</v>
+        <v>286</v>
       </c>
       <c r="B95" t="s">
-        <v>397</v>
+        <v>287</v>
       </c>
       <c r="C95" t="s">
-        <v>398</v>
+        <v>288</v>
       </c>
       <c r="D95" t="s">
-        <v>397</v>
+        <v>289</v>
       </c>
       <c r="E95" t="s">
-        <v>397</v>
+        <v>289</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B96" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C96" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D96" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="E96" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B97" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C97" t="s">
-        <v>300</v>
+        <v>403</v>
       </c>
       <c r="D97" t="s">
-        <v>301</v>
+        <v>435</v>
       </c>
       <c r="E97" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>445</v>
+        <v>297</v>
       </c>
       <c r="B98" t="s">
-        <v>446</v>
+        <v>298</v>
       </c>
       <c r="C98" t="s">
-        <v>447</v>
+        <v>299</v>
       </c>
       <c r="D98" t="s">
-        <v>448</v>
+        <v>298</v>
       </c>
       <c r="E98" t="s">
-        <v>448</v>
+        <v>298</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>432</v>
+        <v>300</v>
       </c>
       <c r="B99" t="s">
-        <v>441</v>
+        <v>301</v>
       </c>
       <c r="C99" t="s">
-        <v>442</v>
+        <v>302</v>
       </c>
       <c r="D99" t="s">
-        <v>443</v>
+        <v>301</v>
       </c>
       <c r="E99" t="s">
-        <v>444</v>
+        <v>301</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>431</v>
+        <v>303</v>
       </c>
       <c r="B100" t="s">
-        <v>438</v>
+        <v>304</v>
       </c>
       <c r="C100" t="s">
-        <v>439</v>
+        <v>305</v>
       </c>
       <c r="D100" t="s">
-        <v>440</v>
+        <v>304</v>
       </c>
       <c r="E100" t="s">
-        <v>440</v>
+        <v>304</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>434</v>
+        <v>306</v>
       </c>
       <c r="B101" t="s">
-        <v>433</v>
+        <v>307</v>
       </c>
       <c r="C101" t="s">
-        <v>435</v>
+        <v>308</v>
       </c>
       <c r="D101" t="s">
-        <v>436</v>
+        <v>309</v>
       </c>
       <c r="E101" t="s">
-        <v>437</v>
+        <v>309</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>302</v>
+        <v>310</v>
       </c>
       <c r="B102" t="s">
-        <v>303</v>
+        <v>311</v>
       </c>
       <c r="C102" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
       <c r="D102" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
       <c r="E102" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>306</v>
+        <v>315</v>
       </c>
       <c r="B103" t="s">
-        <v>307</v>
+        <v>316</v>
       </c>
       <c r="C103" t="s">
-        <v>308</v>
+        <v>317</v>
       </c>
       <c r="D103" t="s">
-        <v>309</v>
+        <v>317</v>
       </c>
       <c r="E103" t="s">
-        <v>309</v>
+        <v>317</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>310</v>
+        <v>318</v>
       </c>
       <c r="B104" t="s">
-        <v>311</v>
+        <v>319</v>
       </c>
       <c r="C104" t="s">
-        <v>425</v>
+        <v>320</v>
       </c>
       <c r="D104" t="s">
-        <v>457</v>
+        <v>321</v>
       </c>
       <c r="E104" t="s">
-        <v>312</v>
+        <v>322</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>313</v>
+        <v>377</v>
       </c>
       <c r="B105" t="s">
-        <v>314</v>
+        <v>379</v>
       </c>
       <c r="C105" t="s">
-        <v>315</v>
+        <v>381</v>
       </c>
       <c r="D105" t="s">
-        <v>314</v>
+        <v>383</v>
       </c>
       <c r="E105" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>316</v>
-      </c>
-      <c r="B106" t="s">
-        <v>317</v>
-      </c>
-      <c r="C106" t="s">
-        <v>318</v>
-      </c>
-      <c r="D106" t="s">
-        <v>317</v>
-      </c>
-      <c r="E106" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>319</v>
-      </c>
-      <c r="B107" t="s">
-        <v>320</v>
-      </c>
-      <c r="C107" t="s">
-        <v>321</v>
-      </c>
-      <c r="D107" t="s">
-        <v>320</v>
-      </c>
-      <c r="E107" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>322</v>
-      </c>
-      <c r="B108" t="s">
-        <v>323</v>
-      </c>
-      <c r="C108" t="s">
-        <v>324</v>
-      </c>
-      <c r="D108" t="s">
-        <v>325</v>
-      </c>
-      <c r="E108" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>326</v>
-      </c>
-      <c r="B109" t="s">
-        <v>327</v>
-      </c>
-      <c r="C109" t="s">
-        <v>328</v>
-      </c>
-      <c r="D109" t="s">
-        <v>329</v>
-      </c>
-      <c r="E109" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>331</v>
-      </c>
-      <c r="B110" t="s">
-        <v>332</v>
-      </c>
-      <c r="C110" t="s">
-        <v>333</v>
-      </c>
-      <c r="D110" t="s">
-        <v>333</v>
-      </c>
-      <c r="E110" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>334</v>
-      </c>
-      <c r="B111" t="s">
-        <v>335</v>
-      </c>
-      <c r="C111" t="s">
-        <v>336</v>
-      </c>
-      <c r="D111" t="s">
-        <v>337</v>
-      </c>
-      <c r="E111" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>399</v>
-      </c>
-      <c r="B112" t="s">
-        <v>401</v>
-      </c>
-      <c r="C112" t="s">
-        <v>403</v>
-      </c>
-      <c r="D112" t="s">
-        <v>405</v>
-      </c>
-      <c r="E112" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>15</v>
-      </c>
-      <c r="B113" t="s">
-        <v>16</v>
-      </c>
-      <c r="C113" t="s">
-        <v>16</v>
-      </c>
-      <c r="D113" t="s">
-        <v>16</v>
-      </c>
-      <c r="E113" t="s">
-        <v>16</v>
+        <v>385</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add fallback when deserialization fails
</commit_message>
<xml_diff>
--- a/assets/Localizations.xlsx
+++ b/assets/Localizations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Grade.ly\Grade.ly - Flutter\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83AF88EE-141D-401D-ABE3-37DADF48BBB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC0F211-D823-49F2-902A-93F17FC895A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="string" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0">string!$A$1:$B$106</definedName>
+    <definedName name="ExternalData_1" localSheetId="0">string!$A$1:$B$107</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="452">
   <si>
     <t>keys</t>
   </si>
@@ -1364,6 +1364,21 @@
   </si>
   <si>
     <t>Systemsprooch</t>
+  </si>
+  <si>
+    <t>storage_error</t>
+  </si>
+  <si>
+    <t>There was an error loading your saved data, so it has been deleted.</t>
+  </si>
+  <si>
+    <t>Une erreur s'est produite lors du chargement de vos données sauvegardées, elles ont donc été supprimées.</t>
+  </si>
+  <si>
+    <t>Es ist ein Fehler beim Laden Ihrer gespeicherten Daten aufgetreten, daher wurden sie gelöscht.</t>
+  </si>
+  <si>
+    <t>Et ass e Feeler beim Lueden vun ären gespäicherten Donnéeën opgetrueden, dofir goufen se geläscht.</t>
   </si>
 </sst>
 </file>
@@ -1425,10 +1440,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="string" displayName="string" ref="A1:E106" totalsRowShown="0">
-  <autoFilter ref="A1:E106" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E106">
-    <sortCondition ref="A1:A106"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="string" displayName="string" ref="A1:E107" totalsRowShown="0">
+  <autoFilter ref="A1:E107" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E107">
+    <sortCondition ref="A1:A107"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="keys"/>
@@ -1729,10 +1744,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E106"/>
+  <dimension ref="A1:E107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="C85" sqref="C85"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="B104" sqref="B104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3208,36 +3223,36 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>274</v>
+        <v>447</v>
       </c>
       <c r="B87" t="s">
-        <v>275</v>
+        <v>448</v>
       </c>
       <c r="C87" t="s">
-        <v>276</v>
+        <v>449</v>
       </c>
       <c r="D87" t="s">
-        <v>277</v>
+        <v>450</v>
       </c>
       <c r="E87" t="s">
-        <v>277</v>
+        <v>451</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>442</v>
+        <v>274</v>
       </c>
       <c r="B88" t="s">
-        <v>443</v>
+        <v>275</v>
       </c>
       <c r="C88" t="s">
-        <v>444</v>
+        <v>276</v>
       </c>
       <c r="D88" t="s">
-        <v>445</v>
+        <v>277</v>
       </c>
       <c r="E88" t="s">
-        <v>446</v>
+        <v>277</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -3259,290 +3274,307 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>278</v>
+        <v>442</v>
       </c>
       <c r="B90" t="s">
-        <v>279</v>
+        <v>443</v>
       </c>
       <c r="C90" t="s">
-        <v>280</v>
+        <v>444</v>
       </c>
       <c r="D90" t="s">
-        <v>281</v>
+        <v>445</v>
       </c>
       <c r="E90" t="s">
-        <v>281</v>
+        <v>446</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="B91" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="C91" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D91" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="E91" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>423</v>
+        <v>282</v>
       </c>
       <c r="B92" t="s">
-        <v>424</v>
+        <v>283</v>
       </c>
       <c r="C92" t="s">
-        <v>425</v>
+        <v>284</v>
       </c>
       <c r="D92" t="s">
-        <v>426</v>
+        <v>285</v>
       </c>
       <c r="E92" t="s">
-        <v>426</v>
+        <v>285</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>410</v>
+        <v>423</v>
       </c>
       <c r="B93" t="s">
-        <v>419</v>
+        <v>424</v>
       </c>
       <c r="C93" t="s">
-        <v>420</v>
+        <v>425</v>
       </c>
       <c r="D93" t="s">
-        <v>421</v>
+        <v>426</v>
       </c>
       <c r="E93" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="B94" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="C94" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="D94" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="E94" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="B95" t="s">
-        <v>411</v>
+        <v>416</v>
       </c>
       <c r="C95" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="D95" t="s">
-        <v>414</v>
+        <v>418</v>
       </c>
       <c r="E95" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>286</v>
+        <v>412</v>
       </c>
       <c r="B96" t="s">
-        <v>287</v>
+        <v>411</v>
       </c>
       <c r="C96" t="s">
-        <v>288</v>
+        <v>413</v>
       </c>
       <c r="D96" t="s">
-        <v>289</v>
+        <v>414</v>
       </c>
       <c r="E96" t="s">
-        <v>289</v>
+        <v>415</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="B97" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="C97" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="D97" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="E97" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B98" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C98" t="s">
-        <v>403</v>
+        <v>292</v>
       </c>
       <c r="D98" t="s">
-        <v>435</v>
+        <v>293</v>
       </c>
       <c r="E98" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B99" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C99" t="s">
-        <v>299</v>
+        <v>403</v>
       </c>
       <c r="D99" t="s">
-        <v>298</v>
+        <v>435</v>
       </c>
       <c r="E99" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="B100" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C100" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D100" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="E100" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="B101" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C101" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="D101" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="E101" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B102" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C102" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="D102" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="E102" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="B103" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="C103" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="D103" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="E103" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="B104" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="C104" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="D104" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="E104" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="B105" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C105" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="D105" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="E105" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
+        <v>318</v>
+      </c>
+      <c r="B106" t="s">
+        <v>319</v>
+      </c>
+      <c r="C106" t="s">
+        <v>320</v>
+      </c>
+      <c r="D106" t="s">
+        <v>321</v>
+      </c>
+      <c r="E106" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
         <v>377</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B107" t="s">
         <v>379</v>
       </c>
-      <c r="C106" t="s">
+      <c r="C107" t="s">
         <v>381</v>
       </c>
-      <c r="D106" t="s">
+      <c r="D107" t="s">
         <v>383</v>
       </c>
-      <c r="E106" t="s">
+      <c r="E107" t="s">
         <v>385</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Improved year view to be clearer
</commit_message>
<xml_diff>
--- a/assets/Localizations.xlsx
+++ b/assets/Localizations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Grade.ly\Grade.ly - Flutter\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC0F211-D823-49F2-902A-93F17FC895A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7508ECB0-9F3A-4211-91E8-8BE9E799758F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="string" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0">string!$A$1:$B$107</definedName>
+    <definedName name="ExternalData_1" localSheetId="0">string!$A$1:$B$109</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="462">
   <si>
     <t>keys</t>
   </si>
@@ -1379,6 +1379,36 @@
   </si>
   <si>
     <t>Et ass e Feeler beim Lueden vun ären gespäicherten Donnéeën opgetrueden, dofir goufen se geläscht.</t>
+  </si>
+  <si>
+    <t>year_overview</t>
+  </si>
+  <si>
+    <t>Jahresübersicht</t>
+  </si>
+  <si>
+    <t>Joresiwwersiicht</t>
+  </si>
+  <si>
+    <t>Aperçu de l'année</t>
+  </si>
+  <si>
+    <t>yearly_average</t>
+  </si>
+  <si>
+    <t>Yearly average</t>
+  </si>
+  <si>
+    <t>Year overview</t>
+  </si>
+  <si>
+    <t>Moyenne annuelle</t>
+  </si>
+  <si>
+    <t>Jahresdurchschnitt</t>
+  </si>
+  <si>
+    <t>Joresmoyenne</t>
   </si>
 </sst>
 </file>
@@ -1440,10 +1470,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="string" displayName="string" ref="A1:E107" totalsRowShown="0">
-  <autoFilter ref="A1:E107" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E107">
-    <sortCondition ref="A1:A107"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="string" displayName="string" ref="A1:E109" totalsRowShown="0">
+  <autoFilter ref="A1:E109" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E109">
+    <sortCondition ref="A1:A109"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="keys"/>
@@ -1744,10 +1774,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E107"/>
+  <dimension ref="A1:E109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="B104" sqref="B104"/>
+    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="B93" sqref="B93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3563,18 +3593,52 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
+        <v>452</v>
+      </c>
+      <c r="B107" t="s">
+        <v>458</v>
+      </c>
+      <c r="C107" t="s">
+        <v>455</v>
+      </c>
+      <c r="D107" t="s">
+        <v>453</v>
+      </c>
+      <c r="E107" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>456</v>
+      </c>
+      <c r="B108" t="s">
+        <v>457</v>
+      </c>
+      <c r="C108" t="s">
+        <v>459</v>
+      </c>
+      <c r="D108" t="s">
+        <v>460</v>
+      </c>
+      <c r="E108" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
         <v>377</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B109" t="s">
         <v>379</v>
       </c>
-      <c r="C107" t="s">
+      <c r="C109" t="s">
         <v>381</v>
       </c>
-      <c r="D107" t="s">
+      <c r="D109" t="s">
         <v>383</v>
       </c>
-      <c r="E107" t="s">
+      <c r="E109" t="s">
         <v>385</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Unify dialogs and fix their padding
</commit_message>
<xml_diff>
--- a/assets/Localizations.xlsx
+++ b/assets/Localizations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Grade.ly\Grade.ly - Flutter\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1F2CDD9-8F2E-45FD-855D-945F564550E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96164258-19AF-4A71-ADBB-2D84742F5552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="string" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0">string!$A$1:$B$109</definedName>
+    <definedName name="ExternalData_1" localSheetId="0">string!$A$1:$B$111</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="475">
   <si>
     <t>keys</t>
   </si>
@@ -1213,9 +1213,6 @@
     <t>ok</t>
   </si>
   <si>
-    <t>Ok</t>
-  </si>
-  <si>
     <t>You can always edit your subjects and other options in the settings later</t>
   </si>
   <si>
@@ -1418,6 +1415,39 @@
   </si>
   <si>
     <t>NightDream Games\nEntwéckler - Damien Pirotte\nVisuell Identitéit - Ellia Walrave\nTesting - Louis Colbus</t>
+  </si>
+  <si>
+    <t>cancel</t>
+  </si>
+  <si>
+    <t>Cancel</t>
+  </si>
+  <si>
+    <t>Annuler</t>
+  </si>
+  <si>
+    <t>Abbrechen</t>
+  </si>
+  <si>
+    <t>Ofbriechen</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>save</t>
+  </si>
+  <si>
+    <t>Save</t>
+  </si>
+  <si>
+    <t>Sauvegarder</t>
+  </si>
+  <si>
+    <t>Speichern</t>
+  </si>
+  <si>
+    <t>Späicheren</t>
   </si>
 </sst>
 </file>
@@ -1479,10 +1509,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="string" displayName="string" ref="A1:E109" totalsRowShown="0">
-  <autoFilter ref="A1:E109" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E109">
-    <sortCondition ref="A1:A109"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="string" displayName="string" ref="A1:E111" totalsRowShown="0">
+  <autoFilter ref="A1:E111" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E111">
+    <sortCondition ref="A1:A111"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="keys"/>
@@ -1783,10 +1813,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E109"/>
+  <dimension ref="A1:E111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="E111" sqref="E111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1837,16 +1867,16 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
+        <v>461</v>
+      </c>
+      <c r="C3" t="s">
+        <v>460</v>
+      </c>
+      <c r="D3" t="s">
         <v>462</v>
       </c>
-      <c r="C3" t="s">
-        <v>461</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>463</v>
-      </c>
-      <c r="E3" t="s">
-        <v>464</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1942,7 +1972,7 @@
         <v>48</v>
       </c>
       <c r="C9" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D9" t="s">
         <v>49</v>
@@ -2038,1616 +2068,1650 @@
     </row>
     <row r="15" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>386</v>
+        <v>464</v>
       </c>
       <c r="B15" t="s">
-        <v>388</v>
+        <v>465</v>
       </c>
       <c r="C15" t="s">
-        <v>389</v>
+        <v>466</v>
       </c>
       <c r="D15" t="s">
-        <v>391</v>
+        <v>467</v>
       </c>
       <c r="E15" t="s">
-        <v>390</v>
+        <v>468</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B16" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="C16" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D16" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="E16" t="s">
-        <v>403</v>
+        <v>390</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>65</v>
+        <v>387</v>
       </c>
       <c r="B17" t="s">
-        <v>66</v>
+        <v>393</v>
       </c>
       <c r="C17" t="s">
-        <v>67</v>
+        <v>392</v>
       </c>
       <c r="D17" t="s">
-        <v>68</v>
+        <v>394</v>
       </c>
       <c r="E17" t="s">
-        <v>69</v>
+        <v>402</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B18" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C18" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D18" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E18" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>338</v>
+        <v>70</v>
       </c>
       <c r="B19" t="s">
-        <v>339</v>
+        <v>71</v>
       </c>
       <c r="C19" t="s">
-        <v>340</v>
+        <v>72</v>
       </c>
       <c r="D19" t="s">
-        <v>341</v>
+        <v>73</v>
       </c>
       <c r="E19" t="s">
-        <v>341</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>75</v>
+        <v>338</v>
       </c>
       <c r="B20" t="s">
-        <v>76</v>
+        <v>339</v>
       </c>
       <c r="C20" t="s">
-        <v>76</v>
+        <v>340</v>
       </c>
       <c r="D20" t="s">
-        <v>77</v>
+        <v>341</v>
       </c>
       <c r="E20" t="s">
-        <v>77</v>
+        <v>341</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B21" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C21" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D21" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E21" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B22" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C22" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D22" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E22" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B23" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C23" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D23" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E23" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B24" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C24" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D24" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E24" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B25" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C25" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D25" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E25" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B26" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C26" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D26" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E26" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B27" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C27" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D27" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E27" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B28" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C28" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D28" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E28" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B29" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C29" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D29" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E29" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B30" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C30" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D30" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E30" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B31" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C31" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="D31" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="E31" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B32" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C32" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D32" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="E32" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B33" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C33" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="D33" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E33" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B34" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C34" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D34" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E34" t="s">
-        <v>404</v>
+        <v>136</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B35" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C35" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D35" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E35" t="s">
-        <v>145</v>
+        <v>403</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>20</v>
+        <v>141</v>
       </c>
       <c r="B36" t="s">
-        <v>21</v>
+        <v>142</v>
       </c>
       <c r="C36" t="s">
-        <v>21</v>
+        <v>143</v>
       </c>
       <c r="D36" t="s">
-        <v>21</v>
+        <v>144</v>
       </c>
       <c r="E36" t="s">
-        <v>21</v>
+        <v>145</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B37" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C37" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D37" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E37" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B38" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C38" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D38" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E38" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>146</v>
+        <v>16</v>
       </c>
       <c r="B39" t="s">
-        <v>147</v>
+        <v>17</v>
       </c>
       <c r="C39" t="s">
-        <v>148</v>
+        <v>17</v>
       </c>
       <c r="D39" t="s">
-        <v>149</v>
+        <v>17</v>
       </c>
       <c r="E39" t="s">
-        <v>150</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>14</v>
+        <v>146</v>
       </c>
       <c r="B40" t="s">
-        <v>15</v>
+        <v>147</v>
       </c>
       <c r="C40" t="s">
-        <v>15</v>
+        <v>148</v>
       </c>
       <c r="D40" t="s">
-        <v>15</v>
+        <v>149</v>
       </c>
       <c r="E40" t="s">
-        <v>15</v>
+        <v>150</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>151</v>
+        <v>14</v>
       </c>
       <c r="B41" t="s">
-        <v>152</v>
+        <v>15</v>
       </c>
       <c r="C41" t="s">
-        <v>153</v>
+        <v>15</v>
       </c>
       <c r="D41" t="s">
-        <v>154</v>
+        <v>15</v>
       </c>
       <c r="E41" t="s">
-        <v>154</v>
+        <v>15</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>10</v>
+        <v>151</v>
       </c>
       <c r="B42" t="s">
-        <v>11</v>
+        <v>152</v>
       </c>
       <c r="C42" t="s">
-        <v>11</v>
+        <v>153</v>
       </c>
       <c r="D42" t="s">
-        <v>11</v>
+        <v>154</v>
       </c>
       <c r="E42" t="s">
-        <v>11</v>
+        <v>154</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>155</v>
+        <v>10</v>
       </c>
       <c r="B43" t="s">
-        <v>156</v>
+        <v>11</v>
       </c>
       <c r="C43" t="s">
-        <v>157</v>
+        <v>11</v>
       </c>
       <c r="D43" t="s">
-        <v>157</v>
+        <v>11</v>
       </c>
       <c r="E43" t="s">
-        <v>158</v>
+        <v>11</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B44" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C44" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D44" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="E44" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B45" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C45" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="D45" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="E45" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B46" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C46" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D46" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E46" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>436</v>
+        <v>169</v>
       </c>
       <c r="B47" t="s">
-        <v>435</v>
+        <v>170</v>
       </c>
       <c r="C47" t="s">
-        <v>437</v>
+        <v>171</v>
       </c>
       <c r="D47" t="s">
-        <v>438</v>
+        <v>172</v>
       </c>
       <c r="E47" t="s">
-        <v>439</v>
+        <v>173</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>174</v>
+        <v>435</v>
       </c>
       <c r="B48" t="s">
-        <v>175</v>
+        <v>434</v>
       </c>
       <c r="C48" t="s">
-        <v>176</v>
+        <v>436</v>
       </c>
       <c r="D48" t="s">
-        <v>177</v>
+        <v>437</v>
       </c>
       <c r="E48" t="s">
-        <v>178</v>
+        <v>438</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="B49" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="C49" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D49" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E49" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B50" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C50" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D50" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E50" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B51" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C51" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D51" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E51" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>18</v>
+        <v>186</v>
       </c>
       <c r="B52" t="s">
-        <v>19</v>
+        <v>187</v>
       </c>
       <c r="C52" t="s">
-        <v>19</v>
+        <v>188</v>
       </c>
       <c r="D52" t="s">
-        <v>19</v>
+        <v>189</v>
       </c>
       <c r="E52" t="s">
-        <v>19</v>
+        <v>190</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>326</v>
+        <v>18</v>
       </c>
       <c r="B53" t="s">
-        <v>327</v>
+        <v>19</v>
       </c>
       <c r="C53" t="s">
-        <v>327</v>
+        <v>19</v>
       </c>
       <c r="D53" t="s">
-        <v>327</v>
+        <v>19</v>
       </c>
       <c r="E53" t="s">
-        <v>327</v>
+        <v>19</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B54" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C54" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="D54" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="E54" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>322</v>
+        <v>328</v>
       </c>
       <c r="B55" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
       <c r="C55" t="s">
-        <v>324</v>
+        <v>330</v>
       </c>
       <c r="D55" t="s">
-        <v>323</v>
+        <v>331</v>
       </c>
       <c r="E55" t="s">
-        <v>325</v>
+        <v>332</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>191</v>
+        <v>322</v>
       </c>
       <c r="B56" t="s">
-        <v>192</v>
+        <v>323</v>
       </c>
       <c r="C56" t="s">
-        <v>193</v>
+        <v>324</v>
       </c>
       <c r="D56" t="s">
-        <v>194</v>
+        <v>323</v>
       </c>
       <c r="E56" t="s">
-        <v>195</v>
+        <v>325</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>377</v>
+        <v>191</v>
       </c>
       <c r="B57" t="s">
-        <v>379</v>
+        <v>192</v>
       </c>
       <c r="C57" t="s">
-        <v>381</v>
+        <v>193</v>
       </c>
       <c r="D57" t="s">
-        <v>383</v>
+        <v>194</v>
       </c>
       <c r="E57" t="s">
-        <v>385</v>
+        <v>195</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>333</v>
+        <v>377</v>
       </c>
       <c r="B58" t="s">
-        <v>334</v>
+        <v>379</v>
       </c>
       <c r="C58" t="s">
-        <v>335</v>
+        <v>381</v>
       </c>
       <c r="D58" t="s">
-        <v>336</v>
+        <v>383</v>
       </c>
       <c r="E58" t="s">
-        <v>337</v>
+        <v>385</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>196</v>
+        <v>333</v>
       </c>
       <c r="B59" t="s">
-        <v>197</v>
+        <v>334</v>
       </c>
       <c r="C59" t="s">
-        <v>197</v>
+        <v>335</v>
       </c>
       <c r="D59" t="s">
-        <v>198</v>
+        <v>336</v>
       </c>
       <c r="E59" t="s">
-        <v>199</v>
+        <v>337</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B60" t="s">
-        <v>397</v>
+        <v>197</v>
       </c>
       <c r="C60" t="s">
-        <v>398</v>
+        <v>197</v>
       </c>
       <c r="D60" t="s">
-        <v>399</v>
+        <v>198</v>
       </c>
       <c r="E60" t="s">
-        <v>406</v>
+        <v>199</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>395</v>
+        <v>200</v>
       </c>
       <c r="B61" t="s">
         <v>396</v>
       </c>
       <c r="C61" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D61" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="E61" t="s">
-        <v>396</v>
+        <v>405</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>201</v>
+        <v>395</v>
       </c>
       <c r="B62" t="s">
-        <v>202</v>
+        <v>469</v>
       </c>
       <c r="C62" t="s">
-        <v>203</v>
+        <v>469</v>
       </c>
       <c r="D62" t="s">
-        <v>204</v>
+        <v>469</v>
       </c>
       <c r="E62" t="s">
-        <v>204</v>
+        <v>469</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B63" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C63" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D63" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E63" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B64" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C64" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="D64" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="E64" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B65" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="C65" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="D65" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="E65" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="B66" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="C66" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D66" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="E66" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="B67" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="C67" t="s">
-        <v>401</v>
+        <v>222</v>
       </c>
       <c r="D67" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="E67" t="s">
-        <v>407</v>
+        <v>224</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B68" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C68" t="s">
-        <v>230</v>
+        <v>400</v>
       </c>
       <c r="D68" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E68" t="s">
-        <v>232</v>
+        <v>406</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B69" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="C69" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="D69" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="E69" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="B70" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="C70" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="D70" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="E70" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>342</v>
+        <v>470</v>
       </c>
       <c r="B71" t="s">
-        <v>343</v>
+        <v>471</v>
       </c>
       <c r="C71" t="s">
-        <v>343</v>
+        <v>472</v>
       </c>
       <c r="D71" t="s">
-        <v>343</v>
+        <v>473</v>
       </c>
       <c r="E71" t="s">
-        <v>344</v>
+        <v>474</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>426</v>
+        <v>238</v>
       </c>
       <c r="B72" t="s">
-        <v>345</v>
+        <v>239</v>
       </c>
       <c r="C72" t="s">
-        <v>352</v>
+        <v>240</v>
       </c>
       <c r="D72" t="s">
-        <v>360</v>
+        <v>241</v>
       </c>
       <c r="E72" t="s">
-        <v>369</v>
+        <v>242</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>428</v>
+        <v>342</v>
       </c>
       <c r="B73" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C73" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="D73" t="s">
-        <v>361</v>
+        <v>343</v>
       </c>
       <c r="E73" t="s">
-        <v>361</v>
+        <v>344</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B74" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="C74" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D74" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="E74" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B75" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="C75" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D75" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="E75" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="B76" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="C76" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D76" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="E76" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="B77" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C77" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D77" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E77" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="B78" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C78" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D78" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="E78" t="s">
-        <v>405</v>
+        <v>370</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="B79" t="s">
-        <v>440</v>
+        <v>348</v>
       </c>
       <c r="C79" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D79" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="E79" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>243</v>
+        <v>431</v>
       </c>
       <c r="B80" t="s">
-        <v>244</v>
+        <v>350</v>
       </c>
       <c r="C80" t="s">
-        <v>245</v>
+        <v>358</v>
       </c>
       <c r="D80" t="s">
-        <v>246</v>
+        <v>366</v>
       </c>
       <c r="E80" t="s">
-        <v>247</v>
+        <v>404</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>248</v>
+        <v>432</v>
       </c>
       <c r="B81" t="s">
-        <v>249</v>
+        <v>439</v>
       </c>
       <c r="C81" t="s">
-        <v>250</v>
+        <v>359</v>
       </c>
       <c r="D81" t="s">
-        <v>249</v>
+        <v>367</v>
       </c>
       <c r="E81" t="s">
-        <v>249</v>
+        <v>372</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="B82" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="C82" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="D82" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="E82" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="B83" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="C83" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="D83" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="E83" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="B84" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="C84" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="D84" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="E84" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="B85" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="C85" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="D85" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="E85" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
       <c r="B86" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="C86" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="D86" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="E86" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>446</v>
+        <v>263</v>
       </c>
       <c r="B87" t="s">
-        <v>447</v>
+        <v>264</v>
       </c>
       <c r="C87" t="s">
-        <v>448</v>
+        <v>265</v>
       </c>
       <c r="D87" t="s">
-        <v>449</v>
+        <v>266</v>
       </c>
       <c r="E87" t="s">
-        <v>450</v>
+        <v>267</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B88" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="C88" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="D88" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="E88" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>373</v>
+        <v>445</v>
       </c>
       <c r="B89" t="s">
-        <v>374</v>
+        <v>446</v>
       </c>
       <c r="C89" t="s">
-        <v>375</v>
+        <v>447</v>
       </c>
       <c r="D89" t="s">
-        <v>374</v>
+        <v>448</v>
       </c>
       <c r="E89" t="s">
-        <v>374</v>
+        <v>449</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>441</v>
+        <v>273</v>
       </c>
       <c r="B90" t="s">
-        <v>442</v>
+        <v>274</v>
       </c>
       <c r="C90" t="s">
-        <v>443</v>
+        <v>275</v>
       </c>
       <c r="D90" t="s">
-        <v>444</v>
+        <v>276</v>
       </c>
       <c r="E90" t="s">
-        <v>445</v>
+        <v>276</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>277</v>
+        <v>373</v>
       </c>
       <c r="B91" t="s">
-        <v>278</v>
+        <v>374</v>
       </c>
       <c r="C91" t="s">
-        <v>279</v>
+        <v>375</v>
       </c>
       <c r="D91" t="s">
-        <v>280</v>
+        <v>374</v>
       </c>
       <c r="E91" t="s">
-        <v>280</v>
+        <v>374</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>281</v>
+        <v>440</v>
       </c>
       <c r="B92" t="s">
-        <v>282</v>
+        <v>441</v>
       </c>
       <c r="C92" t="s">
-        <v>283</v>
+        <v>442</v>
       </c>
       <c r="D92" t="s">
-        <v>284</v>
+        <v>443</v>
       </c>
       <c r="E92" t="s">
-        <v>284</v>
+        <v>444</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>422</v>
+        <v>277</v>
       </c>
       <c r="B93" t="s">
-        <v>423</v>
+        <v>278</v>
       </c>
       <c r="C93" t="s">
-        <v>424</v>
+        <v>279</v>
       </c>
       <c r="D93" t="s">
-        <v>425</v>
+        <v>280</v>
       </c>
       <c r="E93" t="s">
-        <v>425</v>
+        <v>280</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>409</v>
+        <v>281</v>
       </c>
       <c r="B94" t="s">
-        <v>418</v>
+        <v>282</v>
       </c>
       <c r="C94" t="s">
-        <v>419</v>
+        <v>283</v>
       </c>
       <c r="D94" t="s">
-        <v>420</v>
+        <v>284</v>
       </c>
       <c r="E94" t="s">
-        <v>421</v>
+        <v>284</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>408</v>
+        <v>421</v>
       </c>
       <c r="B95" t="s">
-        <v>415</v>
+        <v>422</v>
       </c>
       <c r="C95" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
       <c r="D95" t="s">
-        <v>417</v>
+        <v>424</v>
       </c>
       <c r="E95" t="s">
-        <v>417</v>
+        <v>424</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="B96" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
       <c r="C96" t="s">
-        <v>412</v>
+        <v>418</v>
       </c>
       <c r="D96" t="s">
-        <v>413</v>
+        <v>419</v>
       </c>
       <c r="E96" t="s">
-        <v>414</v>
+        <v>420</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>285</v>
+        <v>407</v>
       </c>
       <c r="B97" t="s">
-        <v>286</v>
+        <v>414</v>
       </c>
       <c r="C97" t="s">
-        <v>287</v>
+        <v>415</v>
       </c>
       <c r="D97" t="s">
-        <v>288</v>
+        <v>416</v>
       </c>
       <c r="E97" t="s">
-        <v>288</v>
+        <v>416</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>289</v>
+        <v>410</v>
       </c>
       <c r="B98" t="s">
-        <v>290</v>
+        <v>409</v>
       </c>
       <c r="C98" t="s">
-        <v>291</v>
+        <v>411</v>
       </c>
       <c r="D98" t="s">
-        <v>292</v>
+        <v>412</v>
       </c>
       <c r="E98" t="s">
-        <v>292</v>
+        <v>413</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="B99" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="C99" t="s">
-        <v>402</v>
+        <v>287</v>
       </c>
       <c r="D99" t="s">
-        <v>434</v>
+        <v>288</v>
       </c>
       <c r="E99" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="B100" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="C100" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="D100" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="E100" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="B101" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="C101" t="s">
-        <v>301</v>
+        <v>401</v>
       </c>
       <c r="D101" t="s">
-        <v>300</v>
+        <v>433</v>
       </c>
       <c r="E101" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="B102" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="C102" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="D102" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="E102" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="B103" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="C103" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="D103" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="E103" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="B104" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="C104" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="D104" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="E104" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="B105" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="C105" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="D105" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="E105" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="B106" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="C106" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="D106" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="E106" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>451</v>
+        <v>314</v>
       </c>
       <c r="B107" t="s">
-        <v>457</v>
+        <v>315</v>
       </c>
       <c r="C107" t="s">
-        <v>454</v>
+        <v>316</v>
       </c>
       <c r="D107" t="s">
-        <v>452</v>
+        <v>316</v>
       </c>
       <c r="E107" t="s">
-        <v>453</v>
+        <v>316</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>455</v>
+        <v>317</v>
       </c>
       <c r="B108" t="s">
-        <v>456</v>
+        <v>318</v>
       </c>
       <c r="C108" t="s">
-        <v>458</v>
+        <v>319</v>
       </c>
       <c r="D108" t="s">
-        <v>459</v>
+        <v>320</v>
       </c>
       <c r="E108" t="s">
-        <v>460</v>
+        <v>321</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
+        <v>450</v>
+      </c>
+      <c r="B109" t="s">
+        <v>456</v>
+      </c>
+      <c r="C109" t="s">
+        <v>453</v>
+      </c>
+      <c r="D109" t="s">
+        <v>451</v>
+      </c>
+      <c r="E109" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>454</v>
+      </c>
+      <c r="B110" t="s">
+        <v>455</v>
+      </c>
+      <c r="C110" t="s">
+        <v>457</v>
+      </c>
+      <c r="D110" t="s">
+        <v>458</v>
+      </c>
+      <c r="E110" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
         <v>376</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B111" t="s">
         <v>378</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C111" t="s">
         <v>380</v>
       </c>
-      <c r="D109" t="s">
+      <c r="D111" t="s">
         <v>382</v>
       </c>
-      <c r="E109" t="s">
+      <c r="E111" t="s">
         <v>384</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Change app name to "Graded"
</commit_message>
<xml_diff>
--- a/assets/Localizations.xlsx
+++ b/assets/Localizations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Grade.ly\Grade.ly - Flutter\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96164258-19AF-4A71-ADBB-2D84742F5552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F22157FB-F1E4-4115-B9A8-00369FC692DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,9 +43,6 @@
     <t>app_name</t>
   </si>
   <si>
-    <t>Grade.ly</t>
-  </si>
-  <si>
     <t>az</t>
   </si>
   <si>
@@ -58,9 +55,6 @@
     <t>github_summary</t>
   </si>
   <si>
-    <t>https://github.com/NightDreamGames/Grade.ly</t>
-  </si>
-  <si>
     <t>english</t>
   </si>
   <si>
@@ -1448,13 +1442,19 @@
   </si>
   <si>
     <t>Späicheren</t>
+  </si>
+  <si>
+    <t>Graded</t>
+  </si>
+  <si>
+    <t>https://github.com/NightDreamGames/Graded</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1464,6 +1464,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1486,13 +1494,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1815,8 +1826,8 @@
   </sheetPr>
   <dimension ref="A1:E111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
-      <selection activeCell="E111" sqref="E111"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43:E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1847,104 +1858,104 @@
     </row>
     <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
         <v>22</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>23</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>24</v>
-      </c>
-      <c r="D2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
+        <v>459</v>
+      </c>
+      <c r="C3" t="s">
+        <v>458</v>
+      </c>
+      <c r="D3" t="s">
+        <v>460</v>
+      </c>
+      <c r="E3" t="s">
         <v>461</v>
-      </c>
-      <c r="C3" t="s">
-        <v>460</v>
-      </c>
-      <c r="D3" t="s">
-        <v>462</v>
-      </c>
-      <c r="E3" t="s">
-        <v>463</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
         <v>27</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>28</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>29</v>
-      </c>
-      <c r="D4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
         <v>32</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>33</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>34</v>
-      </c>
-      <c r="D5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
         <v>37</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
         <v>38</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
         <v>39</v>
-      </c>
-      <c r="D6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" t="s">
         <v>42</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D7" t="s">
         <v>43</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
         <v>44</v>
-      </c>
-      <c r="D7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E7" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1952,1775 +1963,1779 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>473</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>473</v>
       </c>
       <c r="D8" t="s">
-        <v>6</v>
+        <v>473</v>
       </c>
       <c r="E8" t="s">
-        <v>6</v>
+        <v>473</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" t="s">
+        <v>397</v>
+      </c>
+      <c r="D9" t="s">
         <v>47</v>
       </c>
-      <c r="B9" t="s">
+      <c r="E9" t="s">
         <v>48</v>
-      </c>
-      <c r="C9" t="s">
-        <v>399</v>
-      </c>
-      <c r="D9" t="s">
-        <v>49</v>
-      </c>
-      <c r="E9" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" t="s">
         <v>51</v>
       </c>
-      <c r="B10" t="s">
+      <c r="D10" t="s">
         <v>52</v>
       </c>
-      <c r="C10" t="s">
+      <c r="E10" t="s">
         <v>53</v>
-      </c>
-      <c r="D10" t="s">
-        <v>54</v>
-      </c>
-      <c r="E10" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" t="s">
         <v>56</v>
       </c>
-      <c r="B11" t="s">
+      <c r="D11" t="s">
         <v>57</v>
       </c>
-      <c r="C11" t="s">
-        <v>58</v>
-      </c>
-      <c r="D11" t="s">
-        <v>59</v>
-      </c>
       <c r="E11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
         <v>7</v>
       </c>
-      <c r="B12" t="s">
-        <v>8</v>
-      </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" t="s">
         <v>60</v>
       </c>
-      <c r="B13" t="s">
-        <v>61</v>
-      </c>
-      <c r="C13" t="s">
-        <v>62</v>
-      </c>
       <c r="D13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>462</v>
+      </c>
+      <c r="B15" t="s">
+        <v>463</v>
+      </c>
+      <c r="C15" t="s">
         <v>464</v>
       </c>
-      <c r="B15" t="s">
+      <c r="D15" t="s">
         <v>465</v>
       </c>
-      <c r="C15" t="s">
+      <c r="E15" t="s">
         <v>466</v>
-      </c>
-      <c r="D15" t="s">
-        <v>467</v>
-      </c>
-      <c r="E15" t="s">
-        <v>468</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>384</v>
+      </c>
+      <c r="B16" t="s">
         <v>386</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
+        <v>387</v>
+      </c>
+      <c r="D16" t="s">
+        <v>389</v>
+      </c>
+      <c r="E16" t="s">
         <v>388</v>
-      </c>
-      <c r="C16" t="s">
-        <v>389</v>
-      </c>
-      <c r="D16" t="s">
-        <v>391</v>
-      </c>
-      <c r="E16" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B17" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C17" t="s">
+        <v>390</v>
+      </c>
+      <c r="D17" t="s">
         <v>392</v>
       </c>
-      <c r="D17" t="s">
-        <v>394</v>
-      </c>
       <c r="E17" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" t="s">
         <v>65</v>
       </c>
-      <c r="B18" t="s">
+      <c r="D18" t="s">
         <v>66</v>
       </c>
-      <c r="C18" t="s">
+      <c r="E18" t="s">
         <v>67</v>
-      </c>
-      <c r="D18" t="s">
-        <v>68</v>
-      </c>
-      <c r="E18" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" t="s">
         <v>70</v>
       </c>
-      <c r="B19" t="s">
+      <c r="D19" t="s">
         <v>71</v>
       </c>
-      <c r="C19" t="s">
+      <c r="E19" t="s">
         <v>72</v>
-      </c>
-      <c r="D19" t="s">
-        <v>73</v>
-      </c>
-      <c r="E19" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>336</v>
+      </c>
+      <c r="B20" t="s">
+        <v>337</v>
+      </c>
+      <c r="C20" t="s">
         <v>338</v>
       </c>
-      <c r="B20" t="s">
+      <c r="D20" t="s">
         <v>339</v>
       </c>
-      <c r="C20" t="s">
-        <v>340</v>
-      </c>
-      <c r="D20" t="s">
-        <v>341</v>
-      </c>
       <c r="E20" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21" t="s">
         <v>75</v>
       </c>
-      <c r="B21" t="s">
-        <v>76</v>
-      </c>
-      <c r="C21" t="s">
-        <v>76</v>
-      </c>
-      <c r="D21" t="s">
-        <v>77</v>
-      </c>
       <c r="E21" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" t="s">
+        <v>77</v>
+      </c>
+      <c r="C22" t="s">
+        <v>77</v>
+      </c>
+      <c r="D22" t="s">
         <v>78</v>
       </c>
-      <c r="B22" t="s">
-        <v>79</v>
-      </c>
-      <c r="C22" t="s">
-        <v>79</v>
-      </c>
-      <c r="D22" t="s">
-        <v>80</v>
-      </c>
       <c r="E22" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>79</v>
+      </c>
+      <c r="B23" t="s">
+        <v>80</v>
+      </c>
+      <c r="C23" t="s">
+        <v>80</v>
+      </c>
+      <c r="D23" t="s">
         <v>81</v>
       </c>
-      <c r="B23" t="s">
+      <c r="E23" t="s">
         <v>82</v>
-      </c>
-      <c r="C23" t="s">
-        <v>82</v>
-      </c>
-      <c r="D23" t="s">
-        <v>83</v>
-      </c>
-      <c r="E23" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>83</v>
+      </c>
+      <c r="B24" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24" t="s">
         <v>85</v>
       </c>
-      <c r="B24" t="s">
+      <c r="D24" t="s">
         <v>86</v>
       </c>
-      <c r="C24" t="s">
+      <c r="E24" t="s">
         <v>87</v>
-      </c>
-      <c r="D24" t="s">
-        <v>88</v>
-      </c>
-      <c r="E24" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>88</v>
+      </c>
+      <c r="B25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25" t="s">
         <v>90</v>
       </c>
-      <c r="B25" t="s">
+      <c r="D25" t="s">
         <v>91</v>
       </c>
-      <c r="C25" t="s">
+      <c r="E25" t="s">
         <v>92</v>
-      </c>
-      <c r="D25" t="s">
-        <v>93</v>
-      </c>
-      <c r="E25" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>93</v>
+      </c>
+      <c r="B26" t="s">
+        <v>94</v>
+      </c>
+      <c r="C26" t="s">
         <v>95</v>
       </c>
-      <c r="B26" t="s">
+      <c r="D26" t="s">
         <v>96</v>
       </c>
-      <c r="C26" t="s">
-        <v>97</v>
-      </c>
-      <c r="D26" t="s">
-        <v>98</v>
-      </c>
       <c r="E26" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>97</v>
+      </c>
+      <c r="B27" t="s">
+        <v>98</v>
+      </c>
+      <c r="C27" t="s">
         <v>99</v>
       </c>
-      <c r="B27" t="s">
+      <c r="D27" t="s">
         <v>100</v>
       </c>
-      <c r="C27" t="s">
+      <c r="E27" t="s">
         <v>101</v>
-      </c>
-      <c r="D27" t="s">
-        <v>102</v>
-      </c>
-      <c r="E27" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>102</v>
+      </c>
+      <c r="B28" t="s">
+        <v>103</v>
+      </c>
+      <c r="C28" t="s">
         <v>104</v>
       </c>
-      <c r="B28" t="s">
+      <c r="D28" t="s">
         <v>105</v>
       </c>
-      <c r="C28" t="s">
+      <c r="E28" t="s">
         <v>106</v>
-      </c>
-      <c r="D28" t="s">
-        <v>107</v>
-      </c>
-      <c r="E28" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>107</v>
+      </c>
+      <c r="B29" t="s">
+        <v>108</v>
+      </c>
+      <c r="C29" t="s">
         <v>109</v>
       </c>
-      <c r="B29" t="s">
-        <v>110</v>
-      </c>
-      <c r="C29" t="s">
-        <v>111</v>
-      </c>
       <c r="D29" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E29" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>110</v>
+      </c>
+      <c r="B30" t="s">
+        <v>111</v>
+      </c>
+      <c r="C30" t="s">
         <v>112</v>
       </c>
-      <c r="B30" t="s">
+      <c r="D30" t="s">
         <v>113</v>
       </c>
-      <c r="C30" t="s">
+      <c r="E30" t="s">
         <v>114</v>
-      </c>
-      <c r="D30" t="s">
-        <v>115</v>
-      </c>
-      <c r="E30" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>115</v>
+      </c>
+      <c r="B31" t="s">
+        <v>116</v>
+      </c>
+      <c r="C31" t="s">
         <v>117</v>
       </c>
-      <c r="B31" t="s">
+      <c r="D31" t="s">
         <v>118</v>
       </c>
-      <c r="C31" t="s">
+      <c r="E31" t="s">
         <v>119</v>
-      </c>
-      <c r="D31" t="s">
-        <v>120</v>
-      </c>
-      <c r="E31" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>120</v>
+      </c>
+      <c r="B32" t="s">
+        <v>121</v>
+      </c>
+      <c r="C32" t="s">
         <v>122</v>
       </c>
-      <c r="B32" t="s">
+      <c r="D32" t="s">
         <v>123</v>
       </c>
-      <c r="C32" t="s">
+      <c r="E32" t="s">
         <v>124</v>
-      </c>
-      <c r="D32" t="s">
-        <v>125</v>
-      </c>
-      <c r="E32" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>125</v>
+      </c>
+      <c r="B33" t="s">
+        <v>126</v>
+      </c>
+      <c r="C33" t="s">
         <v>127</v>
       </c>
-      <c r="B33" t="s">
+      <c r="D33" t="s">
         <v>128</v>
       </c>
-      <c r="C33" t="s">
+      <c r="E33" t="s">
         <v>129</v>
-      </c>
-      <c r="D33" t="s">
-        <v>130</v>
-      </c>
-      <c r="E33" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>130</v>
+      </c>
+      <c r="B34" t="s">
+        <v>131</v>
+      </c>
+      <c r="C34" t="s">
         <v>132</v>
       </c>
-      <c r="B34" t="s">
+      <c r="D34" t="s">
         <v>133</v>
       </c>
-      <c r="C34" t="s">
+      <c r="E34" t="s">
         <v>134</v>
-      </c>
-      <c r="D34" t="s">
-        <v>135</v>
-      </c>
-      <c r="E34" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>135</v>
+      </c>
+      <c r="B35" t="s">
+        <v>136</v>
+      </c>
+      <c r="C35" t="s">
         <v>137</v>
       </c>
-      <c r="B35" t="s">
+      <c r="D35" t="s">
         <v>138</v>
       </c>
-      <c r="C35" t="s">
-        <v>139</v>
-      </c>
-      <c r="D35" t="s">
-        <v>140</v>
-      </c>
       <c r="E35" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>139</v>
+      </c>
+      <c r="B36" t="s">
+        <v>140</v>
+      </c>
+      <c r="C36" t="s">
         <v>141</v>
       </c>
-      <c r="B36" t="s">
+      <c r="D36" t="s">
         <v>142</v>
       </c>
-      <c r="C36" t="s">
+      <c r="E36" t="s">
         <v>143</v>
-      </c>
-      <c r="D36" t="s">
-        <v>144</v>
-      </c>
-      <c r="E36" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B37" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C37" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D37" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E37" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B38" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C38" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D38" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E38" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B39" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C39" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D39" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E39" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>144</v>
+      </c>
+      <c r="B40" t="s">
+        <v>145</v>
+      </c>
+      <c r="C40" t="s">
         <v>146</v>
       </c>
-      <c r="B40" t="s">
+      <c r="D40" t="s">
         <v>147</v>
       </c>
-      <c r="C40" t="s">
+      <c r="E40" t="s">
         <v>148</v>
-      </c>
-      <c r="D40" t="s">
-        <v>149</v>
-      </c>
-      <c r="E40" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B41" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C41" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D41" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E41" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>149</v>
+      </c>
+      <c r="B42" t="s">
+        <v>150</v>
+      </c>
+      <c r="C42" t="s">
         <v>151</v>
       </c>
-      <c r="B42" t="s">
+      <c r="D42" t="s">
         <v>152</v>
       </c>
-      <c r="C42" t="s">
-        <v>153</v>
-      </c>
-      <c r="D42" t="s">
-        <v>154</v>
-      </c>
       <c r="E42" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>10</v>
-      </c>
-      <c r="B43" t="s">
-        <v>11</v>
-      </c>
-      <c r="C43" t="s">
-        <v>11</v>
-      </c>
-      <c r="D43" t="s">
-        <v>11</v>
-      </c>
-      <c r="E43" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>153</v>
+      </c>
+      <c r="B44" t="s">
+        <v>154</v>
+      </c>
+      <c r="C44" t="s">
         <v>155</v>
       </c>
-      <c r="B44" t="s">
+      <c r="D44" t="s">
+        <v>155</v>
+      </c>
+      <c r="E44" t="s">
         <v>156</v>
-      </c>
-      <c r="C44" t="s">
-        <v>157</v>
-      </c>
-      <c r="D44" t="s">
-        <v>157</v>
-      </c>
-      <c r="E44" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>157</v>
+      </c>
+      <c r="B45" t="s">
+        <v>158</v>
+      </c>
+      <c r="C45" t="s">
         <v>159</v>
       </c>
-      <c r="B45" t="s">
+      <c r="D45" t="s">
         <v>160</v>
       </c>
-      <c r="C45" t="s">
+      <c r="E45" t="s">
         <v>161</v>
-      </c>
-      <c r="D45" t="s">
-        <v>162</v>
-      </c>
-      <c r="E45" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>162</v>
+      </c>
+      <c r="B46" t="s">
+        <v>163</v>
+      </c>
+      <c r="C46" t="s">
         <v>164</v>
       </c>
-      <c r="B46" t="s">
+      <c r="D46" t="s">
         <v>165</v>
       </c>
-      <c r="C46" t="s">
+      <c r="E46" t="s">
         <v>166</v>
-      </c>
-      <c r="D46" t="s">
-        <v>167</v>
-      </c>
-      <c r="E46" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>167</v>
+      </c>
+      <c r="B47" t="s">
+        <v>168</v>
+      </c>
+      <c r="C47" t="s">
         <v>169</v>
       </c>
-      <c r="B47" t="s">
+      <c r="D47" t="s">
         <v>170</v>
       </c>
-      <c r="C47" t="s">
+      <c r="E47" t="s">
         <v>171</v>
-      </c>
-      <c r="D47" t="s">
-        <v>172</v>
-      </c>
-      <c r="E47" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>433</v>
+      </c>
+      <c r="B48" t="s">
+        <v>432</v>
+      </c>
+      <c r="C48" t="s">
+        <v>434</v>
+      </c>
+      <c r="D48" t="s">
         <v>435</v>
       </c>
-      <c r="B48" t="s">
-        <v>434</v>
-      </c>
-      <c r="C48" t="s">
+      <c r="E48" t="s">
         <v>436</v>
-      </c>
-      <c r="D48" t="s">
-        <v>437</v>
-      </c>
-      <c r="E48" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>172</v>
+      </c>
+      <c r="B49" t="s">
+        <v>173</v>
+      </c>
+      <c r="C49" t="s">
         <v>174</v>
       </c>
-      <c r="B49" t="s">
+      <c r="D49" t="s">
         <v>175</v>
       </c>
-      <c r="C49" t="s">
+      <c r="E49" t="s">
         <v>176</v>
-      </c>
-      <c r="D49" t="s">
-        <v>177</v>
-      </c>
-      <c r="E49" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>177</v>
+      </c>
+      <c r="B50" t="s">
+        <v>178</v>
+      </c>
+      <c r="C50" t="s">
+        <v>178</v>
+      </c>
+      <c r="D50" t="s">
         <v>179</v>
       </c>
-      <c r="B50" t="s">
+      <c r="E50" t="s">
         <v>180</v>
-      </c>
-      <c r="C50" t="s">
-        <v>180</v>
-      </c>
-      <c r="D50" t="s">
-        <v>181</v>
-      </c>
-      <c r="E50" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>181</v>
+      </c>
+      <c r="B51" t="s">
+        <v>182</v>
+      </c>
+      <c r="C51" t="s">
+        <v>182</v>
+      </c>
+      <c r="D51" t="s">
         <v>183</v>
       </c>
-      <c r="B51" t="s">
-        <v>184</v>
-      </c>
-      <c r="C51" t="s">
-        <v>184</v>
-      </c>
-      <c r="D51" t="s">
-        <v>185</v>
-      </c>
       <c r="E51" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>184</v>
+      </c>
+      <c r="B52" t="s">
+        <v>185</v>
+      </c>
+      <c r="C52" t="s">
         <v>186</v>
       </c>
-      <c r="B52" t="s">
+      <c r="D52" t="s">
         <v>187</v>
       </c>
-      <c r="C52" t="s">
+      <c r="E52" t="s">
         <v>188</v>
-      </c>
-      <c r="D52" t="s">
-        <v>189</v>
-      </c>
-      <c r="E52" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B53" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C53" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D53" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E53" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B54" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C54" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D54" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="E54" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>326</v>
+      </c>
+      <c r="B55" t="s">
+        <v>327</v>
+      </c>
+      <c r="C55" t="s">
         <v>328</v>
       </c>
-      <c r="B55" t="s">
+      <c r="D55" t="s">
         <v>329</v>
       </c>
-      <c r="C55" t="s">
+      <c r="E55" t="s">
         <v>330</v>
-      </c>
-      <c r="D55" t="s">
-        <v>331</v>
-      </c>
-      <c r="E55" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>320</v>
+      </c>
+      <c r="B56" t="s">
+        <v>321</v>
+      </c>
+      <c r="C56" t="s">
         <v>322</v>
       </c>
-      <c r="B56" t="s">
+      <c r="D56" t="s">
+        <v>321</v>
+      </c>
+      <c r="E56" t="s">
         <v>323</v>
-      </c>
-      <c r="C56" t="s">
-        <v>324</v>
-      </c>
-      <c r="D56" t="s">
-        <v>323</v>
-      </c>
-      <c r="E56" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>189</v>
+      </c>
+      <c r="B57" t="s">
+        <v>190</v>
+      </c>
+      <c r="C57" t="s">
         <v>191</v>
       </c>
-      <c r="B57" t="s">
+      <c r="D57" t="s">
         <v>192</v>
       </c>
-      <c r="C57" t="s">
+      <c r="E57" t="s">
         <v>193</v>
-      </c>
-      <c r="D57" t="s">
-        <v>194</v>
-      </c>
-      <c r="E57" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>375</v>
+      </c>
+      <c r="B58" t="s">
         <v>377</v>
       </c>
-      <c r="B58" t="s">
+      <c r="C58" t="s">
         <v>379</v>
       </c>
-      <c r="C58" t="s">
+      <c r="D58" t="s">
         <v>381</v>
       </c>
-      <c r="D58" t="s">
+      <c r="E58" t="s">
         <v>383</v>
-      </c>
-      <c r="E58" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>331</v>
+      </c>
+      <c r="B59" t="s">
+        <v>332</v>
+      </c>
+      <c r="C59" t="s">
         <v>333</v>
       </c>
-      <c r="B59" t="s">
+      <c r="D59" t="s">
         <v>334</v>
       </c>
-      <c r="C59" t="s">
+      <c r="E59" t="s">
         <v>335</v>
-      </c>
-      <c r="D59" t="s">
-        <v>336</v>
-      </c>
-      <c r="E59" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>194</v>
+      </c>
+      <c r="B60" t="s">
+        <v>195</v>
+      </c>
+      <c r="C60" t="s">
+        <v>195</v>
+      </c>
+      <c r="D60" t="s">
         <v>196</v>
       </c>
-      <c r="B60" t="s">
+      <c r="E60" t="s">
         <v>197</v>
-      </c>
-      <c r="C60" t="s">
-        <v>197</v>
-      </c>
-      <c r="D60" t="s">
-        <v>198</v>
-      </c>
-      <c r="E60" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B61" t="s">
+        <v>394</v>
+      </c>
+      <c r="C61" t="s">
+        <v>395</v>
+      </c>
+      <c r="D61" t="s">
         <v>396</v>
       </c>
-      <c r="C61" t="s">
-        <v>397</v>
-      </c>
-      <c r="D61" t="s">
-        <v>398</v>
-      </c>
       <c r="E61" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B62" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="C62" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="D62" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="E62" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>199</v>
+      </c>
+      <c r="B63" t="s">
+        <v>200</v>
+      </c>
+      <c r="C63" t="s">
         <v>201</v>
       </c>
-      <c r="B63" t="s">
+      <c r="D63" t="s">
         <v>202</v>
       </c>
-      <c r="C63" t="s">
-        <v>203</v>
-      </c>
-      <c r="D63" t="s">
-        <v>204</v>
-      </c>
       <c r="E63" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>203</v>
+      </c>
+      <c r="B64" t="s">
+        <v>204</v>
+      </c>
+      <c r="C64" t="s">
         <v>205</v>
       </c>
-      <c r="B64" t="s">
+      <c r="D64" t="s">
         <v>206</v>
       </c>
-      <c r="C64" t="s">
+      <c r="E64" t="s">
         <v>207</v>
-      </c>
-      <c r="D64" t="s">
-        <v>208</v>
-      </c>
-      <c r="E64" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>208</v>
+      </c>
+      <c r="B65" t="s">
+        <v>209</v>
+      </c>
+      <c r="C65" t="s">
         <v>210</v>
       </c>
-      <c r="B65" t="s">
+      <c r="D65" t="s">
         <v>211</v>
       </c>
-      <c r="C65" t="s">
+      <c r="E65" t="s">
         <v>212</v>
-      </c>
-      <c r="D65" t="s">
-        <v>213</v>
-      </c>
-      <c r="E65" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>213</v>
+      </c>
+      <c r="B66" t="s">
+        <v>214</v>
+      </c>
+      <c r="C66" t="s">
         <v>215</v>
       </c>
-      <c r="B66" t="s">
+      <c r="D66" t="s">
         <v>216</v>
       </c>
-      <c r="C66" t="s">
+      <c r="E66" t="s">
         <v>217</v>
-      </c>
-      <c r="D66" t="s">
-        <v>218</v>
-      </c>
-      <c r="E66" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>218</v>
+      </c>
+      <c r="B67" t="s">
+        <v>219</v>
+      </c>
+      <c r="C67" t="s">
         <v>220</v>
       </c>
-      <c r="B67" t="s">
+      <c r="D67" t="s">
         <v>221</v>
       </c>
-      <c r="C67" t="s">
+      <c r="E67" t="s">
         <v>222</v>
-      </c>
-      <c r="D67" t="s">
-        <v>223</v>
-      </c>
-      <c r="E67" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>223</v>
+      </c>
+      <c r="B68" t="s">
+        <v>224</v>
+      </c>
+      <c r="C68" t="s">
+        <v>398</v>
+      </c>
+      <c r="D68" t="s">
         <v>225</v>
       </c>
-      <c r="B68" t="s">
-        <v>226</v>
-      </c>
-      <c r="C68" t="s">
-        <v>400</v>
-      </c>
-      <c r="D68" t="s">
-        <v>227</v>
-      </c>
       <c r="E68" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>226</v>
+      </c>
+      <c r="B69" t="s">
+        <v>227</v>
+      </c>
+      <c r="C69" t="s">
         <v>228</v>
       </c>
-      <c r="B69" t="s">
+      <c r="D69" t="s">
         <v>229</v>
       </c>
-      <c r="C69" t="s">
+      <c r="E69" t="s">
         <v>230</v>
-      </c>
-      <c r="D69" t="s">
-        <v>231</v>
-      </c>
-      <c r="E69" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>231</v>
+      </c>
+      <c r="B70" t="s">
+        <v>232</v>
+      </c>
+      <c r="C70" t="s">
         <v>233</v>
       </c>
-      <c r="B70" t="s">
+      <c r="D70" t="s">
         <v>234</v>
       </c>
-      <c r="C70" t="s">
+      <c r="E70" t="s">
         <v>235</v>
-      </c>
-      <c r="D70" t="s">
-        <v>236</v>
-      </c>
-      <c r="E70" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>468</v>
+      </c>
+      <c r="B71" t="s">
+        <v>469</v>
+      </c>
+      <c r="C71" t="s">
         <v>470</v>
       </c>
-      <c r="B71" t="s">
+      <c r="D71" t="s">
         <v>471</v>
       </c>
-      <c r="C71" t="s">
+      <c r="E71" t="s">
         <v>472</v>
-      </c>
-      <c r="D71" t="s">
-        <v>473</v>
-      </c>
-      <c r="E71" t="s">
-        <v>474</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>236</v>
+      </c>
+      <c r="B72" t="s">
+        <v>237</v>
+      </c>
+      <c r="C72" t="s">
         <v>238</v>
       </c>
-      <c r="B72" t="s">
+      <c r="D72" t="s">
         <v>239</v>
       </c>
-      <c r="C72" t="s">
+      <c r="E72" t="s">
         <v>240</v>
-      </c>
-      <c r="D72" t="s">
-        <v>241</v>
-      </c>
-      <c r="E72" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>340</v>
+      </c>
+      <c r="B73" t="s">
+        <v>341</v>
+      </c>
+      <c r="C73" t="s">
+        <v>341</v>
+      </c>
+      <c r="D73" t="s">
+        <v>341</v>
+      </c>
+      <c r="E73" t="s">
         <v>342</v>
-      </c>
-      <c r="B73" t="s">
-        <v>343</v>
-      </c>
-      <c r="C73" t="s">
-        <v>343</v>
-      </c>
-      <c r="D73" t="s">
-        <v>343</v>
-      </c>
-      <c r="E73" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B74" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C74" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D74" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E74" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B75" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C75" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D75" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="E75" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B76" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C76" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D76" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="E76" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B77" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C77" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D77" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="E77" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B78" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C78" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D78" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="E78" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B79" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C79" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D79" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="E79" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B80" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C80" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D80" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="E80" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B81" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C81" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D81" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="E81" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>241</v>
+      </c>
+      <c r="B82" t="s">
+        <v>242</v>
+      </c>
+      <c r="C82" t="s">
         <v>243</v>
       </c>
-      <c r="B82" t="s">
+      <c r="D82" t="s">
         <v>244</v>
       </c>
-      <c r="C82" t="s">
+      <c r="E82" t="s">
         <v>245</v>
-      </c>
-      <c r="D82" t="s">
-        <v>246</v>
-      </c>
-      <c r="E82" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
+        <v>246</v>
+      </c>
+      <c r="B83" t="s">
+        <v>247</v>
+      </c>
+      <c r="C83" t="s">
         <v>248</v>
       </c>
-      <c r="B83" t="s">
-        <v>249</v>
-      </c>
-      <c r="C83" t="s">
-        <v>250</v>
-      </c>
       <c r="D83" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E83" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
+        <v>249</v>
+      </c>
+      <c r="B84" t="s">
+        <v>250</v>
+      </c>
+      <c r="C84" t="s">
         <v>251</v>
       </c>
-      <c r="B84" t="s">
-        <v>252</v>
-      </c>
-      <c r="C84" t="s">
-        <v>253</v>
-      </c>
       <c r="D84" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E84" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
+        <v>252</v>
+      </c>
+      <c r="B85" t="s">
+        <v>253</v>
+      </c>
+      <c r="C85" t="s">
         <v>254</v>
       </c>
-      <c r="B85" t="s">
+      <c r="D85" t="s">
         <v>255</v>
       </c>
-      <c r="C85" t="s">
-        <v>256</v>
-      </c>
-      <c r="D85" t="s">
-        <v>257</v>
-      </c>
       <c r="E85" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
+        <v>256</v>
+      </c>
+      <c r="B86" t="s">
+        <v>257</v>
+      </c>
+      <c r="C86" t="s">
         <v>258</v>
       </c>
-      <c r="B86" t="s">
+      <c r="D86" t="s">
         <v>259</v>
       </c>
-      <c r="C86" t="s">
+      <c r="E86" t="s">
         <v>260</v>
-      </c>
-      <c r="D86" t="s">
-        <v>261</v>
-      </c>
-      <c r="E86" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
+        <v>261</v>
+      </c>
+      <c r="B87" t="s">
+        <v>262</v>
+      </c>
+      <c r="C87" t="s">
         <v>263</v>
       </c>
-      <c r="B87" t="s">
+      <c r="D87" t="s">
         <v>264</v>
       </c>
-      <c r="C87" t="s">
+      <c r="E87" t="s">
         <v>265</v>
-      </c>
-      <c r="D87" t="s">
-        <v>266</v>
-      </c>
-      <c r="E87" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
+        <v>266</v>
+      </c>
+      <c r="B88" t="s">
+        <v>267</v>
+      </c>
+      <c r="C88" t="s">
         <v>268</v>
       </c>
-      <c r="B88" t="s">
+      <c r="D88" t="s">
         <v>269</v>
       </c>
-      <c r="C88" t="s">
+      <c r="E88" t="s">
         <v>270</v>
-      </c>
-      <c r="D88" t="s">
-        <v>271</v>
-      </c>
-      <c r="E88" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
+        <v>443</v>
+      </c>
+      <c r="B89" t="s">
+        <v>444</v>
+      </c>
+      <c r="C89" t="s">
         <v>445</v>
       </c>
-      <c r="B89" t="s">
+      <c r="D89" t="s">
         <v>446</v>
       </c>
-      <c r="C89" t="s">
+      <c r="E89" t="s">
         <v>447</v>
-      </c>
-      <c r="D89" t="s">
-        <v>448</v>
-      </c>
-      <c r="E89" t="s">
-        <v>449</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
+        <v>271</v>
+      </c>
+      <c r="B90" t="s">
+        <v>272</v>
+      </c>
+      <c r="C90" t="s">
         <v>273</v>
       </c>
-      <c r="B90" t="s">
+      <c r="D90" t="s">
         <v>274</v>
       </c>
-      <c r="C90" t="s">
-        <v>275</v>
-      </c>
-      <c r="D90" t="s">
-        <v>276</v>
-      </c>
       <c r="E90" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
+        <v>371</v>
+      </c>
+      <c r="B91" t="s">
+        <v>372</v>
+      </c>
+      <c r="C91" t="s">
         <v>373</v>
       </c>
-      <c r="B91" t="s">
-        <v>374</v>
-      </c>
-      <c r="C91" t="s">
-        <v>375</v>
-      </c>
       <c r="D91" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="E91" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
+        <v>438</v>
+      </c>
+      <c r="B92" t="s">
+        <v>439</v>
+      </c>
+      <c r="C92" t="s">
         <v>440</v>
       </c>
-      <c r="B92" t="s">
+      <c r="D92" t="s">
         <v>441</v>
       </c>
-      <c r="C92" t="s">
+      <c r="E92" t="s">
         <v>442</v>
-      </c>
-      <c r="D92" t="s">
-        <v>443</v>
-      </c>
-      <c r="E92" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
+        <v>275</v>
+      </c>
+      <c r="B93" t="s">
+        <v>276</v>
+      </c>
+      <c r="C93" t="s">
         <v>277</v>
       </c>
-      <c r="B93" t="s">
+      <c r="D93" t="s">
         <v>278</v>
       </c>
-      <c r="C93" t="s">
-        <v>279</v>
-      </c>
-      <c r="D93" t="s">
-        <v>280</v>
-      </c>
       <c r="E93" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
+        <v>279</v>
+      </c>
+      <c r="B94" t="s">
+        <v>280</v>
+      </c>
+      <c r="C94" t="s">
         <v>281</v>
       </c>
-      <c r="B94" t="s">
+      <c r="D94" t="s">
         <v>282</v>
       </c>
-      <c r="C94" t="s">
-        <v>283</v>
-      </c>
-      <c r="D94" t="s">
-        <v>284</v>
-      </c>
       <c r="E94" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
+        <v>419</v>
+      </c>
+      <c r="B95" t="s">
+        <v>420</v>
+      </c>
+      <c r="C95" t="s">
         <v>421</v>
       </c>
-      <c r="B95" t="s">
+      <c r="D95" t="s">
         <v>422</v>
       </c>
-      <c r="C95" t="s">
-        <v>423</v>
-      </c>
-      <c r="D95" t="s">
-        <v>424</v>
-      </c>
       <c r="E95" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B96" t="s">
+        <v>415</v>
+      </c>
+      <c r="C96" t="s">
+        <v>416</v>
+      </c>
+      <c r="D96" t="s">
         <v>417</v>
       </c>
-      <c r="C96" t="s">
+      <c r="E96" t="s">
         <v>418</v>
-      </c>
-      <c r="D96" t="s">
-        <v>419</v>
-      </c>
-      <c r="E96" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B97" t="s">
+        <v>412</v>
+      </c>
+      <c r="C97" t="s">
+        <v>413</v>
+      </c>
+      <c r="D97" t="s">
         <v>414</v>
       </c>
-      <c r="C97" t="s">
-        <v>415</v>
-      </c>
-      <c r="D97" t="s">
-        <v>416</v>
-      </c>
       <c r="E97" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
+        <v>408</v>
+      </c>
+      <c r="B98" t="s">
+        <v>407</v>
+      </c>
+      <c r="C98" t="s">
+        <v>409</v>
+      </c>
+      <c r="D98" t="s">
         <v>410</v>
       </c>
-      <c r="B98" t="s">
-        <v>409</v>
-      </c>
-      <c r="C98" t="s">
+      <c r="E98" t="s">
         <v>411</v>
-      </c>
-      <c r="D98" t="s">
-        <v>412</v>
-      </c>
-      <c r="E98" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
+        <v>283</v>
+      </c>
+      <c r="B99" t="s">
+        <v>284</v>
+      </c>
+      <c r="C99" t="s">
         <v>285</v>
       </c>
-      <c r="B99" t="s">
+      <c r="D99" t="s">
         <v>286</v>
       </c>
-      <c r="C99" t="s">
-        <v>287</v>
-      </c>
-      <c r="D99" t="s">
-        <v>288</v>
-      </c>
       <c r="E99" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
+        <v>287</v>
+      </c>
+      <c r="B100" t="s">
+        <v>288</v>
+      </c>
+      <c r="C100" t="s">
         <v>289</v>
       </c>
-      <c r="B100" t="s">
+      <c r="D100" t="s">
         <v>290</v>
       </c>
-      <c r="C100" t="s">
-        <v>291</v>
-      </c>
-      <c r="D100" t="s">
-        <v>292</v>
-      </c>
       <c r="E100" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
+        <v>291</v>
+      </c>
+      <c r="B101" t="s">
+        <v>292</v>
+      </c>
+      <c r="C101" t="s">
+        <v>399</v>
+      </c>
+      <c r="D101" t="s">
+        <v>431</v>
+      </c>
+      <c r="E101" t="s">
         <v>293</v>
-      </c>
-      <c r="B101" t="s">
-        <v>294</v>
-      </c>
-      <c r="C101" t="s">
-        <v>401</v>
-      </c>
-      <c r="D101" t="s">
-        <v>433</v>
-      </c>
-      <c r="E101" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
+        <v>294</v>
+      </c>
+      <c r="B102" t="s">
+        <v>295</v>
+      </c>
+      <c r="C102" t="s">
         <v>296</v>
       </c>
-      <c r="B102" t="s">
-        <v>297</v>
-      </c>
-      <c r="C102" t="s">
-        <v>298</v>
-      </c>
       <c r="D102" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E102" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
+        <v>297</v>
+      </c>
+      <c r="B103" t="s">
+        <v>298</v>
+      </c>
+      <c r="C103" t="s">
         <v>299</v>
       </c>
-      <c r="B103" t="s">
-        <v>300</v>
-      </c>
-      <c r="C103" t="s">
-        <v>301</v>
-      </c>
       <c r="D103" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E103" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
+        <v>300</v>
+      </c>
+      <c r="B104" t="s">
+        <v>301</v>
+      </c>
+      <c r="C104" t="s">
         <v>302</v>
       </c>
-      <c r="B104" t="s">
-        <v>303</v>
-      </c>
-      <c r="C104" t="s">
-        <v>304</v>
-      </c>
       <c r="D104" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E104" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
+        <v>303</v>
+      </c>
+      <c r="B105" t="s">
+        <v>304</v>
+      </c>
+      <c r="C105" t="s">
         <v>305</v>
       </c>
-      <c r="B105" t="s">
+      <c r="D105" t="s">
         <v>306</v>
       </c>
-      <c r="C105" t="s">
-        <v>307</v>
-      </c>
-      <c r="D105" t="s">
-        <v>308</v>
-      </c>
       <c r="E105" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
+        <v>307</v>
+      </c>
+      <c r="B106" t="s">
+        <v>308</v>
+      </c>
+      <c r="C106" t="s">
         <v>309</v>
       </c>
-      <c r="B106" t="s">
+      <c r="D106" t="s">
         <v>310</v>
       </c>
-      <c r="C106" t="s">
+      <c r="E106" t="s">
         <v>311</v>
-      </c>
-      <c r="D106" t="s">
-        <v>312</v>
-      </c>
-      <c r="E106" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
+        <v>312</v>
+      </c>
+      <c r="B107" t="s">
+        <v>313</v>
+      </c>
+      <c r="C107" t="s">
         <v>314</v>
       </c>
-      <c r="B107" t="s">
-        <v>315</v>
-      </c>
-      <c r="C107" t="s">
-        <v>316</v>
-      </c>
       <c r="D107" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E107" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
+        <v>315</v>
+      </c>
+      <c r="B108" t="s">
+        <v>316</v>
+      </c>
+      <c r="C108" t="s">
         <v>317</v>
       </c>
-      <c r="B108" t="s">
+      <c r="D108" t="s">
         <v>318</v>
       </c>
-      <c r="C108" t="s">
+      <c r="E108" t="s">
         <v>319</v>
-      </c>
-      <c r="D108" t="s">
-        <v>320</v>
-      </c>
-      <c r="E108" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
+        <v>448</v>
+      </c>
+      <c r="B109" t="s">
+        <v>454</v>
+      </c>
+      <c r="C109" t="s">
+        <v>451</v>
+      </c>
+      <c r="D109" t="s">
+        <v>449</v>
+      </c>
+      <c r="E109" t="s">
         <v>450</v>
-      </c>
-      <c r="B109" t="s">
-        <v>456</v>
-      </c>
-      <c r="C109" t="s">
-        <v>453</v>
-      </c>
-      <c r="D109" t="s">
-        <v>451</v>
-      </c>
-      <c r="E109" t="s">
-        <v>452</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B110" t="s">
+        <v>453</v>
+      </c>
+      <c r="C110" t="s">
         <v>455</v>
       </c>
-      <c r="C110" t="s">
+      <c r="D110" t="s">
+        <v>456</v>
+      </c>
+      <c r="E110" t="s">
         <v>457</v>
-      </c>
-      <c r="D110" t="s">
-        <v>458</v>
-      </c>
-      <c r="E110" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
+        <v>374</v>
+      </c>
+      <c r="B111" t="s">
         <v>376</v>
       </c>
-      <c r="B111" t="s">
+      <c r="C111" t="s">
         <v>378</v>
       </c>
-      <c r="C111" t="s">
+      <c r="D111" t="s">
         <v>380</v>
       </c>
-      <c r="D111" t="s">
+      <c r="E111" t="s">
         <v>382</v>
-      </c>
-      <c r="E111" t="s">
-        <v>384</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B43" r:id="rId1" xr:uid="{772ACA42-8DE4-4015-A5BA-E378BC1F9836}"/>
+    <hyperlink ref="C43:E43" r:id="rId2" display="https://github.com/NightDreamGames/Graded" xr:uid="{F6D4AF19-D559-447E-AF49-35B5F0BBE70D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added clarification for general system
</commit_message>
<xml_diff>
--- a/assets/Localizations.xlsx
+++ b/assets/Localizations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Graded\Graded - Flutter\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{131F181E-2020-4227-870D-B221B02A8E0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C4C0CC-CC56-479D-A4D6-BDE83F2709FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="string" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0">string!$A$1:$B$111</definedName>
+    <definedName name="ExternalData_1" localSheetId="0">string!$A$1:$B$113</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="483">
   <si>
     <t>keys</t>
   </si>
@@ -463,12 +463,6 @@
     <t>Général</t>
   </si>
   <si>
-    <t>Allgemein</t>
-  </si>
-  <si>
-    <t>Allgemeng</t>
-  </si>
-  <si>
     <t>github</t>
   </si>
   <si>
@@ -1448,6 +1442,36 @@
   </si>
   <si>
     <t>contact@nightdreamgames.com</t>
+  </si>
+  <si>
+    <t>general_note</t>
+  </si>
+  <si>
+    <t>The general system is currently being implemented and is not ready yet. In the meantime, you can select "Other school system" and enter your subjects manually.</t>
+  </si>
+  <si>
+    <t>Le système général est en cours d'implémentation et n'est pas encore prêt. En attendant, vous pouvez sélectionner "Autre système scolaire" et saisir vos matières manuellement.</t>
+  </si>
+  <si>
+    <t>Das generale System wird gerade implementiert und ist noch nicht fertig. In der Zwischenzeit können Sie "Anderes Schulsystem" wählen und Ihre Fächer manuell eingeben.</t>
+  </si>
+  <si>
+    <t>Den Système general gëtt grad implementéiert an ass nach net fäerdeg. An der Zwëschenzäit kënnt dir "Aneren Schoulsystem" wielen an är Fächer manuell aginn.</t>
+  </si>
+  <si>
+    <t>coming_soon</t>
+  </si>
+  <si>
+    <t>Coming soon</t>
+  </si>
+  <si>
+    <t>Demnächst verfügbar</t>
+  </si>
+  <si>
+    <t>Bientôt disponible</t>
+  </si>
+  <si>
+    <t>Deemnächst verfügbar</t>
   </si>
 </sst>
 </file>
@@ -1498,9 +1522,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1520,10 +1547,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="string" displayName="string" ref="A1:E111" totalsRowShown="0">
-  <autoFilter ref="A1:E111" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E111">
-    <sortCondition ref="A1:A111"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="string" displayName="string" ref="A1:E113" totalsRowShown="0">
+  <autoFilter ref="A1:E113" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E113">
+    <sortCondition ref="A1:A113"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="keys"/>
@@ -1824,10 +1851,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E111"/>
+  <dimension ref="A1:E113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="E113" sqref="E113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1878,16 +1905,16 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
+        <v>456</v>
+      </c>
+      <c r="C3" t="s">
+        <v>455</v>
+      </c>
+      <c r="D3" t="s">
+        <v>457</v>
+      </c>
+      <c r="E3" t="s">
         <v>458</v>
-      </c>
-      <c r="C3" t="s">
-        <v>457</v>
-      </c>
-      <c r="D3" t="s">
-        <v>459</v>
-      </c>
-      <c r="E3" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1963,16 +1990,16 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="C8" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="D8" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="E8" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1983,7 +2010,7 @@
         <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D9" t="s">
         <v>46</v>
@@ -2079,53 +2106,53 @@
     </row>
     <row r="15" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>459</v>
+      </c>
+      <c r="B15" t="s">
+        <v>460</v>
+      </c>
+      <c r="C15" t="s">
         <v>461</v>
       </c>
-      <c r="B15" t="s">
+      <c r="D15" t="s">
         <v>462</v>
       </c>
-      <c r="C15" t="s">
+      <c r="E15" t="s">
         <v>463</v>
-      </c>
-      <c r="D15" t="s">
-        <v>464</v>
-      </c>
-      <c r="E15" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>381</v>
+      </c>
+      <c r="B16" t="s">
         <v>383</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
+        <v>384</v>
+      </c>
+      <c r="D16" t="s">
+        <v>386</v>
+      </c>
+      <c r="E16" t="s">
         <v>385</v>
-      </c>
-      <c r="C16" t="s">
-        <v>386</v>
-      </c>
-      <c r="D16" t="s">
-        <v>388</v>
-      </c>
-      <c r="E16" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B17" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C17" t="s">
+        <v>387</v>
+      </c>
+      <c r="D17" t="s">
         <v>389</v>
       </c>
-      <c r="D17" t="s">
-        <v>391</v>
-      </c>
       <c r="E17" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2164,19 +2191,19 @@
     </row>
     <row r="20" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>333</v>
+      </c>
+      <c r="B20" t="s">
+        <v>334</v>
+      </c>
+      <c r="C20" t="s">
         <v>335</v>
       </c>
-      <c r="B20" t="s">
+      <c r="D20" t="s">
         <v>336</v>
       </c>
-      <c r="C20" t="s">
-        <v>337</v>
-      </c>
-      <c r="D20" t="s">
-        <v>338</v>
-      </c>
       <c r="E20" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2232,560 +2259,560 @@
     </row>
     <row r="24" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>82</v>
+        <v>478</v>
       </c>
       <c r="B24" t="s">
-        <v>83</v>
+        <v>479</v>
       </c>
       <c r="C24" t="s">
-        <v>84</v>
+        <v>481</v>
       </c>
       <c r="D24" t="s">
-        <v>85</v>
-      </c>
-      <c r="E24" t="s">
-        <v>86</v>
+        <v>480</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>482</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B25" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C25" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D25" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E25" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B26" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C26" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D26" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E26" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B27" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C27" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D27" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E27" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B28" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C28" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D28" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E28" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B29" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C29" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D29" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E29" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B30" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C30" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D30" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E30" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B31" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C31" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D31" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E31" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B32" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C32" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D32" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E32" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B33" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C33" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D33" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E33" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B34" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C34" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D34" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E34" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B35" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C35" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D35" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E35" t="s">
-        <v>400</v>
+        <v>133</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B36" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C36" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D36" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E36" t="s">
-        <v>142</v>
+        <v>398</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>18</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>474</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>474</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>474</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>474</v>
+        <v>138</v>
+      </c>
+      <c r="B37" t="s">
+        <v>139</v>
+      </c>
+      <c r="C37" t="s">
+        <v>140</v>
+      </c>
+      <c r="D37" t="s">
+        <v>141</v>
+      </c>
+      <c r="E37" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>10</v>
-      </c>
-      <c r="B38" t="s">
-        <v>11</v>
-      </c>
-      <c r="C38" t="s">
-        <v>11</v>
-      </c>
-      <c r="D38" t="s">
-        <v>11</v>
-      </c>
-      <c r="E38" t="s">
-        <v>11</v>
+        <v>18</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B39" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C39" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D39" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E39" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>143</v>
+        <v>14</v>
       </c>
       <c r="B40" t="s">
-        <v>144</v>
+        <v>15</v>
       </c>
       <c r="C40" t="s">
-        <v>145</v>
+        <v>15</v>
       </c>
       <c r="D40" t="s">
-        <v>146</v>
+        <v>15</v>
       </c>
       <c r="E40" t="s">
-        <v>147</v>
+        <v>15</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>12</v>
+        <v>143</v>
       </c>
       <c r="B41" t="s">
-        <v>13</v>
+        <v>144</v>
       </c>
       <c r="C41" t="s">
-        <v>13</v>
+        <v>145</v>
       </c>
       <c r="D41" t="s">
-        <v>13</v>
+        <v>144</v>
       </c>
       <c r="E41" t="s">
-        <v>13</v>
+        <v>144</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>148</v>
+        <v>473</v>
       </c>
       <c r="B42" t="s">
-        <v>149</v>
+        <v>474</v>
       </c>
       <c r="C42" t="s">
-        <v>150</v>
+        <v>475</v>
       </c>
       <c r="D42" t="s">
-        <v>151</v>
-      </c>
-      <c r="E42" t="s">
-        <v>151</v>
+        <v>476</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>477</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>9</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>473</v>
+        <v>12</v>
+      </c>
+      <c r="B43" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43" t="s">
+        <v>13</v>
+      </c>
+      <c r="D43" t="s">
+        <v>13</v>
+      </c>
+      <c r="E43" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B44" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C44" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="D44" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="E44" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>156</v>
-      </c>
-      <c r="B45" t="s">
-        <v>157</v>
-      </c>
-      <c r="C45" t="s">
-        <v>158</v>
-      </c>
-      <c r="D45" t="s">
-        <v>159</v>
-      </c>
-      <c r="E45" t="s">
-        <v>160</v>
+        <v>9</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>471</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="B46" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="C46" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="D46" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="E46" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="B47" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="C47" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="D47" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="E47" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>432</v>
+        <v>159</v>
       </c>
       <c r="B48" t="s">
-        <v>431</v>
+        <v>160</v>
       </c>
       <c r="C48" t="s">
-        <v>433</v>
+        <v>161</v>
       </c>
       <c r="D48" t="s">
-        <v>434</v>
+        <v>162</v>
       </c>
       <c r="E48" t="s">
-        <v>435</v>
+        <v>163</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B49" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="C49" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D49" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="E49" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>176</v>
+        <v>430</v>
       </c>
       <c r="B50" t="s">
-        <v>177</v>
+        <v>429</v>
       </c>
       <c r="C50" t="s">
-        <v>177</v>
+        <v>431</v>
       </c>
       <c r="D50" t="s">
-        <v>178</v>
+        <v>432</v>
       </c>
       <c r="E50" t="s">
-        <v>179</v>
+        <v>433</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="B51" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="C51" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="D51" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="E51" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="B52" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="C52" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="D52" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="E52" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>16</v>
+        <v>178</v>
       </c>
       <c r="B53" t="s">
-        <v>17</v>
+        <v>179</v>
       </c>
       <c r="C53" t="s">
-        <v>17</v>
+        <v>179</v>
       </c>
       <c r="D53" t="s">
-        <v>17</v>
+        <v>180</v>
       </c>
       <c r="E53" t="s">
-        <v>17</v>
+        <v>180</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>323</v>
+        <v>181</v>
       </c>
       <c r="B54" t="s">
-        <v>324</v>
+        <v>182</v>
       </c>
       <c r="C54" t="s">
-        <v>324</v>
+        <v>183</v>
       </c>
       <c r="D54" t="s">
-        <v>324</v>
+        <v>184</v>
       </c>
       <c r="E54" t="s">
-        <v>324</v>
+        <v>185</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>325</v>
+        <v>16</v>
       </c>
       <c r="B55" t="s">
-        <v>326</v>
+        <v>17</v>
       </c>
       <c r="C55" t="s">
-        <v>327</v>
+        <v>17</v>
       </c>
       <c r="D55" t="s">
-        <v>328</v>
+        <v>17</v>
       </c>
       <c r="E55" t="s">
-        <v>329</v>
+        <v>17</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="B56" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="C56" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D56" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="E56" t="s">
         <v>322</v>
@@ -2793,946 +2820,980 @@
     </row>
     <row r="57" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>188</v>
+        <v>323</v>
       </c>
       <c r="B57" t="s">
-        <v>189</v>
+        <v>324</v>
       </c>
       <c r="C57" t="s">
-        <v>190</v>
+        <v>325</v>
       </c>
       <c r="D57" t="s">
-        <v>191</v>
+        <v>326</v>
       </c>
       <c r="E57" t="s">
-        <v>192</v>
+        <v>327</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>374</v>
+        <v>317</v>
       </c>
       <c r="B58" t="s">
-        <v>376</v>
+        <v>318</v>
       </c>
       <c r="C58" t="s">
-        <v>378</v>
+        <v>319</v>
       </c>
       <c r="D58" t="s">
-        <v>380</v>
+        <v>318</v>
       </c>
       <c r="E58" t="s">
-        <v>382</v>
+        <v>320</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>330</v>
+        <v>186</v>
       </c>
       <c r="B59" t="s">
-        <v>331</v>
+        <v>187</v>
       </c>
       <c r="C59" t="s">
-        <v>332</v>
+        <v>188</v>
       </c>
       <c r="D59" t="s">
-        <v>333</v>
+        <v>189</v>
       </c>
       <c r="E59" t="s">
-        <v>334</v>
+        <v>190</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>193</v>
+        <v>372</v>
       </c>
       <c r="B60" t="s">
-        <v>194</v>
+        <v>374</v>
       </c>
       <c r="C60" t="s">
-        <v>194</v>
+        <v>376</v>
       </c>
       <c r="D60" t="s">
-        <v>195</v>
+        <v>378</v>
       </c>
       <c r="E60" t="s">
-        <v>196</v>
+        <v>380</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>197</v>
+        <v>328</v>
       </c>
       <c r="B61" t="s">
-        <v>393</v>
+        <v>329</v>
       </c>
       <c r="C61" t="s">
-        <v>394</v>
+        <v>330</v>
       </c>
       <c r="D61" t="s">
-        <v>395</v>
+        <v>331</v>
       </c>
       <c r="E61" t="s">
-        <v>402</v>
+        <v>332</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>392</v>
+        <v>191</v>
       </c>
       <c r="B62" t="s">
-        <v>466</v>
+        <v>192</v>
       </c>
       <c r="C62" t="s">
-        <v>466</v>
+        <v>192</v>
       </c>
       <c r="D62" t="s">
-        <v>466</v>
+        <v>193</v>
       </c>
       <c r="E62" t="s">
-        <v>466</v>
+        <v>194</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B63" t="s">
-        <v>199</v>
+        <v>391</v>
       </c>
       <c r="C63" t="s">
-        <v>200</v>
+        <v>392</v>
       </c>
       <c r="D63" t="s">
-        <v>201</v>
+        <v>393</v>
       </c>
       <c r="E63" t="s">
-        <v>201</v>
+        <v>400</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>202</v>
+        <v>390</v>
       </c>
       <c r="B64" t="s">
-        <v>203</v>
+        <v>464</v>
       </c>
       <c r="C64" t="s">
-        <v>204</v>
+        <v>464</v>
       </c>
       <c r="D64" t="s">
-        <v>205</v>
+        <v>464</v>
       </c>
       <c r="E64" t="s">
-        <v>206</v>
+        <v>464</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="B65" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="C65" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="D65" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="E65" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="B66" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="C66" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="D66" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="E66" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="B67" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="C67" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="D67" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="E67" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="B68" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="C68" t="s">
-        <v>397</v>
+        <v>212</v>
       </c>
       <c r="D68" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="E68" t="s">
-        <v>403</v>
+        <v>214</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="B69" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="C69" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="D69" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="E69" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="B70" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="C70" t="s">
-        <v>232</v>
+        <v>395</v>
       </c>
       <c r="D70" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="E70" t="s">
-        <v>234</v>
+        <v>401</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>467</v>
+        <v>223</v>
       </c>
       <c r="B71" t="s">
-        <v>468</v>
+        <v>224</v>
       </c>
       <c r="C71" t="s">
-        <v>469</v>
+        <v>225</v>
       </c>
       <c r="D71" t="s">
-        <v>470</v>
+        <v>226</v>
       </c>
       <c r="E71" t="s">
-        <v>471</v>
+        <v>227</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="B72" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="C72" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="D72" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="E72" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>339</v>
+        <v>465</v>
       </c>
       <c r="B73" t="s">
-        <v>340</v>
+        <v>466</v>
       </c>
       <c r="C73" t="s">
-        <v>340</v>
+        <v>467</v>
       </c>
       <c r="D73" t="s">
-        <v>340</v>
+        <v>468</v>
       </c>
       <c r="E73" t="s">
-        <v>341</v>
+        <v>469</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>422</v>
+        <v>233</v>
       </c>
       <c r="B74" t="s">
-        <v>342</v>
+        <v>234</v>
       </c>
       <c r="C74" t="s">
-        <v>349</v>
+        <v>235</v>
       </c>
       <c r="D74" t="s">
-        <v>357</v>
+        <v>236</v>
       </c>
       <c r="E74" t="s">
-        <v>366</v>
+        <v>237</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>424</v>
+        <v>337</v>
       </c>
       <c r="B75" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="C75" t="s">
-        <v>350</v>
+        <v>338</v>
       </c>
       <c r="D75" t="s">
-        <v>358</v>
+        <v>338</v>
       </c>
       <c r="E75" t="s">
-        <v>358</v>
+        <v>339</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="B76" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="C76" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="D76" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="E76" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="B77" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="C77" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="D77" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="E77" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="B78" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="C78" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="D78" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E78" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="B79" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C79" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="D79" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="E79" t="s">
-        <v>368</v>
+        <v>359</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="B80" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="C80" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="D80" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="E80" t="s">
-        <v>401</v>
+        <v>365</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="B81" t="s">
-        <v>436</v>
+        <v>343</v>
       </c>
       <c r="C81" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="D81" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="E81" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>240</v>
+        <v>426</v>
       </c>
       <c r="B82" t="s">
-        <v>241</v>
+        <v>345</v>
       </c>
       <c r="C82" t="s">
-        <v>242</v>
+        <v>353</v>
       </c>
       <c r="D82" t="s">
-        <v>243</v>
+        <v>361</v>
       </c>
       <c r="E82" t="s">
-        <v>244</v>
+        <v>399</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>245</v>
+        <v>427</v>
       </c>
       <c r="B83" t="s">
-        <v>246</v>
+        <v>434</v>
       </c>
       <c r="C83" t="s">
-        <v>247</v>
+        <v>354</v>
       </c>
       <c r="D83" t="s">
-        <v>246</v>
+        <v>362</v>
       </c>
       <c r="E83" t="s">
-        <v>246</v>
+        <v>367</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="B84" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="C84" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="D84" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="E84" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="B85" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="C85" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="D85" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="E85" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="B86" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="C86" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="D86" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
       <c r="E86" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
       <c r="B87" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
       <c r="C87" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="D87" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="E87" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
       <c r="B88" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="C88" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="D88" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="E88" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>442</v>
+        <v>258</v>
       </c>
       <c r="B89" t="s">
-        <v>443</v>
+        <v>259</v>
       </c>
       <c r="C89" t="s">
-        <v>444</v>
+        <v>260</v>
       </c>
       <c r="D89" t="s">
-        <v>445</v>
+        <v>261</v>
       </c>
       <c r="E89" t="s">
-        <v>446</v>
+        <v>262</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="B90" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="C90" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="D90" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="E90" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>370</v>
+        <v>440</v>
       </c>
       <c r="B91" t="s">
-        <v>371</v>
+        <v>441</v>
       </c>
       <c r="C91" t="s">
-        <v>372</v>
+        <v>442</v>
       </c>
       <c r="D91" t="s">
-        <v>371</v>
+        <v>443</v>
       </c>
       <c r="E91" t="s">
-        <v>371</v>
+        <v>444</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>437</v>
+        <v>268</v>
       </c>
       <c r="B92" t="s">
-        <v>438</v>
+        <v>269</v>
       </c>
       <c r="C92" t="s">
-        <v>439</v>
+        <v>270</v>
       </c>
       <c r="D92" t="s">
-        <v>440</v>
+        <v>271</v>
       </c>
       <c r="E92" t="s">
-        <v>441</v>
+        <v>271</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>274</v>
+        <v>368</v>
       </c>
       <c r="B93" t="s">
-        <v>275</v>
+        <v>369</v>
       </c>
       <c r="C93" t="s">
-        <v>276</v>
+        <v>370</v>
       </c>
       <c r="D93" t="s">
-        <v>277</v>
+        <v>369</v>
       </c>
       <c r="E93" t="s">
-        <v>277</v>
+        <v>369</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>278</v>
+        <v>435</v>
       </c>
       <c r="B94" t="s">
-        <v>279</v>
+        <v>436</v>
       </c>
       <c r="C94" t="s">
-        <v>280</v>
+        <v>437</v>
       </c>
       <c r="D94" t="s">
-        <v>281</v>
+        <v>438</v>
       </c>
       <c r="E94" t="s">
-        <v>281</v>
+        <v>439</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>418</v>
+        <v>272</v>
       </c>
       <c r="B95" t="s">
-        <v>419</v>
+        <v>273</v>
       </c>
       <c r="C95" t="s">
-        <v>420</v>
+        <v>274</v>
       </c>
       <c r="D95" t="s">
-        <v>421</v>
+        <v>275</v>
       </c>
       <c r="E95" t="s">
-        <v>421</v>
+        <v>275</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>405</v>
+        <v>276</v>
       </c>
       <c r="B96" t="s">
-        <v>414</v>
+        <v>277</v>
       </c>
       <c r="C96" t="s">
-        <v>415</v>
+        <v>278</v>
       </c>
       <c r="D96" t="s">
-        <v>416</v>
+        <v>279</v>
       </c>
       <c r="E96" t="s">
-        <v>417</v>
+        <v>279</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>404</v>
+        <v>416</v>
       </c>
       <c r="B97" t="s">
-        <v>411</v>
+        <v>417</v>
       </c>
       <c r="C97" t="s">
-        <v>412</v>
+        <v>418</v>
       </c>
       <c r="D97" t="s">
-        <v>413</v>
+        <v>419</v>
       </c>
       <c r="E97" t="s">
-        <v>413</v>
+        <v>419</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="B98" t="s">
-        <v>406</v>
+        <v>412</v>
       </c>
       <c r="C98" t="s">
-        <v>408</v>
+        <v>413</v>
       </c>
       <c r="D98" t="s">
-        <v>409</v>
+        <v>414</v>
       </c>
       <c r="E98" t="s">
-        <v>410</v>
+        <v>415</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>282</v>
+        <v>402</v>
       </c>
       <c r="B99" t="s">
-        <v>283</v>
+        <v>409</v>
       </c>
       <c r="C99" t="s">
-        <v>284</v>
+        <v>410</v>
       </c>
       <c r="D99" t="s">
-        <v>285</v>
+        <v>411</v>
       </c>
       <c r="E99" t="s">
-        <v>285</v>
+        <v>411</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>286</v>
+        <v>405</v>
       </c>
       <c r="B100" t="s">
-        <v>287</v>
+        <v>404</v>
       </c>
       <c r="C100" t="s">
-        <v>288</v>
+        <v>406</v>
       </c>
       <c r="D100" t="s">
-        <v>289</v>
+        <v>407</v>
       </c>
       <c r="E100" t="s">
-        <v>289</v>
+        <v>408</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="B101" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="C101" t="s">
-        <v>398</v>
+        <v>282</v>
       </c>
       <c r="D101" t="s">
-        <v>430</v>
+        <v>283</v>
       </c>
       <c r="E101" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="B102" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="C102" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="D102" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="E102" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="B103" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="C103" t="s">
-        <v>298</v>
+        <v>396</v>
       </c>
       <c r="D103" t="s">
-        <v>297</v>
+        <v>428</v>
       </c>
       <c r="E103" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="B104" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="C104" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="D104" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="E104" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="B105" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="C105" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="D105" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="E105" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="B106" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="C106" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="D106" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
       <c r="E106" t="s">
-        <v>310</v>
+        <v>298</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
       <c r="B107" t="s">
-        <v>312</v>
+        <v>301</v>
       </c>
       <c r="C107" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
       <c r="D107" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
       <c r="E107" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="B108" t="s">
-        <v>315</v>
+        <v>305</v>
       </c>
       <c r="C108" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="D108" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
       <c r="E108" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>447</v>
+        <v>309</v>
       </c>
       <c r="B109" t="s">
-        <v>453</v>
+        <v>310</v>
       </c>
       <c r="C109" t="s">
-        <v>450</v>
+        <v>311</v>
       </c>
       <c r="D109" t="s">
-        <v>448</v>
+        <v>311</v>
       </c>
       <c r="E109" t="s">
-        <v>449</v>
+        <v>311</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>451</v>
+        <v>312</v>
       </c>
       <c r="B110" t="s">
-        <v>452</v>
+        <v>313</v>
       </c>
       <c r="C110" t="s">
-        <v>454</v>
+        <v>314</v>
       </c>
       <c r="D110" t="s">
-        <v>455</v>
+        <v>315</v>
       </c>
       <c r="E110" t="s">
-        <v>456</v>
+        <v>316</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
+        <v>445</v>
+      </c>
+      <c r="B111" t="s">
+        <v>451</v>
+      </c>
+      <c r="C111" t="s">
+        <v>448</v>
+      </c>
+      <c r="D111" t="s">
+        <v>446</v>
+      </c>
+      <c r="E111" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>449</v>
+      </c>
+      <c r="B112" t="s">
+        <v>450</v>
+      </c>
+      <c r="C112" t="s">
+        <v>452</v>
+      </c>
+      <c r="D112" t="s">
+        <v>453</v>
+      </c>
+      <c r="E112" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>371</v>
+      </c>
+      <c r="B113" t="s">
         <v>373</v>
       </c>
-      <c r="B111" t="s">
+      <c r="C113" t="s">
         <v>375</v>
       </c>
-      <c r="C111" t="s">
+      <c r="D113" t="s">
         <v>377</v>
       </c>
-      <c r="D111" t="s">
+      <c r="E113" t="s">
         <v>379</v>
-      </c>
-      <c r="E111" t="s">
-        <v>381</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B43" r:id="rId1" xr:uid="{772ACA42-8DE4-4015-A5BA-E378BC1F9836}"/>
-    <hyperlink ref="C43:E43" r:id="rId2" display="https://github.com/NightDreamGames/Graded" xr:uid="{F6D4AF19-D559-447E-AF49-35B5F0BBE70D}"/>
-    <hyperlink ref="B37" r:id="rId3" xr:uid="{7E3A0FC6-064A-4102-B40F-1969830D4899}"/>
-    <hyperlink ref="C37:E37" r:id="rId4" display="contact@nightdreamgames.com" xr:uid="{49649B53-773A-4287-9E32-3113566F351E}"/>
+    <hyperlink ref="B45" r:id="rId1" xr:uid="{772ACA42-8DE4-4015-A5BA-E378BC1F9836}"/>
+    <hyperlink ref="C45:E45" r:id="rId2" display="https://github.com/NightDreamGames/Graded" xr:uid="{F6D4AF19-D559-447E-AF49-35B5F0BBE70D}"/>
+    <hyperlink ref="B38" r:id="rId3" xr:uid="{7E3A0FC6-064A-4102-B40F-1969830D4899}"/>
+    <hyperlink ref="C38:E38" r:id="rId4" display="contact@nightdreamgames.com" xr:uid="{49649B53-773A-4287-9E32-3113566F351E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>

</xml_diff>

<commit_message>
Refuse non unique subject names
</commit_message>
<xml_diff>
--- a/assets/Localizations.xlsx
+++ b/assets/Localizations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Graded\Graded - Flutter\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C4C0CC-CC56-479D-A4D6-BDE83F2709FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1A1A994-DF79-4E3D-B7BA-650E93148707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="string" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0">string!$A$1:$B$113</definedName>
+    <definedName name="ExternalData_1" localSheetId="0">string!$A$1:$B$114</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="488">
   <si>
     <t>keys</t>
   </si>
@@ -1472,6 +1472,21 @@
   </si>
   <si>
     <t>Deemnächst verfügbar</t>
+  </si>
+  <si>
+    <t>enter_unique</t>
+  </si>
+  <si>
+    <t>Enter a unique name</t>
+  </si>
+  <si>
+    <t>Entrez un nom unique</t>
+  </si>
+  <si>
+    <t>Geben Sie einen eindeutigen Namen ein</t>
+  </si>
+  <si>
+    <t>Gidd en eendeitegen Numm un</t>
   </si>
 </sst>
 </file>
@@ -1547,10 +1562,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="string" displayName="string" ref="A1:E113" totalsRowShown="0">
-  <autoFilter ref="A1:E113" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E113">
-    <sortCondition ref="A1:A113"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="string" displayName="string" ref="A1:E114" totalsRowShown="0">
+  <autoFilter ref="A1:E114" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E114">
+    <sortCondition ref="A1:A114"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="keys"/>
@@ -1851,10 +1866,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E113"/>
+  <dimension ref="A1:E114"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="E113" sqref="E113"/>
+      <selection sqref="A1:E114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2531,1267 +2546,1284 @@
     </row>
     <row r="40" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>14</v>
+        <v>483</v>
       </c>
       <c r="B40" t="s">
-        <v>15</v>
+        <v>484</v>
       </c>
       <c r="C40" t="s">
-        <v>15</v>
+        <v>485</v>
       </c>
       <c r="D40" t="s">
-        <v>15</v>
+        <v>486</v>
       </c>
       <c r="E40" t="s">
-        <v>15</v>
+        <v>487</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>143</v>
+        <v>14</v>
       </c>
       <c r="B41" t="s">
-        <v>144</v>
+        <v>15</v>
       </c>
       <c r="C41" t="s">
-        <v>145</v>
+        <v>15</v>
       </c>
       <c r="D41" t="s">
-        <v>144</v>
+        <v>15</v>
       </c>
       <c r="E41" t="s">
-        <v>144</v>
+        <v>15</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>473</v>
+        <v>143</v>
       </c>
       <c r="B42" t="s">
-        <v>474</v>
+        <v>144</v>
       </c>
       <c r="C42" t="s">
-        <v>475</v>
+        <v>145</v>
       </c>
       <c r="D42" t="s">
-        <v>476</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>477</v>
+        <v>144</v>
+      </c>
+      <c r="E42" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>12</v>
+        <v>473</v>
       </c>
       <c r="B43" t="s">
-        <v>13</v>
+        <v>474</v>
       </c>
       <c r="C43" t="s">
-        <v>13</v>
+        <v>475</v>
       </c>
       <c r="D43" t="s">
-        <v>13</v>
-      </c>
-      <c r="E43" t="s">
-        <v>13</v>
+        <v>476</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>477</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>146</v>
+        <v>12</v>
       </c>
       <c r="B44" t="s">
-        <v>147</v>
+        <v>13</v>
       </c>
       <c r="C44" t="s">
-        <v>148</v>
+        <v>13</v>
       </c>
       <c r="D44" t="s">
-        <v>149</v>
+        <v>13</v>
       </c>
       <c r="E44" t="s">
-        <v>149</v>
+        <v>13</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>9</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>471</v>
+        <v>146</v>
+      </c>
+      <c r="B45" t="s">
+        <v>147</v>
+      </c>
+      <c r="C45" t="s">
+        <v>148</v>
+      </c>
+      <c r="D45" t="s">
+        <v>149</v>
+      </c>
+      <c r="E45" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>150</v>
-      </c>
-      <c r="B46" t="s">
-        <v>151</v>
-      </c>
-      <c r="C46" t="s">
-        <v>152</v>
-      </c>
-      <c r="D46" t="s">
-        <v>152</v>
-      </c>
-      <c r="E46" t="s">
-        <v>153</v>
+        <v>9</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>471</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B47" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C47" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D47" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="E47" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B48" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C48" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="D48" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="E48" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B49" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C49" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="D49" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="E49" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>430</v>
+        <v>164</v>
       </c>
       <c r="B50" t="s">
-        <v>429</v>
+        <v>165</v>
       </c>
       <c r="C50" t="s">
-        <v>431</v>
+        <v>166</v>
       </c>
       <c r="D50" t="s">
-        <v>432</v>
+        <v>167</v>
       </c>
       <c r="E50" t="s">
-        <v>433</v>
+        <v>168</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>169</v>
+        <v>430</v>
       </c>
       <c r="B51" t="s">
-        <v>170</v>
+        <v>429</v>
       </c>
       <c r="C51" t="s">
-        <v>171</v>
+        <v>431</v>
       </c>
       <c r="D51" t="s">
-        <v>172</v>
+        <v>432</v>
       </c>
       <c r="E51" t="s">
-        <v>173</v>
+        <v>433</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B52" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C52" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D52" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E52" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B53" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C53" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D53" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E53" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B54" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C54" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D54" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="E54" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>16</v>
+        <v>181</v>
       </c>
       <c r="B55" t="s">
-        <v>17</v>
+        <v>182</v>
       </c>
       <c r="C55" t="s">
-        <v>17</v>
+        <v>183</v>
       </c>
       <c r="D55" t="s">
-        <v>17</v>
+        <v>184</v>
       </c>
       <c r="E55" t="s">
-        <v>17</v>
+        <v>185</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>321</v>
+        <v>16</v>
       </c>
       <c r="B56" t="s">
-        <v>322</v>
+        <v>17</v>
       </c>
       <c r="C56" t="s">
-        <v>322</v>
+        <v>17</v>
       </c>
       <c r="D56" t="s">
-        <v>322</v>
+        <v>17</v>
       </c>
       <c r="E56" t="s">
-        <v>322</v>
+        <v>17</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B57" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C57" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="D57" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="E57" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>317</v>
+        <v>323</v>
       </c>
       <c r="B58" t="s">
-        <v>318</v>
+        <v>324</v>
       </c>
       <c r="C58" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
       <c r="D58" t="s">
-        <v>318</v>
+        <v>326</v>
       </c>
       <c r="E58" t="s">
-        <v>320</v>
+        <v>327</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>186</v>
+        <v>317</v>
       </c>
       <c r="B59" t="s">
-        <v>187</v>
+        <v>318</v>
       </c>
       <c r="C59" t="s">
-        <v>188</v>
+        <v>319</v>
       </c>
       <c r="D59" t="s">
-        <v>189</v>
+        <v>318</v>
       </c>
       <c r="E59" t="s">
-        <v>190</v>
+        <v>320</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>372</v>
+        <v>186</v>
       </c>
       <c r="B60" t="s">
-        <v>374</v>
+        <v>187</v>
       </c>
       <c r="C60" t="s">
-        <v>376</v>
+        <v>188</v>
       </c>
       <c r="D60" t="s">
-        <v>378</v>
+        <v>189</v>
       </c>
       <c r="E60" t="s">
-        <v>380</v>
+        <v>190</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>328</v>
+        <v>372</v>
       </c>
       <c r="B61" t="s">
-        <v>329</v>
+        <v>374</v>
       </c>
       <c r="C61" t="s">
-        <v>330</v>
+        <v>376</v>
       </c>
       <c r="D61" t="s">
-        <v>331</v>
+        <v>378</v>
       </c>
       <c r="E61" t="s">
-        <v>332</v>
+        <v>380</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>191</v>
+        <v>328</v>
       </c>
       <c r="B62" t="s">
-        <v>192</v>
+        <v>329</v>
       </c>
       <c r="C62" t="s">
-        <v>192</v>
+        <v>330</v>
       </c>
       <c r="D62" t="s">
-        <v>193</v>
+        <v>331</v>
       </c>
       <c r="E62" t="s">
-        <v>194</v>
+        <v>332</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B63" t="s">
-        <v>391</v>
+        <v>192</v>
       </c>
       <c r="C63" t="s">
-        <v>392</v>
+        <v>192</v>
       </c>
       <c r="D63" t="s">
-        <v>393</v>
+        <v>193</v>
       </c>
       <c r="E63" t="s">
-        <v>400</v>
+        <v>194</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>390</v>
+        <v>195</v>
       </c>
       <c r="B64" t="s">
-        <v>464</v>
+        <v>391</v>
       </c>
       <c r="C64" t="s">
-        <v>464</v>
+        <v>392</v>
       </c>
       <c r="D64" t="s">
-        <v>464</v>
+        <v>393</v>
       </c>
       <c r="E64" t="s">
-        <v>464</v>
+        <v>400</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>196</v>
+        <v>390</v>
       </c>
       <c r="B65" t="s">
-        <v>197</v>
+        <v>464</v>
       </c>
       <c r="C65" t="s">
-        <v>198</v>
+        <v>464</v>
       </c>
       <c r="D65" t="s">
-        <v>199</v>
+        <v>464</v>
       </c>
       <c r="E65" t="s">
-        <v>199</v>
+        <v>464</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B66" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C66" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="D66" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="E66" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B67" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="C67" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D67" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="E67" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B68" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C68" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="D68" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="E68" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B69" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="C69" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="D69" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="E69" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="B70" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="C70" t="s">
-        <v>395</v>
+        <v>217</v>
       </c>
       <c r="D70" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="E70" t="s">
-        <v>401</v>
+        <v>219</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B71" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C71" t="s">
-        <v>225</v>
+        <v>395</v>
       </c>
       <c r="D71" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="E71" t="s">
-        <v>227</v>
+        <v>401</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="B72" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C72" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="D72" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="E72" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>465</v>
+        <v>228</v>
       </c>
       <c r="B73" t="s">
-        <v>466</v>
+        <v>229</v>
       </c>
       <c r="C73" t="s">
-        <v>467</v>
+        <v>230</v>
       </c>
       <c r="D73" t="s">
-        <v>468</v>
+        <v>231</v>
       </c>
       <c r="E73" t="s">
-        <v>469</v>
+        <v>232</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>233</v>
+        <v>465</v>
       </c>
       <c r="B74" t="s">
-        <v>234</v>
+        <v>466</v>
       </c>
       <c r="C74" t="s">
-        <v>235</v>
+        <v>467</v>
       </c>
       <c r="D74" t="s">
-        <v>236</v>
+        <v>468</v>
       </c>
       <c r="E74" t="s">
-        <v>237</v>
+        <v>469</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>337</v>
+        <v>233</v>
       </c>
       <c r="B75" t="s">
-        <v>338</v>
+        <v>234</v>
       </c>
       <c r="C75" t="s">
-        <v>338</v>
+        <v>235</v>
       </c>
       <c r="D75" t="s">
-        <v>338</v>
+        <v>236</v>
       </c>
       <c r="E75" t="s">
-        <v>339</v>
+        <v>237</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>420</v>
+        <v>337</v>
       </c>
       <c r="B76" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C76" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
       <c r="D76" t="s">
-        <v>355</v>
+        <v>338</v>
       </c>
       <c r="E76" t="s">
-        <v>364</v>
+        <v>339</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B77" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C77" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D77" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E77" t="s">
-        <v>356</v>
+        <v>364</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="B78" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="C78" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D78" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="E78" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B79" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="C79" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D79" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E79" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B80" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="C80" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D80" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="E80" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B81" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C81" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D81" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="E81" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B82" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C82" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D82" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E82" t="s">
-        <v>399</v>
+        <v>366</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B83" t="s">
-        <v>434</v>
+        <v>345</v>
       </c>
       <c r="C83" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D83" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E83" t="s">
-        <v>367</v>
+        <v>399</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>238</v>
+        <v>427</v>
       </c>
       <c r="B84" t="s">
-        <v>239</v>
+        <v>434</v>
       </c>
       <c r="C84" t="s">
-        <v>240</v>
+        <v>354</v>
       </c>
       <c r="D84" t="s">
-        <v>241</v>
+        <v>362</v>
       </c>
       <c r="E84" t="s">
-        <v>242</v>
+        <v>367</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="B85" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="C85" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="D85" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="E85" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B86" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C86" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D86" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E86" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B87" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C87" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="D87" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="E87" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="B88" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="C88" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="D88" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="E88" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="B89" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="C89" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="D89" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="E89" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="B90" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="C90" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="D90" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="E90" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>440</v>
+        <v>263</v>
       </c>
       <c r="B91" t="s">
-        <v>441</v>
+        <v>264</v>
       </c>
       <c r="C91" t="s">
-        <v>442</v>
+        <v>265</v>
       </c>
       <c r="D91" t="s">
-        <v>443</v>
+        <v>266</v>
       </c>
       <c r="E91" t="s">
-        <v>444</v>
+        <v>267</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>268</v>
+        <v>440</v>
       </c>
       <c r="B92" t="s">
-        <v>269</v>
+        <v>441</v>
       </c>
       <c r="C92" t="s">
-        <v>270</v>
+        <v>442</v>
       </c>
       <c r="D92" t="s">
-        <v>271</v>
+        <v>443</v>
       </c>
       <c r="E92" t="s">
-        <v>271</v>
+        <v>444</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>368</v>
+        <v>268</v>
       </c>
       <c r="B93" t="s">
-        <v>369</v>
+        <v>269</v>
       </c>
       <c r="C93" t="s">
-        <v>370</v>
+        <v>270</v>
       </c>
       <c r="D93" t="s">
-        <v>369</v>
+        <v>271</v>
       </c>
       <c r="E93" t="s">
-        <v>369</v>
+        <v>271</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>435</v>
+        <v>368</v>
       </c>
       <c r="B94" t="s">
-        <v>436</v>
+        <v>369</v>
       </c>
       <c r="C94" t="s">
-        <v>437</v>
+        <v>370</v>
       </c>
       <c r="D94" t="s">
-        <v>438</v>
+        <v>369</v>
       </c>
       <c r="E94" t="s">
-        <v>439</v>
+        <v>369</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>272</v>
+        <v>435</v>
       </c>
       <c r="B95" t="s">
-        <v>273</v>
+        <v>436</v>
       </c>
       <c r="C95" t="s">
-        <v>274</v>
+        <v>437</v>
       </c>
       <c r="D95" t="s">
-        <v>275</v>
+        <v>438</v>
       </c>
       <c r="E95" t="s">
-        <v>275</v>
+        <v>439</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B96" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="C96" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D96" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="E96" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>416</v>
+        <v>276</v>
       </c>
       <c r="B97" t="s">
-        <v>417</v>
+        <v>277</v>
       </c>
       <c r="C97" t="s">
-        <v>418</v>
+        <v>278</v>
       </c>
       <c r="D97" t="s">
-        <v>419</v>
+        <v>279</v>
       </c>
       <c r="E97" t="s">
-        <v>419</v>
+        <v>279</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>403</v>
+        <v>416</v>
       </c>
       <c r="B98" t="s">
-        <v>412</v>
+        <v>417</v>
       </c>
       <c r="C98" t="s">
-        <v>413</v>
+        <v>418</v>
       </c>
       <c r="D98" t="s">
-        <v>414</v>
+        <v>419</v>
       </c>
       <c r="E98" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B99" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="C99" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
       <c r="D99" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="E99" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="B100" t="s">
-        <v>404</v>
+        <v>409</v>
       </c>
       <c r="C100" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
       <c r="D100" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
       <c r="E100" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>280</v>
+        <v>405</v>
       </c>
       <c r="B101" t="s">
-        <v>281</v>
+        <v>404</v>
       </c>
       <c r="C101" t="s">
-        <v>282</v>
+        <v>406</v>
       </c>
       <c r="D101" t="s">
-        <v>283</v>
+        <v>407</v>
       </c>
       <c r="E101" t="s">
-        <v>283</v>
+        <v>408</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="B102" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C102" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="D102" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="E102" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="B103" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="C103" t="s">
-        <v>396</v>
+        <v>286</v>
       </c>
       <c r="D103" t="s">
-        <v>428</v>
+        <v>287</v>
       </c>
       <c r="E103" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B104" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C104" t="s">
-        <v>293</v>
+        <v>396</v>
       </c>
       <c r="D104" t="s">
-        <v>292</v>
+        <v>428</v>
       </c>
       <c r="E104" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B105" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C105" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D105" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E105" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B106" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C106" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D106" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="E106" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="B107" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C107" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D107" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="E107" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B108" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C108" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D108" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="E108" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="B109" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="C109" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="D109" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="E109" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B110" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C110" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="D110" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="E110" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>445</v>
+        <v>312</v>
       </c>
       <c r="B111" t="s">
-        <v>451</v>
+        <v>313</v>
       </c>
       <c r="C111" t="s">
-        <v>448</v>
+        <v>314</v>
       </c>
       <c r="D111" t="s">
-        <v>446</v>
+        <v>315</v>
       </c>
       <c r="E111" t="s">
-        <v>447</v>
+        <v>316</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="B112" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="C112" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="D112" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
       <c r="E112" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
+        <v>449</v>
+      </c>
+      <c r="B113" t="s">
+        <v>450</v>
+      </c>
+      <c r="C113" t="s">
+        <v>452</v>
+      </c>
+      <c r="D113" t="s">
+        <v>453</v>
+      </c>
+      <c r="E113" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
         <v>371</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B114" t="s">
         <v>373</v>
       </c>
-      <c r="C113" t="s">
+      <c r="C114" t="s">
         <v>375</v>
       </c>
-      <c r="D113" t="s">
+      <c r="D114" t="s">
         <v>377</v>
       </c>
-      <c r="E113" t="s">
+      <c r="E114" t="s">
         <v>379</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B45" r:id="rId1" xr:uid="{772ACA42-8DE4-4015-A5BA-E378BC1F9836}"/>
-    <hyperlink ref="C45:E45" r:id="rId2" display="https://github.com/NightDreamGames/Graded" xr:uid="{F6D4AF19-D559-447E-AF49-35B5F0BBE70D}"/>
+    <hyperlink ref="B46" r:id="rId1" xr:uid="{772ACA42-8DE4-4015-A5BA-E378BC1F9836}"/>
+    <hyperlink ref="C46:E46" r:id="rId2" display="https://github.com/NightDreamGames/Graded" xr:uid="{F6D4AF19-D559-447E-AF49-35B5F0BBE70D}"/>
     <hyperlink ref="B38" r:id="rId3" xr:uid="{7E3A0FC6-064A-4102-B40F-1969830D4899}"/>
     <hyperlink ref="C38:E38" r:id="rId4" display="contact@nightdreamgames.com" xr:uid="{49649B53-773A-4287-9E32-3113566F351E}"/>
   </hyperlinks>

</xml_diff>

<commit_message>
Add UI for Subject Groups
</commit_message>
<xml_diff>
--- a/assets/Localizations.xlsx
+++ b/assets/Localizations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Graded\Graded - Flutter\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E11EA5E5-0C8C-41F8-B2E9-DFB3FF5AF2C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1EF9F41-52D7-46FE-A414-982C37F4FEFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="string" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0">string!$A$1:$B$111</definedName>
+    <definedName name="ExternalData_1" localSheetId="0">string!$A$1:$B$116</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="499">
   <si>
     <t>keys</t>
   </si>
@@ -1457,6 +1457,69 @@
   </si>
   <si>
     <t>Semestre</t>
+  </si>
+  <si>
+    <t>Exam</t>
+  </si>
+  <si>
+    <t>exams</t>
+  </si>
+  <si>
+    <t>Exams</t>
+  </si>
+  <si>
+    <t>Examens</t>
+  </si>
+  <si>
+    <t>Examen</t>
+  </si>
+  <si>
+    <t>exam</t>
+  </si>
+  <si>
+    <t>Add group</t>
+  </si>
+  <si>
+    <t>add_group</t>
+  </si>
+  <si>
+    <t>Ajouter un groupe</t>
+  </si>
+  <si>
+    <t>Gruppe hinzufügen</t>
+  </si>
+  <si>
+    <t>Grupp zoufügen</t>
+  </si>
+  <si>
+    <t>edit_group</t>
+  </si>
+  <si>
+    <t>Edit group</t>
+  </si>
+  <si>
+    <t>Modifier un groupe</t>
+  </si>
+  <si>
+    <t>Gruppe bearbeiten</t>
+  </si>
+  <si>
+    <t>Grupp beaarbechten</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Groupe</t>
+  </si>
+  <si>
+    <t>Gruppe</t>
+  </si>
+  <si>
+    <t>Grupp</t>
   </si>
 </sst>
 </file>
@@ -1532,10 +1595,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="string" displayName="string" ref="A1:E111" totalsRowShown="0">
-  <autoFilter ref="A1:E111" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E111">
-    <sortCondition ref="A1:A111"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="string" displayName="string" ref="A1:E116" totalsRowShown="0">
+  <autoFilter ref="A1:E116" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E116">
+    <sortCondition ref="A1:A116"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="keys"/>
@@ -1836,10 +1899,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E111"/>
+  <dimension ref="A1:E116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="A104" sqref="A104:C105"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="E116" sqref="E116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1921,1830 +1984,1915 @@
     </row>
     <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>485</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>484</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>486</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>487</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
+        <v>488</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E6" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E7" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>455</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>455</v>
+        <v>41</v>
       </c>
       <c r="D8" t="s">
-        <v>455</v>
+        <v>42</v>
       </c>
       <c r="E8" t="s">
-        <v>455</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>455</v>
       </c>
       <c r="C9" t="s">
-        <v>379</v>
+        <v>455</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
+        <v>455</v>
       </c>
       <c r="E9" t="s">
-        <v>47</v>
+        <v>455</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>379</v>
       </c>
       <c r="D10" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E10" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B11" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D11" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>55</v>
       </c>
       <c r="D12" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="E12" t="s">
-        <v>7</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>58</v>
+        <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>59</v>
+        <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>58</v>
+        <v>7</v>
       </c>
       <c r="E13" t="s">
-        <v>58</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D14" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E14" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>444</v>
+        <v>60</v>
       </c>
       <c r="B15" t="s">
-        <v>445</v>
+        <v>61</v>
       </c>
       <c r="C15" t="s">
-        <v>446</v>
+        <v>61</v>
       </c>
       <c r="D15" t="s">
-        <v>447</v>
+        <v>61</v>
       </c>
       <c r="E15" t="s">
-        <v>448</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>366</v>
+        <v>444</v>
       </c>
       <c r="B16" t="s">
-        <v>368</v>
+        <v>445</v>
       </c>
       <c r="C16" t="s">
-        <v>369</v>
+        <v>446</v>
       </c>
       <c r="D16" t="s">
-        <v>371</v>
+        <v>447</v>
       </c>
       <c r="E16" t="s">
-        <v>370</v>
+        <v>448</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B17" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="C17" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="D17" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="E17" t="s">
-        <v>382</v>
+        <v>370</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>62</v>
+        <v>367</v>
       </c>
       <c r="B18" t="s">
-        <v>63</v>
+        <v>373</v>
       </c>
       <c r="C18" t="s">
-        <v>64</v>
+        <v>372</v>
       </c>
       <c r="D18" t="s">
-        <v>65</v>
+        <v>374</v>
       </c>
       <c r="E18" t="s">
-        <v>66</v>
+        <v>382</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B19" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C19" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D19" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E19" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>318</v>
+        <v>67</v>
       </c>
       <c r="B20" t="s">
-        <v>319</v>
+        <v>68</v>
       </c>
       <c r="C20" t="s">
-        <v>320</v>
+        <v>69</v>
       </c>
       <c r="D20" t="s">
-        <v>321</v>
+        <v>70</v>
       </c>
       <c r="E20" t="s">
-        <v>321</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>72</v>
+        <v>318</v>
       </c>
       <c r="B21" t="s">
-        <v>73</v>
+        <v>319</v>
       </c>
       <c r="C21" t="s">
-        <v>73</v>
+        <v>320</v>
       </c>
       <c r="D21" t="s">
-        <v>74</v>
+        <v>321</v>
       </c>
       <c r="E21" t="s">
-        <v>74</v>
+        <v>321</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B22" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C22" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D22" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E22" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B23" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C23" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D23" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E23" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>463</v>
+        <v>78</v>
       </c>
       <c r="B24" t="s">
-        <v>464</v>
+        <v>79</v>
       </c>
       <c r="C24" t="s">
-        <v>466</v>
+        <v>79</v>
       </c>
       <c r="D24" t="s">
-        <v>465</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>467</v>
+        <v>80</v>
+      </c>
+      <c r="E24" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>82</v>
+        <v>463</v>
       </c>
       <c r="B25" t="s">
-        <v>83</v>
+        <v>464</v>
       </c>
       <c r="C25" t="s">
-        <v>84</v>
+        <v>466</v>
       </c>
       <c r="D25" t="s">
-        <v>85</v>
-      </c>
-      <c r="E25" t="s">
-        <v>86</v>
+        <v>465</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>467</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B26" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C26" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D26" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E26" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B27" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C27" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D27" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E27" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B28" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C28" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D28" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E28" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B29" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C29" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D29" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E29" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B30" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C30" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D30" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E30" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B31" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C31" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D31" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E31" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B32" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C32" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D32" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E32" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B33" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C33" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D33" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E33" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B34" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C34" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D34" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E34" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>129</v>
+        <v>489</v>
       </c>
       <c r="B35" t="s">
-        <v>130</v>
+        <v>490</v>
       </c>
       <c r="C35" t="s">
-        <v>131</v>
+        <v>491</v>
       </c>
       <c r="D35" t="s">
-        <v>132</v>
+        <v>492</v>
       </c>
       <c r="E35" t="s">
-        <v>133</v>
+        <v>493</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="B36" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="C36" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="D36" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="E36" t="s">
-        <v>383</v>
+        <v>128</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="B37" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="C37" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="D37" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="E37" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>18</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>457</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>457</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>457</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>457</v>
+        <v>134</v>
+      </c>
+      <c r="B38" t="s">
+        <v>135</v>
+      </c>
+      <c r="C38" t="s">
+        <v>136</v>
+      </c>
+      <c r="D38" t="s">
+        <v>137</v>
+      </c>
+      <c r="E38" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>10</v>
+        <v>138</v>
       </c>
       <c r="B39" t="s">
-        <v>11</v>
+        <v>139</v>
       </c>
       <c r="C39" t="s">
-        <v>11</v>
+        <v>140</v>
       </c>
       <c r="D39" t="s">
-        <v>11</v>
+        <v>141</v>
       </c>
       <c r="E39" t="s">
-        <v>11</v>
+        <v>142</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>468</v>
-      </c>
-      <c r="B40" t="s">
-        <v>469</v>
-      </c>
-      <c r="C40" t="s">
-        <v>470</v>
-      </c>
-      <c r="D40" t="s">
-        <v>471</v>
-      </c>
-      <c r="E40" t="s">
-        <v>472</v>
+        <v>18</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B41" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C41" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D41" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E41" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>143</v>
+        <v>468</v>
       </c>
       <c r="B42" t="s">
-        <v>144</v>
+        <v>469</v>
       </c>
       <c r="C42" t="s">
-        <v>145</v>
+        <v>470</v>
       </c>
       <c r="D42" t="s">
-        <v>144</v>
+        <v>471</v>
       </c>
       <c r="E42" t="s">
-        <v>144</v>
+        <v>472</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>458</v>
+        <v>483</v>
       </c>
       <c r="B43" t="s">
-        <v>459</v>
+        <v>478</v>
       </c>
       <c r="C43" t="s">
-        <v>460</v>
+        <v>482</v>
       </c>
       <c r="D43" t="s">
-        <v>461</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>462</v>
+        <v>482</v>
+      </c>
+      <c r="E43" t="s">
+        <v>482</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>12</v>
+        <v>479</v>
       </c>
       <c r="B44" t="s">
-        <v>13</v>
+        <v>480</v>
       </c>
       <c r="C44" t="s">
-        <v>13</v>
+        <v>481</v>
       </c>
       <c r="D44" t="s">
-        <v>13</v>
+        <v>482</v>
       </c>
       <c r="E44" t="s">
-        <v>13</v>
+        <v>482</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>146</v>
+        <v>14</v>
       </c>
       <c r="B45" t="s">
-        <v>147</v>
+        <v>15</v>
       </c>
       <c r="C45" t="s">
-        <v>148</v>
+        <v>15</v>
       </c>
       <c r="D45" t="s">
-        <v>149</v>
+        <v>15</v>
       </c>
       <c r="E45" t="s">
-        <v>149</v>
+        <v>15</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>9</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>456</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>456</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>456</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>456</v>
+        <v>143</v>
+      </c>
+      <c r="B46" t="s">
+        <v>144</v>
+      </c>
+      <c r="C46" t="s">
+        <v>145</v>
+      </c>
+      <c r="D46" t="s">
+        <v>144</v>
+      </c>
+      <c r="E46" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>150</v>
+        <v>458</v>
       </c>
       <c r="B47" t="s">
-        <v>151</v>
+        <v>459</v>
       </c>
       <c r="C47" t="s">
-        <v>152</v>
+        <v>460</v>
       </c>
       <c r="D47" t="s">
-        <v>152</v>
-      </c>
-      <c r="E47" t="s">
-        <v>153</v>
+        <v>461</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>154</v>
+        <v>12</v>
       </c>
       <c r="B48" t="s">
-        <v>155</v>
+        <v>13</v>
       </c>
       <c r="C48" t="s">
-        <v>156</v>
+        <v>13</v>
       </c>
       <c r="D48" t="s">
-        <v>157</v>
+        <v>13</v>
       </c>
       <c r="E48" t="s">
-        <v>158</v>
+        <v>13</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="B49" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="C49" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="D49" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="E49" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>164</v>
-      </c>
-      <c r="B50" t="s">
-        <v>165</v>
-      </c>
-      <c r="C50" t="s">
-        <v>166</v>
-      </c>
-      <c r="D50" t="s">
-        <v>167</v>
-      </c>
-      <c r="E50" t="s">
-        <v>168</v>
+        <v>9</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>456</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>415</v>
+        <v>150</v>
       </c>
       <c r="B51" t="s">
-        <v>414</v>
+        <v>151</v>
       </c>
       <c r="C51" t="s">
-        <v>416</v>
+        <v>152</v>
       </c>
       <c r="D51" t="s">
-        <v>417</v>
+        <v>152</v>
       </c>
       <c r="E51" t="s">
-        <v>418</v>
+        <v>153</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="B52" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="C52" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="D52" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="E52" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>174</v>
+        <v>494</v>
       </c>
       <c r="B53" t="s">
-        <v>175</v>
+        <v>495</v>
       </c>
       <c r="C53" t="s">
-        <v>175</v>
+        <v>496</v>
       </c>
       <c r="D53" t="s">
-        <v>176</v>
+        <v>497</v>
       </c>
       <c r="E53" t="s">
-        <v>177</v>
+        <v>498</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>178</v>
+        <v>159</v>
       </c>
       <c r="B54" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
       <c r="C54" t="s">
-        <v>179</v>
+        <v>161</v>
       </c>
       <c r="D54" t="s">
-        <v>180</v>
+        <v>162</v>
       </c>
       <c r="E54" t="s">
-        <v>180</v>
+        <v>163</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>181</v>
+        <v>164</v>
       </c>
       <c r="B55" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="C55" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
       <c r="D55" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="E55" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>16</v>
+        <v>415</v>
       </c>
       <c r="B56" t="s">
-        <v>17</v>
+        <v>414</v>
       </c>
       <c r="C56" t="s">
-        <v>17</v>
+        <v>416</v>
       </c>
       <c r="D56" t="s">
-        <v>17</v>
+        <v>417</v>
       </c>
       <c r="E56" t="s">
-        <v>17</v>
+        <v>418</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>306</v>
+        <v>169</v>
       </c>
       <c r="B57" t="s">
-        <v>307</v>
+        <v>170</v>
       </c>
       <c r="C57" t="s">
-        <v>307</v>
+        <v>171</v>
       </c>
       <c r="D57" t="s">
-        <v>307</v>
+        <v>172</v>
       </c>
       <c r="E57" t="s">
-        <v>307</v>
+        <v>173</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>308</v>
+        <v>174</v>
       </c>
       <c r="B58" t="s">
-        <v>309</v>
+        <v>175</v>
       </c>
       <c r="C58" t="s">
-        <v>310</v>
+        <v>175</v>
       </c>
       <c r="D58" t="s">
-        <v>311</v>
+        <v>176</v>
       </c>
       <c r="E58" t="s">
-        <v>312</v>
+        <v>177</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>302</v>
+        <v>178</v>
       </c>
       <c r="B59" t="s">
-        <v>303</v>
+        <v>179</v>
       </c>
       <c r="C59" t="s">
-        <v>304</v>
+        <v>179</v>
       </c>
       <c r="D59" t="s">
-        <v>303</v>
+        <v>180</v>
       </c>
       <c r="E59" t="s">
-        <v>305</v>
+        <v>180</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="B60" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="C60" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="D60" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E60" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>357</v>
+        <v>16</v>
       </c>
       <c r="B61" t="s">
-        <v>359</v>
+        <v>17</v>
       </c>
       <c r="C61" t="s">
-        <v>361</v>
+        <v>17</v>
       </c>
       <c r="D61" t="s">
-        <v>363</v>
+        <v>17</v>
       </c>
       <c r="E61" t="s">
-        <v>365</v>
+        <v>17</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="B62" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="C62" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="D62" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E62" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>191</v>
+        <v>308</v>
       </c>
       <c r="B63" t="s">
-        <v>192</v>
+        <v>309</v>
       </c>
       <c r="C63" t="s">
-        <v>192</v>
+        <v>310</v>
       </c>
       <c r="D63" t="s">
-        <v>193</v>
+        <v>311</v>
       </c>
       <c r="E63" t="s">
-        <v>194</v>
+        <v>312</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>195</v>
+        <v>302</v>
       </c>
       <c r="B64" t="s">
-        <v>376</v>
+        <v>303</v>
       </c>
       <c r="C64" t="s">
-        <v>377</v>
+        <v>304</v>
       </c>
       <c r="D64" t="s">
-        <v>378</v>
+        <v>303</v>
       </c>
       <c r="E64" t="s">
-        <v>385</v>
+        <v>305</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>375</v>
+        <v>186</v>
       </c>
       <c r="B65" t="s">
-        <v>449</v>
+        <v>187</v>
       </c>
       <c r="C65" t="s">
-        <v>449</v>
+        <v>188</v>
       </c>
       <c r="D65" t="s">
-        <v>449</v>
+        <v>189</v>
       </c>
       <c r="E65" t="s">
-        <v>449</v>
+        <v>190</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>196</v>
+        <v>357</v>
       </c>
       <c r="B66" t="s">
-        <v>197</v>
+        <v>359</v>
       </c>
       <c r="C66" t="s">
-        <v>198</v>
+        <v>361</v>
       </c>
       <c r="D66" t="s">
-        <v>199</v>
+        <v>363</v>
       </c>
       <c r="E66" t="s">
-        <v>199</v>
+        <v>365</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>200</v>
+        <v>313</v>
       </c>
       <c r="B67" t="s">
-        <v>201</v>
+        <v>314</v>
       </c>
       <c r="C67" t="s">
-        <v>202</v>
+        <v>315</v>
       </c>
       <c r="D67" t="s">
-        <v>203</v>
+        <v>316</v>
       </c>
       <c r="E67" t="s">
-        <v>204</v>
+        <v>317</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="B68" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="C68" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="D68" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="E68" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
       <c r="B69" t="s">
-        <v>211</v>
+        <v>376</v>
       </c>
       <c r="C69" t="s">
-        <v>212</v>
+        <v>377</v>
       </c>
       <c r="D69" t="s">
-        <v>213</v>
+        <v>378</v>
       </c>
       <c r="E69" t="s">
-        <v>214</v>
+        <v>385</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>215</v>
+        <v>375</v>
       </c>
       <c r="B70" t="s">
-        <v>216</v>
+        <v>449</v>
       </c>
       <c r="C70" t="s">
-        <v>217</v>
+        <v>449</v>
       </c>
       <c r="D70" t="s">
-        <v>218</v>
+        <v>449</v>
       </c>
       <c r="E70" t="s">
-        <v>219</v>
+        <v>449</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>220</v>
+        <v>196</v>
       </c>
       <c r="B71" t="s">
-        <v>221</v>
+        <v>197</v>
       </c>
       <c r="C71" t="s">
-        <v>380</v>
+        <v>198</v>
       </c>
       <c r="D71" t="s">
-        <v>222</v>
+        <v>199</v>
       </c>
       <c r="E71" t="s">
-        <v>386</v>
+        <v>199</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>223</v>
+        <v>200</v>
       </c>
       <c r="B72" t="s">
-        <v>224</v>
+        <v>201</v>
       </c>
       <c r="C72" t="s">
-        <v>225</v>
+        <v>202</v>
       </c>
       <c r="D72" t="s">
-        <v>226</v>
+        <v>203</v>
       </c>
       <c r="E72" t="s">
-        <v>227</v>
+        <v>204</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>228</v>
+        <v>205</v>
       </c>
       <c r="B73" t="s">
-        <v>229</v>
+        <v>206</v>
       </c>
       <c r="C73" t="s">
-        <v>230</v>
+        <v>207</v>
       </c>
       <c r="D73" t="s">
-        <v>231</v>
+        <v>208</v>
       </c>
       <c r="E73" t="s">
-        <v>232</v>
+        <v>209</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>450</v>
+        <v>210</v>
       </c>
       <c r="B74" t="s">
-        <v>451</v>
+        <v>211</v>
       </c>
       <c r="C74" t="s">
-        <v>452</v>
+        <v>212</v>
       </c>
       <c r="D74" t="s">
-        <v>453</v>
+        <v>213</v>
       </c>
       <c r="E74" t="s">
-        <v>454</v>
+        <v>214</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="B75" t="s">
-        <v>234</v>
+        <v>216</v>
       </c>
       <c r="C75" t="s">
-        <v>235</v>
+        <v>217</v>
       </c>
       <c r="D75" t="s">
-        <v>236</v>
+        <v>218</v>
       </c>
       <c r="E75" t="s">
-        <v>237</v>
+        <v>219</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>322</v>
+        <v>220</v>
       </c>
       <c r="B76" t="s">
-        <v>323</v>
+        <v>221</v>
       </c>
       <c r="C76" t="s">
-        <v>323</v>
+        <v>380</v>
       </c>
       <c r="D76" t="s">
-        <v>473</v>
+        <v>222</v>
       </c>
       <c r="E76" t="s">
-        <v>324</v>
+        <v>386</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>405</v>
+        <v>223</v>
       </c>
       <c r="B77" t="s">
-        <v>325</v>
+        <v>224</v>
       </c>
       <c r="C77" t="s">
-        <v>332</v>
+        <v>225</v>
       </c>
       <c r="D77" t="s">
-        <v>340</v>
+        <v>226</v>
       </c>
       <c r="E77" t="s">
-        <v>349</v>
+        <v>227</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>407</v>
+        <v>228</v>
       </c>
       <c r="B78" t="s">
-        <v>326</v>
+        <v>229</v>
       </c>
       <c r="C78" t="s">
-        <v>333</v>
+        <v>230</v>
       </c>
       <c r="D78" t="s">
-        <v>341</v>
+        <v>231</v>
       </c>
       <c r="E78" t="s">
-        <v>341</v>
+        <v>232</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>406</v>
+        <v>450</v>
       </c>
       <c r="B79" t="s">
-        <v>331</v>
+        <v>451</v>
       </c>
       <c r="C79" t="s">
-        <v>334</v>
+        <v>452</v>
       </c>
       <c r="D79" t="s">
-        <v>343</v>
+        <v>453</v>
       </c>
       <c r="E79" t="s">
-        <v>348</v>
+        <v>454</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>408</v>
+        <v>233</v>
       </c>
       <c r="B80" t="s">
-        <v>329</v>
+        <v>234</v>
       </c>
       <c r="C80" t="s">
-        <v>335</v>
+        <v>235</v>
       </c>
       <c r="D80" t="s">
-        <v>344</v>
+        <v>236</v>
       </c>
       <c r="E80" t="s">
-        <v>344</v>
+        <v>237</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>409</v>
+        <v>322</v>
       </c>
       <c r="B81" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="C81" t="s">
-        <v>336</v>
+        <v>323</v>
       </c>
       <c r="D81" t="s">
-        <v>342</v>
+        <v>473</v>
       </c>
       <c r="E81" t="s">
-        <v>350</v>
+        <v>324</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="B82" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C82" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="D82" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="E82" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="B83" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="C83" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="D83" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="E83" t="s">
-        <v>384</v>
+        <v>341</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="B84" t="s">
-        <v>419</v>
+        <v>331</v>
       </c>
       <c r="C84" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="D84" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="E84" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>238</v>
+        <v>408</v>
       </c>
       <c r="B85" t="s">
-        <v>239</v>
+        <v>329</v>
       </c>
       <c r="C85" t="s">
-        <v>240</v>
+        <v>335</v>
       </c>
       <c r="D85" t="s">
-        <v>241</v>
+        <v>344</v>
       </c>
       <c r="E85" t="s">
-        <v>242</v>
+        <v>344</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>476</v>
+        <v>409</v>
       </c>
       <c r="B86" t="s">
-        <v>246</v>
+        <v>327</v>
       </c>
       <c r="C86" t="s">
-        <v>477</v>
+        <v>336</v>
       </c>
       <c r="D86" t="s">
-        <v>246</v>
+        <v>342</v>
       </c>
       <c r="E86" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>243</v>
+        <v>410</v>
       </c>
       <c r="B87" t="s">
-        <v>244</v>
+        <v>328</v>
       </c>
       <c r="C87" t="s">
-        <v>245</v>
+        <v>337</v>
       </c>
       <c r="D87" t="s">
-        <v>246</v>
+        <v>345</v>
       </c>
       <c r="E87" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>247</v>
+        <v>411</v>
       </c>
       <c r="B88" t="s">
-        <v>248</v>
+        <v>330</v>
       </c>
       <c r="C88" t="s">
-        <v>249</v>
+        <v>338</v>
       </c>
       <c r="D88" t="s">
-        <v>250</v>
+        <v>346</v>
       </c>
       <c r="E88" t="s">
-        <v>251</v>
+        <v>384</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>252</v>
+        <v>412</v>
       </c>
       <c r="B89" t="s">
-        <v>253</v>
+        <v>419</v>
       </c>
       <c r="C89" t="s">
-        <v>254</v>
+        <v>339</v>
       </c>
       <c r="D89" t="s">
-        <v>255</v>
+        <v>347</v>
       </c>
       <c r="E89" t="s">
-        <v>256</v>
+        <v>352</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>257</v>
+        <v>238</v>
       </c>
       <c r="B90" t="s">
-        <v>258</v>
+        <v>239</v>
       </c>
       <c r="C90" t="s">
-        <v>259</v>
+        <v>240</v>
       </c>
       <c r="D90" t="s">
-        <v>260</v>
+        <v>241</v>
       </c>
       <c r="E90" t="s">
-        <v>261</v>
+        <v>242</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>425</v>
+        <v>476</v>
       </c>
       <c r="B91" t="s">
-        <v>426</v>
+        <v>246</v>
       </c>
       <c r="C91" t="s">
-        <v>427</v>
+        <v>477</v>
       </c>
       <c r="D91" t="s">
-        <v>428</v>
+        <v>246</v>
       </c>
       <c r="E91" t="s">
-        <v>429</v>
+        <v>246</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>262</v>
+        <v>243</v>
       </c>
       <c r="B92" t="s">
-        <v>263</v>
+        <v>244</v>
       </c>
       <c r="C92" t="s">
-        <v>264</v>
+        <v>245</v>
       </c>
       <c r="D92" t="s">
-        <v>265</v>
+        <v>246</v>
       </c>
       <c r="E92" t="s">
-        <v>265</v>
+        <v>246</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>353</v>
+        <v>247</v>
       </c>
       <c r="B93" t="s">
-        <v>354</v>
+        <v>248</v>
       </c>
       <c r="C93" t="s">
-        <v>355</v>
+        <v>249</v>
       </c>
       <c r="D93" t="s">
-        <v>354</v>
+        <v>250</v>
       </c>
       <c r="E93" t="s">
-        <v>354</v>
+        <v>251</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>420</v>
+        <v>252</v>
       </c>
       <c r="B94" t="s">
-        <v>421</v>
+        <v>253</v>
       </c>
       <c r="C94" t="s">
-        <v>422</v>
+        <v>254</v>
       </c>
       <c r="D94" t="s">
-        <v>423</v>
+        <v>255</v>
       </c>
       <c r="E94" t="s">
-        <v>424</v>
+        <v>256</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="B95" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="C95" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="D95" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="E95" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>270</v>
+        <v>425</v>
       </c>
       <c r="B96" t="s">
-        <v>271</v>
+        <v>426</v>
       </c>
       <c r="C96" t="s">
-        <v>272</v>
+        <v>427</v>
       </c>
       <c r="D96" t="s">
-        <v>273</v>
+        <v>428</v>
       </c>
       <c r="E96" t="s">
-        <v>273</v>
+        <v>429</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>401</v>
+        <v>262</v>
       </c>
       <c r="B97" t="s">
-        <v>402</v>
+        <v>263</v>
       </c>
       <c r="C97" t="s">
-        <v>403</v>
+        <v>264</v>
       </c>
       <c r="D97" t="s">
-        <v>404</v>
+        <v>265</v>
       </c>
       <c r="E97" t="s">
-        <v>404</v>
+        <v>265</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>388</v>
+        <v>353</v>
       </c>
       <c r="B98" t="s">
-        <v>397</v>
+        <v>354</v>
       </c>
       <c r="C98" t="s">
-        <v>398</v>
+        <v>355</v>
       </c>
       <c r="D98" t="s">
-        <v>399</v>
+        <v>354</v>
       </c>
       <c r="E98" t="s">
-        <v>400</v>
+        <v>354</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>387</v>
+        <v>420</v>
       </c>
       <c r="B99" t="s">
-        <v>394</v>
+        <v>421</v>
       </c>
       <c r="C99" t="s">
-        <v>395</v>
+        <v>422</v>
       </c>
       <c r="D99" t="s">
-        <v>396</v>
+        <v>423</v>
       </c>
       <c r="E99" t="s">
-        <v>396</v>
+        <v>424</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>390</v>
+        <v>266</v>
       </c>
       <c r="B100" t="s">
-        <v>389</v>
+        <v>267</v>
       </c>
       <c r="C100" t="s">
-        <v>391</v>
+        <v>268</v>
       </c>
       <c r="D100" t="s">
-        <v>392</v>
+        <v>269</v>
       </c>
       <c r="E100" t="s">
-        <v>393</v>
+        <v>269</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B101" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C101" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D101" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="E101" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>278</v>
+        <v>401</v>
       </c>
       <c r="B102" t="s">
-        <v>279</v>
+        <v>402</v>
       </c>
       <c r="C102" t="s">
-        <v>280</v>
+        <v>403</v>
       </c>
       <c r="D102" t="s">
-        <v>281</v>
+        <v>404</v>
       </c>
       <c r="E102" t="s">
-        <v>281</v>
+        <v>404</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>282</v>
+        <v>388</v>
       </c>
       <c r="B103" t="s">
-        <v>283</v>
+        <v>397</v>
       </c>
       <c r="C103" t="s">
-        <v>381</v>
+        <v>398</v>
       </c>
       <c r="D103" t="s">
-        <v>413</v>
+        <v>399</v>
       </c>
       <c r="E103" t="s">
-        <v>284</v>
+        <v>400</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>474</v>
+        <v>387</v>
       </c>
       <c r="B104" t="s">
-        <v>288</v>
+        <v>394</v>
       </c>
       <c r="C104" t="s">
-        <v>475</v>
+        <v>395</v>
       </c>
       <c r="D104" t="s">
-        <v>288</v>
+        <v>396</v>
       </c>
       <c r="E104" t="s">
-        <v>288</v>
+        <v>396</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>285</v>
+        <v>390</v>
       </c>
       <c r="B105" t="s">
-        <v>286</v>
+        <v>389</v>
       </c>
       <c r="C105" t="s">
-        <v>287</v>
+        <v>391</v>
       </c>
       <c r="D105" t="s">
-        <v>288</v>
+        <v>392</v>
       </c>
       <c r="E105" t="s">
-        <v>288</v>
+        <v>393</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>289</v>
+        <v>274</v>
       </c>
       <c r="B106" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
       <c r="C106" t="s">
-        <v>291</v>
+        <v>276</v>
       </c>
       <c r="D106" t="s">
-        <v>292</v>
+        <v>277</v>
       </c>
       <c r="E106" t="s">
-        <v>293</v>
+        <v>277</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>294</v>
+        <v>278</v>
       </c>
       <c r="B107" t="s">
-        <v>295</v>
+        <v>279</v>
       </c>
       <c r="C107" t="s">
-        <v>296</v>
+        <v>280</v>
       </c>
       <c r="D107" t="s">
-        <v>296</v>
+        <v>281</v>
       </c>
       <c r="E107" t="s">
-        <v>296</v>
+        <v>281</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>297</v>
+        <v>282</v>
       </c>
       <c r="B108" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="C108" t="s">
-        <v>299</v>
+        <v>381</v>
       </c>
       <c r="D108" t="s">
-        <v>300</v>
+        <v>413</v>
       </c>
       <c r="E108" t="s">
-        <v>301</v>
+        <v>284</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>430</v>
+        <v>474</v>
       </c>
       <c r="B109" t="s">
-        <v>436</v>
+        <v>288</v>
       </c>
       <c r="C109" t="s">
-        <v>433</v>
+        <v>475</v>
       </c>
       <c r="D109" t="s">
-        <v>431</v>
+        <v>288</v>
       </c>
       <c r="E109" t="s">
-        <v>432</v>
+        <v>288</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>434</v>
+        <v>285</v>
       </c>
       <c r="B110" t="s">
-        <v>435</v>
+        <v>286</v>
       </c>
       <c r="C110" t="s">
-        <v>437</v>
+        <v>287</v>
       </c>
       <c r="D110" t="s">
-        <v>438</v>
+        <v>288</v>
       </c>
       <c r="E110" t="s">
-        <v>439</v>
+        <v>288</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
+        <v>289</v>
+      </c>
+      <c r="B111" t="s">
+        <v>290</v>
+      </c>
+      <c r="C111" t="s">
+        <v>291</v>
+      </c>
+      <c r="D111" t="s">
+        <v>292</v>
+      </c>
+      <c r="E111" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>294</v>
+      </c>
+      <c r="B112" t="s">
+        <v>295</v>
+      </c>
+      <c r="C112" t="s">
+        <v>296</v>
+      </c>
+      <c r="D112" t="s">
+        <v>296</v>
+      </c>
+      <c r="E112" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>297</v>
+      </c>
+      <c r="B113" t="s">
+        <v>298</v>
+      </c>
+      <c r="C113" t="s">
+        <v>299</v>
+      </c>
+      <c r="D113" t="s">
+        <v>300</v>
+      </c>
+      <c r="E113" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>430</v>
+      </c>
+      <c r="B114" t="s">
+        <v>436</v>
+      </c>
+      <c r="C114" t="s">
+        <v>433</v>
+      </c>
+      <c r="D114" t="s">
+        <v>431</v>
+      </c>
+      <c r="E114" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>434</v>
+      </c>
+      <c r="B115" t="s">
+        <v>435</v>
+      </c>
+      <c r="C115" t="s">
+        <v>437</v>
+      </c>
+      <c r="D115" t="s">
+        <v>438</v>
+      </c>
+      <c r="E115" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
         <v>356</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B116" t="s">
         <v>358</v>
       </c>
-      <c r="C111" t="s">
+      <c r="C116" t="s">
         <v>360</v>
       </c>
-      <c r="D111" t="s">
+      <c r="D116" t="s">
         <v>362</v>
       </c>
-      <c r="E111" t="s">
+      <c r="E116" t="s">
         <v>364</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B46" r:id="rId1" xr:uid="{772ACA42-8DE4-4015-A5BA-E378BC1F9836}"/>
-    <hyperlink ref="C46:E46" r:id="rId2" display="https://github.com/NightDreamGames/Graded" xr:uid="{F6D4AF19-D559-447E-AF49-35B5F0BBE70D}"/>
-    <hyperlink ref="B38" r:id="rId3" xr:uid="{7E3A0FC6-064A-4102-B40F-1969830D4899}"/>
-    <hyperlink ref="C38:E38" r:id="rId4" display="contact@nightdreamgames.com" xr:uid="{49649B53-773A-4287-9E32-3113566F351E}"/>
+    <hyperlink ref="B50" r:id="rId1" xr:uid="{772ACA42-8DE4-4015-A5BA-E378BC1F9836}"/>
+    <hyperlink ref="C50:E50" r:id="rId2" display="https://github.com/NightDreamGames/Graded" xr:uid="{F6D4AF19-D559-447E-AF49-35B5F0BBE70D}"/>
+    <hyperlink ref="B40" r:id="rId3" xr:uid="{7E3A0FC6-064A-4102-B40F-1969830D4899}"/>
+    <hyperlink ref="C40:E40" r:id="rId4" display="contact@nightdreamgames.com" xr:uid="{49649B53-773A-4287-9E32-3113566F351E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>

</xml_diff>

<commit_message>
Implement new setup system
Now uses the new JSON dataset, also implements the general system. The bug with the SettingsTile showing "Not set" when it actually is should now be fixed.
Storage class is now global
</commit_message>
<xml_diff>
--- a/assets/Localizations.xlsx
+++ b/assets/Localizations.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Graded\Graded - Flutter\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A145F7-5AB5-41A9-B9A0-D9821A60D4C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B48B4B07-F247-498F-9C3A-9157298C8D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="string" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0">string!$A$1:$B$116</definedName>
+    <definedName name="ExternalData_1" localSheetId="0">string!$A$1:$B$142</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="499">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="602">
   <si>
     <t>keys</t>
   </si>
@@ -208,21 +208,6 @@
     <t>Bonus:</t>
   </si>
   <si>
-    <t>chinese</t>
-  </si>
-  <si>
-    <t>Chinese</t>
-  </si>
-  <si>
-    <t>Chinois</t>
-  </si>
-  <si>
-    <t>Chinesisch</t>
-  </si>
-  <si>
-    <t>Chineesesch</t>
-  </si>
-  <si>
     <t>class_string</t>
   </si>
   <si>
@@ -544,18 +529,6 @@
     <t>Sprooch</t>
   </si>
   <si>
-    <t>latin</t>
-  </si>
-  <si>
-    <t>Latin</t>
-  </si>
-  <si>
-    <t>Lateinisch</t>
-  </si>
-  <si>
-    <t>Latäin</t>
-  </si>
-  <si>
     <t>licenses</t>
   </si>
   <si>
@@ -1520,6 +1493,342 @@
   </si>
   <si>
     <t>lb</t>
+  </si>
+  <si>
+    <t>L - Latin</t>
+  </si>
+  <si>
+    <t>L - Lateinisch</t>
+  </si>
+  <si>
+    <t>L - Latäin</t>
+  </si>
+  <si>
+    <t>ZH - Chinese</t>
+  </si>
+  <si>
+    <t>ZH - Chinois</t>
+  </si>
+  <si>
+    <t>ZH - Chinesisch</t>
+  </si>
+  <si>
+    <t>ZH - Chineesesch</t>
+  </si>
+  <si>
+    <t>section_general_gh</t>
+  </si>
+  <si>
+    <t>section_general_so</t>
+  </si>
+  <si>
+    <t>section_general_a3d</t>
+  </si>
+  <si>
+    <t>section_general_ig</t>
+  </si>
+  <si>
+    <t>section_general_sn</t>
+  </si>
+  <si>
+    <t>section_general_acv</t>
+  </si>
+  <si>
+    <t>section_general_cm</t>
+  </si>
+  <si>
+    <t>section_general_ps</t>
+  </si>
+  <si>
+    <t>section_general_cg</t>
+  </si>
+  <si>
+    <t>section_general_cc</t>
+  </si>
+  <si>
+    <t>section_general_cf</t>
+  </si>
+  <si>
+    <t>section_general_mm</t>
+  </si>
+  <si>
+    <t>section_general_ed</t>
+  </si>
+  <si>
+    <t>section_general_si</t>
+  </si>
+  <si>
+    <t>section_general_sh</t>
+  </si>
+  <si>
+    <t>section_general_in</t>
+  </si>
+  <si>
+    <t>section_general_se</t>
+  </si>
+  <si>
+    <t>variant_general_fr</t>
+  </si>
+  <si>
+    <t>variant_general_p</t>
+  </si>
+  <si>
+    <t>variant_general_ia</t>
+  </si>
+  <si>
+    <t>variant_general_if</t>
+  </si>
+  <si>
+    <t>variant_general_pf</t>
+  </si>
+  <si>
+    <t>variant_general_ad</t>
+  </si>
+  <si>
+    <t>variant_general_adf</t>
+  </si>
+  <si>
+    <t>variant_general_a</t>
+  </si>
+  <si>
+    <t>P - Voie de préparation</t>
+  </si>
+  <si>
+    <t>PF - Voie de préparation française</t>
+  </si>
+  <si>
+    <t>AD - Classe d'adaptation</t>
+  </si>
+  <si>
+    <t>ADF - Classe d'adaptation française</t>
+  </si>
+  <si>
+    <t>GH - Gestion de l'hospitalité</t>
+  </si>
+  <si>
+    <t>SO - Sciences sociales</t>
+  </si>
+  <si>
+    <t>A3D - Architecture, design et développement durable</t>
+  </si>
+  <si>
+    <t>IG - Ingénierie</t>
+  </si>
+  <si>
+    <t>SN - Sciences naturelles</t>
+  </si>
+  <si>
+    <t>ACV - Arts et communication visuelle</t>
+  </si>
+  <si>
+    <t>CM - Administratif et commercial</t>
+  </si>
+  <si>
+    <t>PS - Professions de santé et professions sociales</t>
+  </si>
+  <si>
+    <t>CG - Gestion</t>
+  </si>
+  <si>
+    <t>CC - Communication et organisation</t>
+  </si>
+  <si>
+    <t>CF - Finance</t>
+  </si>
+  <si>
+    <t>MM - Marketing, médias et communication</t>
+  </si>
+  <si>
+    <t>ED - Formation de l'éducateur</t>
+  </si>
+  <si>
+    <t>SI - Formation de l'infirmier</t>
+  </si>
+  <si>
+    <t>SH - Sciences de la santé</t>
+  </si>
+  <si>
+    <t>IN - Informatique</t>
+  </si>
+  <si>
+    <t>SE - Sciences environnementales</t>
+  </si>
+  <si>
+    <t>IF - Apprentissage du français</t>
+  </si>
+  <si>
+    <t>A - Continuation de l'allemand</t>
+  </si>
+  <si>
+    <t>F - Début de l'allemand</t>
+  </si>
+  <si>
+    <t>IA - Apprentissage de l'allemand</t>
+  </si>
+  <si>
+    <t>FR - Régime francophone</t>
+  </si>
+  <si>
+    <t>variant_general_f</t>
+  </si>
+  <si>
+    <t>GH - Hospitality Management</t>
+  </si>
+  <si>
+    <t>A3D - Architecture, design and sustainable development</t>
+  </si>
+  <si>
+    <t>IG - Engineering</t>
+  </si>
+  <si>
+    <t>IN - Informatics</t>
+  </si>
+  <si>
+    <t>P - Preparation route</t>
+  </si>
+  <si>
+    <t>PF - French Preparation Way</t>
+  </si>
+  <si>
+    <t>ADF - French adaptation class</t>
+  </si>
+  <si>
+    <t>SO - Sozialwissenschaften</t>
+  </si>
+  <si>
+    <t>A3D - Architektur, Design und nachhaltige Entwicklung</t>
+  </si>
+  <si>
+    <t>IG - Ingenieurwesen</t>
+  </si>
+  <si>
+    <t>SN - Naturwissenschaften</t>
+  </si>
+  <si>
+    <t>CM - Verwaltung und Handel</t>
+  </si>
+  <si>
+    <t>PS - Gesundheits- und Sozialberufe</t>
+  </si>
+  <si>
+    <t>CC - Kommunikation und Organisation</t>
+  </si>
+  <si>
+    <t>CF - Finanzen</t>
+  </si>
+  <si>
+    <t>MM - Marketing, Medien und Kommunikation</t>
+  </si>
+  <si>
+    <t>ED - Pädagogenausbildung</t>
+  </si>
+  <si>
+    <t>SI - Ausbildung zur Krankenschwester</t>
+  </si>
+  <si>
+    <t>SH - Gesundheitswissenschaften</t>
+  </si>
+  <si>
+    <t>IN - Informatik</t>
+  </si>
+  <si>
+    <t>SE - Umweltwissenschaften</t>
+  </si>
+  <si>
+    <t>P - Vorbereitungsweg</t>
+  </si>
+  <si>
+    <t>IA - Deutsch lernen</t>
+  </si>
+  <si>
+    <t>IF - Französisch lernen</t>
+  </si>
+  <si>
+    <t>AD - Anpassungsklasse</t>
+  </si>
+  <si>
+    <t>ADF - Französische Anpassungsklasse</t>
+  </si>
+  <si>
+    <t>A - Fortsetzung des Deutschen</t>
+  </si>
+  <si>
+    <t>F - Beginn des Deutschen</t>
+  </si>
+  <si>
+    <t>//TODO</t>
+  </si>
+  <si>
+    <t>variant_classic_l</t>
+  </si>
+  <si>
+    <t>variant_classic_zh</t>
+  </si>
+  <si>
+    <t>CC - Communication and organization</t>
+  </si>
+  <si>
+    <t>CM - Administrative and commercial</t>
+  </si>
+  <si>
+    <t>ED - Educator training</t>
+  </si>
+  <si>
+    <t>GH - Hospitality management</t>
+  </si>
+  <si>
+    <t>MM - Marketing, media and communication</t>
+  </si>
+  <si>
+    <t>PS - Health and social professions</t>
+  </si>
+  <si>
+    <t>SE - Environmental sciences</t>
+  </si>
+  <si>
+    <t>SH - Health sciences</t>
+  </si>
+  <si>
+    <t>SI - Nurse training</t>
+  </si>
+  <si>
+    <t>SN - Natural sciences</t>
+  </si>
+  <si>
+    <t>SO - Social sciences</t>
+  </si>
+  <si>
+    <t>ACV - Arts and visual communication</t>
+  </si>
+  <si>
+    <t>ACV - Kunst und visuelle Kommunikation</t>
+  </si>
+  <si>
+    <t>CG - Management</t>
+  </si>
+  <si>
+    <t>A - Continuation of german</t>
+  </si>
+  <si>
+    <t>AD - Adaptation class</t>
+  </si>
+  <si>
+    <t>F - Beginning of german</t>
+  </si>
+  <si>
+    <t>IA - Learning german</t>
+  </si>
+  <si>
+    <t>IF - Learning french</t>
+  </si>
+  <si>
+    <t>PF - French preparation way</t>
+  </si>
+  <si>
+    <t>FR - Francophone regime</t>
+  </si>
+  <si>
+    <t>FR - Frankophones Regime</t>
   </si>
 </sst>
 </file>
@@ -1595,10 +1904,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="string" displayName="string" ref="A1:E116" totalsRowShown="0">
-  <autoFilter ref="A1:E116" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E116">
-    <sortCondition ref="A1:A116"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="string" displayName="string" ref="A1:E142" totalsRowShown="0">
+  <autoFilter ref="A1:E142" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E142">
+    <sortCondition ref="A1:A142"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="keys"/>
@@ -1899,13 +2208,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E116"/>
+  <dimension ref="A1:E142"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="A126" workbookViewId="0">
+      <selection activeCell="D132" sqref="D132"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.85546875" bestFit="1" customWidth="1"/>
@@ -1928,7 +2237,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>498</v>
+        <v>489</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1953,16 +2262,16 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>440</v>
+        <v>431</v>
       </c>
       <c r="C3" t="s">
-        <v>439</v>
+        <v>430</v>
       </c>
       <c r="D3" t="s">
-        <v>441</v>
+        <v>432</v>
       </c>
       <c r="E3" t="s">
-        <v>442</v>
+        <v>433</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1984,19 +2293,19 @@
     </row>
     <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>484</v>
+        <v>475</v>
       </c>
       <c r="B5" t="s">
-        <v>483</v>
+        <v>474</v>
       </c>
       <c r="C5" t="s">
-        <v>485</v>
+        <v>476</v>
       </c>
       <c r="D5" t="s">
-        <v>486</v>
+        <v>477</v>
       </c>
       <c r="E5" t="s">
-        <v>487</v>
+        <v>478</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2055,16 +2364,16 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>454</v>
+        <v>445</v>
       </c>
       <c r="C9" t="s">
-        <v>454</v>
+        <v>445</v>
       </c>
       <c r="D9" t="s">
-        <v>454</v>
+        <v>445</v>
       </c>
       <c r="E9" t="s">
-        <v>454</v>
+        <v>445</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2075,7 +2384,7 @@
         <v>44</v>
       </c>
       <c r="C10" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="D10" t="s">
         <v>45</v>
@@ -2171,53 +2480,53 @@
     </row>
     <row r="16" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>443</v>
+        <v>434</v>
       </c>
       <c r="B16" t="s">
-        <v>444</v>
+        <v>435</v>
       </c>
       <c r="C16" t="s">
-        <v>445</v>
+        <v>436</v>
       </c>
       <c r="D16" t="s">
-        <v>446</v>
+        <v>437</v>
       </c>
       <c r="E16" t="s">
-        <v>447</v>
+        <v>438</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>365</v>
+        <v>356</v>
       </c>
       <c r="B17" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="C17" t="s">
-        <v>368</v>
+        <v>359</v>
       </c>
       <c r="D17" t="s">
-        <v>370</v>
+        <v>361</v>
       </c>
       <c r="E17" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="B18" t="s">
+        <v>363</v>
+      </c>
+      <c r="C18" t="s">
+        <v>362</v>
+      </c>
+      <c r="D18" t="s">
+        <v>364</v>
+      </c>
+      <c r="E18" t="s">
         <v>372</v>
-      </c>
-      <c r="C18" t="s">
-        <v>371</v>
-      </c>
-      <c r="D18" t="s">
-        <v>373</v>
-      </c>
-      <c r="E18" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2239,104 +2548,104 @@
     </row>
     <row r="20" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>66</v>
+        <v>308</v>
       </c>
       <c r="B20" t="s">
-        <v>67</v>
+        <v>309</v>
       </c>
       <c r="C20" t="s">
-        <v>68</v>
+        <v>310</v>
       </c>
       <c r="D20" t="s">
-        <v>69</v>
+        <v>311</v>
       </c>
       <c r="E20" t="s">
-        <v>70</v>
+        <v>311</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>317</v>
+        <v>66</v>
       </c>
       <c r="B21" t="s">
-        <v>318</v>
+        <v>67</v>
       </c>
       <c r="C21" t="s">
-        <v>319</v>
+        <v>67</v>
       </c>
       <c r="D21" t="s">
-        <v>320</v>
+        <v>68</v>
       </c>
       <c r="E21" t="s">
-        <v>320</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" t="s">
+        <v>70</v>
+      </c>
+      <c r="D22" t="s">
         <v>71</v>
       </c>
-      <c r="B22" t="s">
-        <v>72</v>
-      </c>
-      <c r="C22" t="s">
-        <v>72</v>
-      </c>
-      <c r="D22" t="s">
-        <v>73</v>
-      </c>
       <c r="E22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" t="s">
+        <v>73</v>
+      </c>
+      <c r="D23" t="s">
         <v>74</v>
       </c>
-      <c r="B23" t="s">
+      <c r="E23" t="s">
         <v>75</v>
-      </c>
-      <c r="C23" t="s">
-        <v>75</v>
-      </c>
-      <c r="D23" t="s">
-        <v>76</v>
-      </c>
-      <c r="E23" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>77</v>
+        <v>453</v>
       </c>
       <c r="B24" t="s">
-        <v>78</v>
+        <v>454</v>
       </c>
       <c r="C24" t="s">
-        <v>78</v>
+        <v>456</v>
       </c>
       <c r="D24" t="s">
-        <v>79</v>
-      </c>
-      <c r="E24" t="s">
-        <v>80</v>
+        <v>455</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>462</v>
+        <v>76</v>
       </c>
       <c r="B25" t="s">
-        <v>463</v>
+        <v>77</v>
       </c>
       <c r="C25" t="s">
-        <v>465</v>
+        <v>78</v>
       </c>
       <c r="D25" t="s">
-        <v>464</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>466</v>
+        <v>79</v>
+      </c>
+      <c r="E25" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2370,21 +2679,21 @@
         <v>89</v>
       </c>
       <c r="E27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>90</v>
+      </c>
+      <c r="B28" t="s">
         <v>91</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>92</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>93</v>
-      </c>
-      <c r="D28" t="s">
-        <v>94</v>
       </c>
       <c r="E28" t="s">
         <v>94</v>
@@ -2418,27 +2727,27 @@
         <v>102</v>
       </c>
       <c r="D30" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E30" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>103</v>
+      </c>
+      <c r="B31" t="s">
+        <v>104</v>
+      </c>
+      <c r="C31" t="s">
         <v>105</v>
-      </c>
-      <c r="B31" t="s">
-        <v>106</v>
-      </c>
-      <c r="C31" t="s">
-        <v>107</v>
       </c>
       <c r="D31" t="s">
         <v>106</v>
       </c>
       <c r="E31" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2477,36 +2786,36 @@
     </row>
     <row r="34" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>118</v>
+        <v>479</v>
       </c>
       <c r="B34" t="s">
-        <v>119</v>
+        <v>480</v>
       </c>
       <c r="C34" t="s">
-        <v>120</v>
+        <v>481</v>
       </c>
       <c r="D34" t="s">
-        <v>121</v>
+        <v>482</v>
       </c>
       <c r="E34" t="s">
-        <v>122</v>
+        <v>483</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>488</v>
+        <v>118</v>
       </c>
       <c r="B35" t="s">
-        <v>489</v>
+        <v>119</v>
       </c>
       <c r="C35" t="s">
-        <v>490</v>
+        <v>120</v>
       </c>
       <c r="D35" t="s">
-        <v>491</v>
+        <v>121</v>
       </c>
       <c r="E35" t="s">
-        <v>492</v>
+        <v>122</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2540,239 +2849,239 @@
         <v>131</v>
       </c>
       <c r="E37" t="s">
-        <v>132</v>
+        <v>373</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>132</v>
+      </c>
+      <c r="B38" t="s">
         <v>133</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>134</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>135</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>136</v>
-      </c>
-      <c r="E38" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>137</v>
-      </c>
-      <c r="B39" t="s">
-        <v>138</v>
-      </c>
-      <c r="C39" t="s">
-        <v>139</v>
-      </c>
-      <c r="D39" t="s">
-        <v>140</v>
-      </c>
-      <c r="E39" t="s">
-        <v>141</v>
+        <v>17</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>447</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>17</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>456</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>456</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>456</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>456</v>
+        <v>9</v>
+      </c>
+      <c r="B40" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>9</v>
+        <v>458</v>
       </c>
       <c r="B41" t="s">
-        <v>10</v>
+        <v>459</v>
       </c>
       <c r="C41" t="s">
-        <v>10</v>
+        <v>460</v>
       </c>
       <c r="D41" t="s">
-        <v>10</v>
+        <v>461</v>
       </c>
       <c r="E41" t="s">
-        <v>10</v>
+        <v>462</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="B42" t="s">
         <v>468</v>
       </c>
       <c r="C42" t="s">
-        <v>469</v>
+        <v>472</v>
       </c>
       <c r="D42" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="E42" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>482</v>
+        <v>469</v>
       </c>
       <c r="B43" t="s">
-        <v>477</v>
+        <v>470</v>
       </c>
       <c r="C43" t="s">
-        <v>481</v>
+        <v>471</v>
       </c>
       <c r="D43" t="s">
-        <v>481</v>
+        <v>472</v>
       </c>
       <c r="E43" t="s">
-        <v>481</v>
+        <v>472</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>478</v>
+        <v>13</v>
       </c>
       <c r="B44" t="s">
-        <v>479</v>
+        <v>14</v>
       </c>
       <c r="C44" t="s">
-        <v>480</v>
+        <v>14</v>
       </c>
       <c r="D44" t="s">
-        <v>481</v>
+        <v>14</v>
       </c>
       <c r="E44" t="s">
-        <v>481</v>
+        <v>14</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>13</v>
+        <v>137</v>
       </c>
       <c r="B45" t="s">
-        <v>14</v>
+        <v>138</v>
       </c>
       <c r="C45" t="s">
-        <v>14</v>
+        <v>139</v>
       </c>
       <c r="D45" t="s">
-        <v>14</v>
+        <v>138</v>
       </c>
       <c r="E45" t="s">
-        <v>14</v>
+        <v>138</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>142</v>
+        <v>448</v>
       </c>
       <c r="B46" t="s">
-        <v>143</v>
+        <v>449</v>
       </c>
       <c r="C46" t="s">
-        <v>144</v>
+        <v>450</v>
       </c>
       <c r="D46" t="s">
-        <v>143</v>
-      </c>
-      <c r="E46" t="s">
-        <v>143</v>
+        <v>451</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>452</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>457</v>
+        <v>11</v>
       </c>
       <c r="B47" t="s">
-        <v>458</v>
+        <v>12</v>
       </c>
       <c r="C47" t="s">
-        <v>459</v>
+        <v>12</v>
       </c>
       <c r="D47" t="s">
-        <v>460</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>461</v>
+        <v>12</v>
+      </c>
+      <c r="E47" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>11</v>
+        <v>140</v>
       </c>
       <c r="B48" t="s">
-        <v>12</v>
+        <v>141</v>
       </c>
       <c r="C48" t="s">
-        <v>12</v>
+        <v>142</v>
       </c>
       <c r="D48" t="s">
-        <v>12</v>
+        <v>143</v>
       </c>
       <c r="E48" t="s">
-        <v>12</v>
+        <v>143</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>145</v>
-      </c>
-      <c r="B49" t="s">
-        <v>146</v>
-      </c>
-      <c r="C49" t="s">
-        <v>147</v>
-      </c>
-      <c r="D49" t="s">
-        <v>148</v>
-      </c>
-      <c r="E49" t="s">
-        <v>148</v>
+        <v>8</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>8</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>455</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>455</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>455</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>455</v>
+        <v>144</v>
+      </c>
+      <c r="B50" t="s">
+        <v>145</v>
+      </c>
+      <c r="C50" t="s">
+        <v>146</v>
+      </c>
+      <c r="D50" t="s">
+        <v>146</v>
+      </c>
+      <c r="E50" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>148</v>
+      </c>
+      <c r="B51" t="s">
         <v>149</v>
       </c>
-      <c r="B51" t="s">
+      <c r="C51" t="s">
         <v>150</v>
-      </c>
-      <c r="C51" t="s">
-        <v>151</v>
       </c>
       <c r="D51" t="s">
         <v>151</v>
@@ -2783,36 +3092,36 @@
     </row>
     <row r="52" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>153</v>
+        <v>484</v>
       </c>
       <c r="B52" t="s">
-        <v>154</v>
+        <v>485</v>
       </c>
       <c r="C52" t="s">
-        <v>155</v>
+        <v>486</v>
       </c>
       <c r="D52" t="s">
-        <v>156</v>
+        <v>487</v>
       </c>
       <c r="E52" t="s">
-        <v>157</v>
+        <v>488</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>493</v>
+        <v>153</v>
       </c>
       <c r="B53" t="s">
-        <v>494</v>
+        <v>154</v>
       </c>
       <c r="C53" t="s">
-        <v>495</v>
+        <v>155</v>
       </c>
       <c r="D53" t="s">
-        <v>496</v>
+        <v>156</v>
       </c>
       <c r="E53" t="s">
-        <v>497</v>
+        <v>157</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2834,36 +3143,36 @@
     </row>
     <row r="55" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>163</v>
+        <v>405</v>
       </c>
       <c r="B55" t="s">
-        <v>164</v>
+        <v>404</v>
       </c>
       <c r="C55" t="s">
-        <v>165</v>
+        <v>406</v>
       </c>
       <c r="D55" t="s">
-        <v>166</v>
+        <v>407</v>
       </c>
       <c r="E55" t="s">
-        <v>167</v>
+        <v>408</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>414</v>
+        <v>163</v>
       </c>
       <c r="B56" t="s">
-        <v>413</v>
+        <v>164</v>
       </c>
       <c r="C56" t="s">
-        <v>415</v>
+        <v>165</v>
       </c>
       <c r="D56" t="s">
-        <v>416</v>
+        <v>166</v>
       </c>
       <c r="E56" t="s">
-        <v>417</v>
+        <v>167</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2874,234 +3183,234 @@
         <v>169</v>
       </c>
       <c r="C57" t="s">
+        <v>169</v>
+      </c>
+      <c r="D57" t="s">
         <v>170</v>
       </c>
-      <c r="D57" t="s">
-        <v>171</v>
-      </c>
       <c r="E57" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>171</v>
+      </c>
+      <c r="B58" t="s">
+        <v>172</v>
+      </c>
+      <c r="C58" t="s">
         <v>173</v>
       </c>
-      <c r="B58" t="s">
+      <c r="D58" t="s">
         <v>174</v>
       </c>
-      <c r="C58" t="s">
-        <v>174</v>
-      </c>
-      <c r="D58" t="s">
+      <c r="E58" t="s">
         <v>175</v>
-      </c>
-      <c r="E58" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>177</v>
+        <v>15</v>
       </c>
       <c r="B59" t="s">
-        <v>178</v>
+        <v>16</v>
       </c>
       <c r="C59" t="s">
-        <v>178</v>
+        <v>16</v>
       </c>
       <c r="D59" t="s">
-        <v>179</v>
+        <v>16</v>
       </c>
       <c r="E59" t="s">
-        <v>179</v>
+        <v>16</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>180</v>
+        <v>296</v>
       </c>
       <c r="B60" t="s">
-        <v>181</v>
+        <v>297</v>
       </c>
       <c r="C60" t="s">
-        <v>182</v>
+        <v>297</v>
       </c>
       <c r="D60" t="s">
-        <v>183</v>
+        <v>297</v>
       </c>
       <c r="E60" t="s">
-        <v>184</v>
+        <v>297</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>15</v>
+        <v>298</v>
       </c>
       <c r="B61" t="s">
-        <v>16</v>
+        <v>299</v>
       </c>
       <c r="C61" t="s">
-        <v>16</v>
+        <v>300</v>
       </c>
       <c r="D61" t="s">
-        <v>16</v>
+        <v>301</v>
       </c>
       <c r="E61" t="s">
-        <v>16</v>
+        <v>302</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>305</v>
+        <v>292</v>
       </c>
       <c r="B62" t="s">
-        <v>306</v>
+        <v>293</v>
       </c>
       <c r="C62" t="s">
-        <v>306</v>
+        <v>294</v>
       </c>
       <c r="D62" t="s">
-        <v>306</v>
+        <v>293</v>
       </c>
       <c r="E62" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>307</v>
+        <v>176</v>
       </c>
       <c r="B63" t="s">
-        <v>308</v>
+        <v>177</v>
       </c>
       <c r="C63" t="s">
-        <v>309</v>
+        <v>178</v>
       </c>
       <c r="D63" t="s">
-        <v>310</v>
+        <v>179</v>
       </c>
       <c r="E63" t="s">
-        <v>311</v>
+        <v>180</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>301</v>
+        <v>347</v>
       </c>
       <c r="B64" t="s">
-        <v>302</v>
+        <v>349</v>
       </c>
       <c r="C64" t="s">
-        <v>303</v>
+        <v>351</v>
       </c>
       <c r="D64" t="s">
-        <v>302</v>
+        <v>353</v>
       </c>
       <c r="E64" t="s">
-        <v>304</v>
+        <v>355</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>185</v>
+        <v>303</v>
       </c>
       <c r="B65" t="s">
-        <v>186</v>
+        <v>304</v>
       </c>
       <c r="C65" t="s">
-        <v>187</v>
+        <v>305</v>
       </c>
       <c r="D65" t="s">
-        <v>188</v>
+        <v>306</v>
       </c>
       <c r="E65" t="s">
-        <v>189</v>
+        <v>307</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>356</v>
+        <v>181</v>
       </c>
       <c r="B66" t="s">
-        <v>358</v>
+        <v>182</v>
       </c>
       <c r="C66" t="s">
-        <v>360</v>
+        <v>182</v>
       </c>
       <c r="D66" t="s">
-        <v>362</v>
+        <v>183</v>
       </c>
       <c r="E66" t="s">
-        <v>364</v>
+        <v>184</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>312</v>
+        <v>185</v>
       </c>
       <c r="B67" t="s">
-        <v>313</v>
+        <v>366</v>
       </c>
       <c r="C67" t="s">
-        <v>314</v>
+        <v>367</v>
       </c>
       <c r="D67" t="s">
-        <v>315</v>
+        <v>368</v>
       </c>
       <c r="E67" t="s">
-        <v>316</v>
+        <v>375</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>190</v>
+        <v>365</v>
       </c>
       <c r="B68" t="s">
-        <v>191</v>
+        <v>439</v>
       </c>
       <c r="C68" t="s">
-        <v>191</v>
+        <v>439</v>
       </c>
       <c r="D68" t="s">
-        <v>192</v>
+        <v>439</v>
       </c>
       <c r="E68" t="s">
-        <v>193</v>
+        <v>439</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="B69" t="s">
-        <v>375</v>
+        <v>187</v>
       </c>
       <c r="C69" t="s">
-        <v>376</v>
+        <v>188</v>
       </c>
       <c r="D69" t="s">
-        <v>377</v>
+        <v>189</v>
       </c>
       <c r="E69" t="s">
-        <v>384</v>
+        <v>189</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>374</v>
+        <v>190</v>
       </c>
       <c r="B70" t="s">
-        <v>448</v>
+        <v>191</v>
       </c>
       <c r="C70" t="s">
-        <v>448</v>
+        <v>192</v>
       </c>
       <c r="D70" t="s">
-        <v>448</v>
+        <v>193</v>
       </c>
       <c r="E70" t="s">
-        <v>448</v>
+        <v>194</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3118,781 +3427,1223 @@
         <v>198</v>
       </c>
       <c r="E71" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B72" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C72" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D72" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E72" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B73" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C73" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D73" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E73" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B74" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C74" t="s">
-        <v>211</v>
+        <v>370</v>
       </c>
       <c r="D74" t="s">
         <v>212</v>
       </c>
       <c r="E74" t="s">
-        <v>213</v>
+        <v>376</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
+        <v>213</v>
+      </c>
+      <c r="B75" t="s">
         <v>214</v>
       </c>
-      <c r="B75" t="s">
+      <c r="C75" t="s">
         <v>215</v>
       </c>
-      <c r="C75" t="s">
+      <c r="D75" t="s">
         <v>216</v>
       </c>
-      <c r="D75" t="s">
+      <c r="E75" t="s">
         <v>217</v>
-      </c>
-      <c r="E75" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
+        <v>218</v>
+      </c>
+      <c r="B76" t="s">
         <v>219</v>
       </c>
-      <c r="B76" t="s">
+      <c r="C76" t="s">
         <v>220</v>
-      </c>
-      <c r="C76" t="s">
-        <v>379</v>
       </c>
       <c r="D76" t="s">
         <v>221</v>
       </c>
       <c r="E76" t="s">
-        <v>385</v>
+        <v>222</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>222</v>
+        <v>440</v>
       </c>
       <c r="B77" t="s">
-        <v>223</v>
+        <v>441</v>
       </c>
       <c r="C77" t="s">
-        <v>224</v>
+        <v>442</v>
       </c>
       <c r="D77" t="s">
-        <v>225</v>
+        <v>443</v>
       </c>
       <c r="E77" t="s">
-        <v>226</v>
+        <v>444</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
+        <v>223</v>
+      </c>
+      <c r="B78" t="s">
+        <v>224</v>
+      </c>
+      <c r="C78" t="s">
+        <v>225</v>
+      </c>
+      <c r="D78" t="s">
+        <v>226</v>
+      </c>
+      <c r="E78" t="s">
         <v>227</v>
-      </c>
-      <c r="B78" t="s">
-        <v>228</v>
-      </c>
-      <c r="C78" t="s">
-        <v>229</v>
-      </c>
-      <c r="D78" t="s">
-        <v>230</v>
-      </c>
-      <c r="E78" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>449</v>
+        <v>312</v>
       </c>
       <c r="B79" t="s">
-        <v>450</v>
+        <v>313</v>
       </c>
       <c r="C79" t="s">
-        <v>451</v>
+        <v>313</v>
       </c>
       <c r="D79" t="s">
-        <v>452</v>
+        <v>463</v>
       </c>
       <c r="E79" t="s">
-        <v>453</v>
+        <v>314</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>232</v>
+        <v>395</v>
       </c>
       <c r="B80" t="s">
-        <v>233</v>
+        <v>315</v>
       </c>
       <c r="C80" t="s">
-        <v>234</v>
+        <v>322</v>
       </c>
       <c r="D80" t="s">
-        <v>235</v>
+        <v>330</v>
       </c>
       <c r="E80" t="s">
-        <v>236</v>
+        <v>339</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>321</v>
+        <v>397</v>
       </c>
       <c r="B81" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="C81" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="D81" t="s">
-        <v>472</v>
+        <v>331</v>
       </c>
       <c r="E81" t="s">
-        <v>323</v>
+        <v>331</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="B82" t="s">
+        <v>321</v>
+      </c>
+      <c r="C82" t="s">
         <v>324</v>
       </c>
-      <c r="C82" t="s">
-        <v>331</v>
-      </c>
       <c r="D82" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="E82" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="B83" t="s">
+        <v>319</v>
+      </c>
+      <c r="C83" t="s">
         <v>325</v>
       </c>
-      <c r="C83" t="s">
-        <v>332</v>
-      </c>
       <c r="D83" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="E83" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="B84" t="s">
-        <v>330</v>
+        <v>317</v>
       </c>
       <c r="C84" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="D84" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
       <c r="E84" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
       <c r="B85" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
       <c r="C85" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="D85" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="E85" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
       <c r="B86" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="C86" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="D86" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="E86" t="s">
-        <v>349</v>
+        <v>374</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
+        <v>402</v>
+      </c>
+      <c r="B87" t="s">
         <v>409</v>
       </c>
-      <c r="B87" t="s">
-        <v>327</v>
-      </c>
       <c r="C87" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="D87" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="E87" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
+        <v>499</v>
+      </c>
+      <c r="B88" t="s">
+        <v>550</v>
+      </c>
+      <c r="C88" t="s">
+        <v>528</v>
+      </c>
+      <c r="D88" t="s">
+        <v>557</v>
+      </c>
+      <c r="E88" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>502</v>
+      </c>
+      <c r="B89" t="s">
+        <v>591</v>
+      </c>
+      <c r="C89" t="s">
+        <v>531</v>
+      </c>
+      <c r="D89" t="s">
+        <v>592</v>
+      </c>
+      <c r="E89" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>506</v>
+      </c>
+      <c r="B90" t="s">
+        <v>580</v>
+      </c>
+      <c r="C90" t="s">
+        <v>535</v>
+      </c>
+      <c r="D90" t="s">
+        <v>562</v>
+      </c>
+      <c r="E90" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>507</v>
+      </c>
+      <c r="B91" t="s">
+        <v>536</v>
+      </c>
+      <c r="C91" t="s">
+        <v>536</v>
+      </c>
+      <c r="D91" t="s">
+        <v>563</v>
+      </c>
+      <c r="E91" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>505</v>
+      </c>
+      <c r="B92" t="s">
+        <v>593</v>
+      </c>
+      <c r="C92" t="s">
+        <v>534</v>
+      </c>
+      <c r="D92" t="s">
+        <v>593</v>
+      </c>
+      <c r="E92" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>503</v>
+      </c>
+      <c r="B93" t="s">
+        <v>581</v>
+      </c>
+      <c r="C93" t="s">
+        <v>532</v>
+      </c>
+      <c r="D93" t="s">
+        <v>560</v>
+      </c>
+      <c r="E93" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>509</v>
+      </c>
+      <c r="B94" t="s">
+        <v>582</v>
+      </c>
+      <c r="C94" t="s">
+        <v>538</v>
+      </c>
+      <c r="D94" t="s">
+        <v>565</v>
+      </c>
+      <c r="E94" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>497</v>
+      </c>
+      <c r="B95" t="s">
+        <v>583</v>
+      </c>
+      <c r="C95" t="s">
+        <v>526</v>
+      </c>
+      <c r="D95" t="s">
+        <v>549</v>
+      </c>
+      <c r="E95" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>500</v>
+      </c>
+      <c r="B96" t="s">
+        <v>551</v>
+      </c>
+      <c r="C96" t="s">
+        <v>529</v>
+      </c>
+      <c r="D96" t="s">
+        <v>558</v>
+      </c>
+      <c r="E96" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>512</v>
+      </c>
+      <c r="B97" t="s">
+        <v>552</v>
+      </c>
+      <c r="C97" t="s">
+        <v>541</v>
+      </c>
+      <c r="D97" t="s">
+        <v>568</v>
+      </c>
+      <c r="E97" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>508</v>
+      </c>
+      <c r="B98" t="s">
+        <v>584</v>
+      </c>
+      <c r="C98" t="s">
+        <v>537</v>
+      </c>
+      <c r="D98" t="s">
+        <v>564</v>
+      </c>
+      <c r="E98" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>504</v>
+      </c>
+      <c r="B99" t="s">
+        <v>585</v>
+      </c>
+      <c r="C99" t="s">
+        <v>533</v>
+      </c>
+      <c r="D99" t="s">
+        <v>561</v>
+      </c>
+      <c r="E99" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>513</v>
+      </c>
+      <c r="B100" t="s">
+        <v>586</v>
+      </c>
+      <c r="C100" t="s">
+        <v>542</v>
+      </c>
+      <c r="D100" t="s">
+        <v>569</v>
+      </c>
+      <c r="E100" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>511</v>
+      </c>
+      <c r="B101" t="s">
+        <v>587</v>
+      </c>
+      <c r="C101" t="s">
+        <v>540</v>
+      </c>
+      <c r="D101" t="s">
+        <v>567</v>
+      </c>
+      <c r="E101" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>510</v>
+      </c>
+      <c r="B102" t="s">
+        <v>588</v>
+      </c>
+      <c r="C102" t="s">
+        <v>539</v>
+      </c>
+      <c r="D102" t="s">
+        <v>566</v>
+      </c>
+      <c r="E102" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>501</v>
+      </c>
+      <c r="B103" t="s">
+        <v>589</v>
+      </c>
+      <c r="C103" t="s">
+        <v>530</v>
+      </c>
+      <c r="D103" t="s">
+        <v>559</v>
+      </c>
+      <c r="E103" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>498</v>
+      </c>
+      <c r="B104" t="s">
+        <v>590</v>
+      </c>
+      <c r="C104" t="s">
+        <v>527</v>
+      </c>
+      <c r="D104" t="s">
+        <v>556</v>
+      </c>
+      <c r="E104" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>228</v>
+      </c>
+      <c r="B105" t="s">
+        <v>229</v>
+      </c>
+      <c r="C105" t="s">
+        <v>230</v>
+      </c>
+      <c r="D105" t="s">
+        <v>231</v>
+      </c>
+      <c r="E105" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>466</v>
+      </c>
+      <c r="B106" t="s">
+        <v>236</v>
+      </c>
+      <c r="C106" t="s">
+        <v>467</v>
+      </c>
+      <c r="D106" t="s">
+        <v>236</v>
+      </c>
+      <c r="E106" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>233</v>
+      </c>
+      <c r="B107" t="s">
+        <v>234</v>
+      </c>
+      <c r="C107" t="s">
+        <v>235</v>
+      </c>
+      <c r="D107" t="s">
+        <v>236</v>
+      </c>
+      <c r="E107" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>237</v>
+      </c>
+      <c r="B108" t="s">
+        <v>238</v>
+      </c>
+      <c r="C108" t="s">
+        <v>239</v>
+      </c>
+      <c r="D108" t="s">
+        <v>240</v>
+      </c>
+      <c r="E108" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>242</v>
+      </c>
+      <c r="B109" t="s">
+        <v>243</v>
+      </c>
+      <c r="C109" t="s">
+        <v>244</v>
+      </c>
+      <c r="D109" t="s">
+        <v>245</v>
+      </c>
+      <c r="E109" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>247</v>
+      </c>
+      <c r="B110" t="s">
+        <v>248</v>
+      </c>
+      <c r="C110" t="s">
+        <v>249</v>
+      </c>
+      <c r="D110" t="s">
+        <v>250</v>
+      </c>
+      <c r="E110" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>415</v>
+      </c>
+      <c r="B111" t="s">
+        <v>416</v>
+      </c>
+      <c r="C111" t="s">
+        <v>417</v>
+      </c>
+      <c r="D111" t="s">
+        <v>418</v>
+      </c>
+      <c r="E111" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>252</v>
+      </c>
+      <c r="B112" t="s">
+        <v>253</v>
+      </c>
+      <c r="C112" t="s">
+        <v>254</v>
+      </c>
+      <c r="D112" t="s">
+        <v>255</v>
+      </c>
+      <c r="E112" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>343</v>
+      </c>
+      <c r="B113" t="s">
+        <v>344</v>
+      </c>
+      <c r="C113" t="s">
+        <v>345</v>
+      </c>
+      <c r="D113" t="s">
+        <v>344</v>
+      </c>
+      <c r="E113" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
         <v>410</v>
       </c>
-      <c r="B88" t="s">
-        <v>329</v>
-      </c>
-      <c r="C88" t="s">
-        <v>337</v>
-      </c>
-      <c r="D88" t="s">
-        <v>345</v>
-      </c>
-      <c r="E88" t="s">
+      <c r="B114" t="s">
+        <v>411</v>
+      </c>
+      <c r="C114" t="s">
+        <v>412</v>
+      </c>
+      <c r="D114" t="s">
+        <v>413</v>
+      </c>
+      <c r="E114" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>256</v>
+      </c>
+      <c r="B115" t="s">
+        <v>257</v>
+      </c>
+      <c r="C115" t="s">
+        <v>258</v>
+      </c>
+      <c r="D115" t="s">
+        <v>259</v>
+      </c>
+      <c r="E115" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>260</v>
+      </c>
+      <c r="B116" t="s">
+        <v>261</v>
+      </c>
+      <c r="C116" t="s">
+        <v>262</v>
+      </c>
+      <c r="D116" t="s">
+        <v>263</v>
+      </c>
+      <c r="E116" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>391</v>
+      </c>
+      <c r="B117" t="s">
+        <v>392</v>
+      </c>
+      <c r="C117" t="s">
+        <v>393</v>
+      </c>
+      <c r="D117" t="s">
+        <v>394</v>
+      </c>
+      <c r="E117" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>378</v>
+      </c>
+      <c r="B118" t="s">
+        <v>387</v>
+      </c>
+      <c r="C118" t="s">
+        <v>388</v>
+      </c>
+      <c r="D118" t="s">
+        <v>389</v>
+      </c>
+      <c r="E118" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>377</v>
+      </c>
+      <c r="B119" t="s">
+        <v>384</v>
+      </c>
+      <c r="C119" t="s">
+        <v>385</v>
+      </c>
+      <c r="D119" t="s">
+        <v>386</v>
+      </c>
+      <c r="E119" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>380</v>
+      </c>
+      <c r="B120" t="s">
+        <v>379</v>
+      </c>
+      <c r="C120" t="s">
+        <v>381</v>
+      </c>
+      <c r="D120" t="s">
+        <v>382</v>
+      </c>
+      <c r="E120" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>411</v>
-      </c>
-      <c r="B89" t="s">
-        <v>418</v>
-      </c>
-      <c r="C89" t="s">
-        <v>338</v>
-      </c>
-      <c r="D89" t="s">
+    <row r="121" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>264</v>
+      </c>
+      <c r="B121" t="s">
+        <v>265</v>
+      </c>
+      <c r="C121" t="s">
+        <v>266</v>
+      </c>
+      <c r="D121" t="s">
+        <v>267</v>
+      </c>
+      <c r="E121" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>268</v>
+      </c>
+      <c r="B122" t="s">
+        <v>269</v>
+      </c>
+      <c r="C122" t="s">
+        <v>270</v>
+      </c>
+      <c r="D122" t="s">
+        <v>271</v>
+      </c>
+      <c r="E122" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>272</v>
+      </c>
+      <c r="B123" t="s">
+        <v>273</v>
+      </c>
+      <c r="C123" t="s">
+        <v>371</v>
+      </c>
+      <c r="D123" t="s">
+        <v>403</v>
+      </c>
+      <c r="E123" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>464</v>
+      </c>
+      <c r="B124" t="s">
+        <v>278</v>
+      </c>
+      <c r="C124" t="s">
+        <v>465</v>
+      </c>
+      <c r="D124" t="s">
+        <v>278</v>
+      </c>
+      <c r="E124" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>275</v>
+      </c>
+      <c r="B125" t="s">
+        <v>276</v>
+      </c>
+      <c r="C125" t="s">
+        <v>277</v>
+      </c>
+      <c r="D125" t="s">
+        <v>278</v>
+      </c>
+      <c r="E125" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>279</v>
+      </c>
+      <c r="B126" t="s">
+        <v>280</v>
+      </c>
+      <c r="C126" t="s">
+        <v>281</v>
+      </c>
+      <c r="D126" t="s">
+        <v>282</v>
+      </c>
+      <c r="E126" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>284</v>
+      </c>
+      <c r="B127" t="s">
+        <v>285</v>
+      </c>
+      <c r="C127" t="s">
+        <v>286</v>
+      </c>
+      <c r="D127" t="s">
+        <v>286</v>
+      </c>
+      <c r="E127" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>578</v>
+      </c>
+      <c r="B128" t="s">
+        <v>490</v>
+      </c>
+      <c r="C128" t="s">
+        <v>490</v>
+      </c>
+      <c r="D128" t="s">
+        <v>491</v>
+      </c>
+      <c r="E128" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>579</v>
+      </c>
+      <c r="B129" t="s">
+        <v>493</v>
+      </c>
+      <c r="C129" t="s">
+        <v>494</v>
+      </c>
+      <c r="D129" t="s">
+        <v>495</v>
+      </c>
+      <c r="E129" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>521</v>
+      </c>
+      <c r="B130" t="s">
+        <v>594</v>
+      </c>
+      <c r="C130" t="s">
+        <v>544</v>
+      </c>
+      <c r="D130" t="s">
+        <v>575</v>
+      </c>
+      <c r="E130" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>519</v>
+      </c>
+      <c r="B131" t="s">
+        <v>595</v>
+      </c>
+      <c r="C131" t="s">
+        <v>524</v>
+      </c>
+      <c r="D131" t="s">
+        <v>573</v>
+      </c>
+      <c r="E131" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>520</v>
+      </c>
+      <c r="B132" t="s">
+        <v>555</v>
+      </c>
+      <c r="C132" t="s">
+        <v>525</v>
+      </c>
+      <c r="D132" t="s">
+        <v>574</v>
+      </c>
+      <c r="E132" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>548</v>
+      </c>
+      <c r="B133" t="s">
+        <v>596</v>
+      </c>
+      <c r="C133" t="s">
+        <v>545</v>
+      </c>
+      <c r="D133" t="s">
+        <v>576</v>
+      </c>
+      <c r="E133" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>514</v>
+      </c>
+      <c r="B134" t="s">
+        <v>600</v>
+      </c>
+      <c r="C134" t="s">
+        <v>547</v>
+      </c>
+      <c r="D134" t="s">
+        <v>601</v>
+      </c>
+      <c r="E134" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>516</v>
+      </c>
+      <c r="B135" t="s">
+        <v>597</v>
+      </c>
+      <c r="C135" t="s">
+        <v>546</v>
+      </c>
+      <c r="D135" t="s">
+        <v>571</v>
+      </c>
+      <c r="E135" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>517</v>
+      </c>
+      <c r="B136" t="s">
+        <v>598</v>
+      </c>
+      <c r="C136" t="s">
+        <v>543</v>
+      </c>
+      <c r="D136" t="s">
+        <v>572</v>
+      </c>
+      <c r="E136" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>515</v>
+      </c>
+      <c r="B137" t="s">
+        <v>553</v>
+      </c>
+      <c r="C137" t="s">
+        <v>522</v>
+      </c>
+      <c r="D137" t="s">
+        <v>570</v>
+      </c>
+      <c r="E137" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>518</v>
+      </c>
+      <c r="B138" t="s">
+        <v>599</v>
+      </c>
+      <c r="C138" t="s">
+        <v>523</v>
+      </c>
+      <c r="D138" t="s">
+        <v>554</v>
+      </c>
+      <c r="E138" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>287</v>
+      </c>
+      <c r="B139" t="s">
+        <v>288</v>
+      </c>
+      <c r="C139" t="s">
+        <v>289</v>
+      </c>
+      <c r="D139" t="s">
+        <v>290</v>
+      </c>
+      <c r="E139" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>420</v>
+      </c>
+      <c r="B140" t="s">
+        <v>426</v>
+      </c>
+      <c r="C140" t="s">
+        <v>423</v>
+      </c>
+      <c r="D140" t="s">
+        <v>421</v>
+      </c>
+      <c r="E140" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>424</v>
+      </c>
+      <c r="B141" t="s">
+        <v>425</v>
+      </c>
+      <c r="C141" t="s">
+        <v>427</v>
+      </c>
+      <c r="D141" t="s">
+        <v>428</v>
+      </c>
+      <c r="E141" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
         <v>346</v>
       </c>
-      <c r="E89" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>237</v>
-      </c>
-      <c r="B90" t="s">
-        <v>238</v>
-      </c>
-      <c r="C90" t="s">
-        <v>239</v>
-      </c>
-      <c r="D90" t="s">
-        <v>240</v>
-      </c>
-      <c r="E90" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>475</v>
-      </c>
-      <c r="B91" t="s">
-        <v>245</v>
-      </c>
-      <c r="C91" t="s">
-        <v>476</v>
-      </c>
-      <c r="D91" t="s">
-        <v>245</v>
-      </c>
-      <c r="E91" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>242</v>
-      </c>
-      <c r="B92" t="s">
-        <v>243</v>
-      </c>
-      <c r="C92" t="s">
-        <v>244</v>
-      </c>
-      <c r="D92" t="s">
-        <v>245</v>
-      </c>
-      <c r="E92" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>246</v>
-      </c>
-      <c r="B93" t="s">
-        <v>247</v>
-      </c>
-      <c r="C93" t="s">
-        <v>248</v>
-      </c>
-      <c r="D93" t="s">
-        <v>249</v>
-      </c>
-      <c r="E93" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>251</v>
-      </c>
-      <c r="B94" t="s">
-        <v>252</v>
-      </c>
-      <c r="C94" t="s">
-        <v>253</v>
-      </c>
-      <c r="D94" t="s">
-        <v>254</v>
-      </c>
-      <c r="E94" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>256</v>
-      </c>
-      <c r="B95" t="s">
-        <v>257</v>
-      </c>
-      <c r="C95" t="s">
-        <v>258</v>
-      </c>
-      <c r="D95" t="s">
-        <v>259</v>
-      </c>
-      <c r="E95" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>424</v>
-      </c>
-      <c r="B96" t="s">
-        <v>425</v>
-      </c>
-      <c r="C96" t="s">
-        <v>426</v>
-      </c>
-      <c r="D96" t="s">
-        <v>427</v>
-      </c>
-      <c r="E96" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>261</v>
-      </c>
-      <c r="B97" t="s">
-        <v>262</v>
-      </c>
-      <c r="C97" t="s">
-        <v>263</v>
-      </c>
-      <c r="D97" t="s">
-        <v>264</v>
-      </c>
-      <c r="E97" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+      <c r="B142" t="s">
+        <v>348</v>
+      </c>
+      <c r="C142" t="s">
+        <v>350</v>
+      </c>
+      <c r="D142" t="s">
         <v>352</v>
       </c>
-      <c r="B98" t="s">
-        <v>353</v>
-      </c>
-      <c r="C98" t="s">
+      <c r="E142" t="s">
         <v>354</v>
-      </c>
-      <c r="D98" t="s">
-        <v>353</v>
-      </c>
-      <c r="E98" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>419</v>
-      </c>
-      <c r="B99" t="s">
-        <v>420</v>
-      </c>
-      <c r="C99" t="s">
-        <v>421</v>
-      </c>
-      <c r="D99" t="s">
-        <v>422</v>
-      </c>
-      <c r="E99" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>265</v>
-      </c>
-      <c r="B100" t="s">
-        <v>266</v>
-      </c>
-      <c r="C100" t="s">
-        <v>267</v>
-      </c>
-      <c r="D100" t="s">
-        <v>268</v>
-      </c>
-      <c r="E100" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>269</v>
-      </c>
-      <c r="B101" t="s">
-        <v>270</v>
-      </c>
-      <c r="C101" t="s">
-        <v>271</v>
-      </c>
-      <c r="D101" t="s">
-        <v>272</v>
-      </c>
-      <c r="E101" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>400</v>
-      </c>
-      <c r="B102" t="s">
-        <v>401</v>
-      </c>
-      <c r="C102" t="s">
-        <v>402</v>
-      </c>
-      <c r="D102" t="s">
-        <v>403</v>
-      </c>
-      <c r="E102" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>387</v>
-      </c>
-      <c r="B103" t="s">
-        <v>396</v>
-      </c>
-      <c r="C103" t="s">
-        <v>397</v>
-      </c>
-      <c r="D103" t="s">
-        <v>398</v>
-      </c>
-      <c r="E103" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>386</v>
-      </c>
-      <c r="B104" t="s">
-        <v>393</v>
-      </c>
-      <c r="C104" t="s">
-        <v>394</v>
-      </c>
-      <c r="D104" t="s">
-        <v>395</v>
-      </c>
-      <c r="E104" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>389</v>
-      </c>
-      <c r="B105" t="s">
-        <v>388</v>
-      </c>
-      <c r="C105" t="s">
-        <v>390</v>
-      </c>
-      <c r="D105" t="s">
-        <v>391</v>
-      </c>
-      <c r="E105" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>273</v>
-      </c>
-      <c r="B106" t="s">
-        <v>274</v>
-      </c>
-      <c r="C106" t="s">
-        <v>275</v>
-      </c>
-      <c r="D106" t="s">
-        <v>276</v>
-      </c>
-      <c r="E106" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>277</v>
-      </c>
-      <c r="B107" t="s">
-        <v>278</v>
-      </c>
-      <c r="C107" t="s">
-        <v>279</v>
-      </c>
-      <c r="D107" t="s">
-        <v>280</v>
-      </c>
-      <c r="E107" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>281</v>
-      </c>
-      <c r="B108" t="s">
-        <v>282</v>
-      </c>
-      <c r="C108" t="s">
-        <v>380</v>
-      </c>
-      <c r="D108" t="s">
-        <v>412</v>
-      </c>
-      <c r="E108" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>473</v>
-      </c>
-      <c r="B109" t="s">
-        <v>287</v>
-      </c>
-      <c r="C109" t="s">
-        <v>474</v>
-      </c>
-      <c r="D109" t="s">
-        <v>287</v>
-      </c>
-      <c r="E109" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>284</v>
-      </c>
-      <c r="B110" t="s">
-        <v>285</v>
-      </c>
-      <c r="C110" t="s">
-        <v>286</v>
-      </c>
-      <c r="D110" t="s">
-        <v>287</v>
-      </c>
-      <c r="E110" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>288</v>
-      </c>
-      <c r="B111" t="s">
-        <v>289</v>
-      </c>
-      <c r="C111" t="s">
-        <v>290</v>
-      </c>
-      <c r="D111" t="s">
-        <v>291</v>
-      </c>
-      <c r="E111" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>293</v>
-      </c>
-      <c r="B112" t="s">
-        <v>294</v>
-      </c>
-      <c r="C112" t="s">
-        <v>295</v>
-      </c>
-      <c r="D112" t="s">
-        <v>295</v>
-      </c>
-      <c r="E112" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>296</v>
-      </c>
-      <c r="B113" t="s">
-        <v>297</v>
-      </c>
-      <c r="C113" t="s">
-        <v>298</v>
-      </c>
-      <c r="D113" t="s">
-        <v>299</v>
-      </c>
-      <c r="E113" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>429</v>
-      </c>
-      <c r="B114" t="s">
-        <v>435</v>
-      </c>
-      <c r="C114" t="s">
-        <v>432</v>
-      </c>
-      <c r="D114" t="s">
-        <v>430</v>
-      </c>
-      <c r="E114" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>433</v>
-      </c>
-      <c r="B115" t="s">
-        <v>434</v>
-      </c>
-      <c r="C115" t="s">
-        <v>436</v>
-      </c>
-      <c r="D115" t="s">
-        <v>437</v>
-      </c>
-      <c r="E115" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>355</v>
-      </c>
-      <c r="B116" t="s">
-        <v>357</v>
-      </c>
-      <c r="C116" t="s">
-        <v>359</v>
-      </c>
-      <c r="D116" t="s">
-        <v>361</v>
-      </c>
-      <c r="E116" t="s">
-        <v>363</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B50" r:id="rId1" xr:uid="{772ACA42-8DE4-4015-A5BA-E378BC1F9836}"/>
-    <hyperlink ref="C50:E50" r:id="rId2" display="https://github.com/NightDreamGames/Graded" xr:uid="{F6D4AF19-D559-447E-AF49-35B5F0BBE70D}"/>
-    <hyperlink ref="B40" r:id="rId3" xr:uid="{7E3A0FC6-064A-4102-B40F-1969830D4899}"/>
-    <hyperlink ref="C40:E40" r:id="rId4" display="contact@nightdreamgames.com" xr:uid="{49649B53-773A-4287-9E32-3113566F351E}"/>
+    <hyperlink ref="B49" r:id="rId1" xr:uid="{772ACA42-8DE4-4015-A5BA-E378BC1F9836}"/>
+    <hyperlink ref="C49:E49" r:id="rId2" display="https://github.com/NightDreamGames/Graded" xr:uid="{F6D4AF19-D559-447E-AF49-35B5F0BBE70D}"/>
+    <hyperlink ref="B39" r:id="rId3" xr:uid="{7E3A0FC6-064A-4102-B40F-1969830D4899}"/>
+    <hyperlink ref="C39:E39" r:id="rId4" display="contact@nightdreamgames.com" xr:uid="{49649B53-773A-4287-9E32-3113566F351E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>

</xml_diff>

<commit_message>
Add tutorial to subject editing route
</commit_message>
<xml_diff>
--- a/assets/Localizations.xlsx
+++ b/assets/Localizations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Graded\Graded - Flutter\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C10EEBC-3542-4FE0-9AA4-B488D76A2816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61DE77DD-91DE-440F-903E-54F08C67CD32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="string" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0">string!$A$1:$B$147</definedName>
+    <definedName name="ExternalData_1" localSheetId="0">string!$A$1:$B$149</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="625">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="634">
   <si>
     <t>keys</t>
   </si>
@@ -1898,6 +1898,33 @@
   </si>
   <si>
     <t>Sauvegarde importée avec succès.</t>
+  </si>
+  <si>
+    <t>showcase_drag_subject</t>
+  </si>
+  <si>
+    <t>showcase_tap_subject</t>
+  </si>
+  <si>
+    <t>Drag to change subject order</t>
+  </si>
+  <si>
+    <t>Ziehe, um die Reihenfolge der Fächer zu ändern</t>
+  </si>
+  <si>
+    <t>Glissez pour changer l'ordre des matières</t>
+  </si>
+  <si>
+    <t>Zéi fir d'Reiefolleg vun de Fächer ze änneren</t>
+  </si>
+  <si>
+    <t>Tap to make the subject above a subject group</t>
+  </si>
+  <si>
+    <t>Appuyez pour faire du sujet au-dessus un groupe de matières</t>
+  </si>
+  <si>
+    <t>Berühre um aus dem Fach drüber eine Fachgruppe zu machen</t>
   </si>
 </sst>
 </file>
@@ -1973,10 +2000,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="string" displayName="string" ref="A1:E147" totalsRowShown="0">
-  <autoFilter ref="A1:E147" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E147">
-    <sortCondition ref="A1:A147"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="string" displayName="string" ref="A1:E149" totalsRowShown="0">
+  <autoFilter ref="A1:E149" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E149">
+    <sortCondition ref="A1:A149"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="keys"/>
@@ -2277,10 +2304,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E147"/>
+  <dimension ref="A1:E149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="C147" sqref="C147"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="A131" sqref="A131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4232,390 +4259,390 @@
     </row>
     <row r="115" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>247</v>
+        <v>625</v>
       </c>
       <c r="B115" t="s">
-        <v>248</v>
+        <v>627</v>
       </c>
       <c r="C115" t="s">
-        <v>249</v>
+        <v>629</v>
       </c>
       <c r="D115" t="s">
-        <v>250</v>
+        <v>628</v>
       </c>
       <c r="E115" t="s">
-        <v>251</v>
+        <v>630</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>415</v>
+        <v>626</v>
       </c>
       <c r="B116" t="s">
-        <v>416</v>
+        <v>631</v>
       </c>
       <c r="C116" t="s">
-        <v>417</v>
+        <v>632</v>
       </c>
       <c r="D116" t="s">
-        <v>418</v>
+        <v>633</v>
       </c>
       <c r="E116" t="s">
-        <v>419</v>
+        <v>572</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="B117" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="C117" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="D117" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="E117" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>343</v>
+        <v>415</v>
       </c>
       <c r="B118" t="s">
-        <v>344</v>
+        <v>416</v>
       </c>
       <c r="C118" t="s">
-        <v>345</v>
+        <v>417</v>
       </c>
       <c r="D118" t="s">
-        <v>344</v>
+        <v>418</v>
       </c>
       <c r="E118" t="s">
-        <v>344</v>
+        <v>419</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>410</v>
+        <v>252</v>
       </c>
       <c r="B119" t="s">
-        <v>411</v>
+        <v>253</v>
       </c>
       <c r="C119" t="s">
-        <v>412</v>
+        <v>254</v>
       </c>
       <c r="D119" t="s">
-        <v>413</v>
+        <v>255</v>
       </c>
       <c r="E119" t="s">
-        <v>414</v>
+        <v>255</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>256</v>
+        <v>343</v>
       </c>
       <c r="B120" t="s">
-        <v>257</v>
+        <v>344</v>
       </c>
       <c r="C120" t="s">
-        <v>258</v>
+        <v>345</v>
       </c>
       <c r="D120" t="s">
-        <v>259</v>
+        <v>344</v>
       </c>
       <c r="E120" t="s">
-        <v>259</v>
+        <v>344</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>260</v>
+        <v>410</v>
       </c>
       <c r="B121" t="s">
-        <v>261</v>
+        <v>411</v>
       </c>
       <c r="C121" t="s">
-        <v>262</v>
+        <v>412</v>
       </c>
       <c r="D121" t="s">
-        <v>263</v>
+        <v>413</v>
       </c>
       <c r="E121" t="s">
-        <v>263</v>
+        <v>414</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>391</v>
+        <v>256</v>
       </c>
       <c r="B122" t="s">
-        <v>392</v>
+        <v>257</v>
       </c>
       <c r="C122" t="s">
-        <v>393</v>
+        <v>258</v>
       </c>
       <c r="D122" t="s">
-        <v>394</v>
+        <v>259</v>
       </c>
       <c r="E122" t="s">
-        <v>394</v>
+        <v>259</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>378</v>
+        <v>260</v>
       </c>
       <c r="B123" t="s">
-        <v>387</v>
+        <v>261</v>
       </c>
       <c r="C123" t="s">
-        <v>388</v>
+        <v>262</v>
       </c>
       <c r="D123" t="s">
-        <v>389</v>
+        <v>263</v>
       </c>
       <c r="E123" t="s">
-        <v>390</v>
+        <v>263</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>377</v>
+        <v>391</v>
       </c>
       <c r="B124" t="s">
-        <v>384</v>
+        <v>392</v>
       </c>
       <c r="C124" t="s">
-        <v>385</v>
+        <v>393</v>
       </c>
       <c r="D124" t="s">
-        <v>386</v>
+        <v>394</v>
       </c>
       <c r="E124" t="s">
-        <v>386</v>
+        <v>394</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B125" t="s">
-        <v>379</v>
+        <v>387</v>
       </c>
       <c r="C125" t="s">
-        <v>381</v>
+        <v>388</v>
       </c>
       <c r="D125" t="s">
-        <v>382</v>
+        <v>389</v>
       </c>
       <c r="E125" t="s">
-        <v>383</v>
+        <v>390</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>264</v>
+        <v>377</v>
       </c>
       <c r="B126" t="s">
-        <v>265</v>
+        <v>384</v>
       </c>
       <c r="C126" t="s">
-        <v>266</v>
+        <v>385</v>
       </c>
       <c r="D126" t="s">
-        <v>267</v>
+        <v>386</v>
       </c>
       <c r="E126" t="s">
-        <v>267</v>
+        <v>386</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>268</v>
+        <v>380</v>
       </c>
       <c r="B127" t="s">
-        <v>269</v>
+        <v>379</v>
       </c>
       <c r="C127" t="s">
-        <v>270</v>
+        <v>381</v>
       </c>
       <c r="D127" t="s">
-        <v>271</v>
+        <v>382</v>
       </c>
       <c r="E127" t="s">
-        <v>271</v>
+        <v>383</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="B128" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="C128" t="s">
-        <v>371</v>
+        <v>266</v>
       </c>
       <c r="D128" t="s">
-        <v>403</v>
+        <v>267</v>
       </c>
       <c r="E128" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>459</v>
+        <v>268</v>
       </c>
       <c r="B129" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="C129" t="s">
-        <v>460</v>
+        <v>270</v>
       </c>
       <c r="D129" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="E129" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B130" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C130" t="s">
-        <v>277</v>
+        <v>371</v>
       </c>
       <c r="D130" t="s">
-        <v>278</v>
+        <v>403</v>
       </c>
       <c r="E130" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>279</v>
+        <v>459</v>
       </c>
       <c r="B131" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C131" t="s">
-        <v>281</v>
+        <v>460</v>
       </c>
       <c r="D131" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="E131" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="B132" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="C132" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="D132" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="E132" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>573</v>
+        <v>279</v>
       </c>
       <c r="B133" t="s">
-        <v>485</v>
+        <v>280</v>
       </c>
       <c r="C133" t="s">
-        <v>485</v>
+        <v>281</v>
       </c>
       <c r="D133" t="s">
-        <v>486</v>
+        <v>282</v>
       </c>
       <c r="E133" t="s">
-        <v>487</v>
+        <v>283</v>
       </c>
     </row>
     <row r="134" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>574</v>
+        <v>284</v>
       </c>
       <c r="B134" t="s">
-        <v>488</v>
+        <v>285</v>
       </c>
       <c r="C134" t="s">
-        <v>489</v>
+        <v>286</v>
       </c>
       <c r="D134" t="s">
-        <v>490</v>
+        <v>286</v>
       </c>
       <c r="E134" t="s">
-        <v>491</v>
+        <v>286</v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>516</v>
+        <v>573</v>
       </c>
       <c r="B135" t="s">
-        <v>589</v>
+        <v>485</v>
       </c>
       <c r="C135" t="s">
-        <v>539</v>
+        <v>485</v>
       </c>
       <c r="D135" t="s">
-        <v>570</v>
+        <v>486</v>
       </c>
       <c r="E135" t="s">
-        <v>572</v>
+        <v>487</v>
       </c>
     </row>
     <row r="136" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>514</v>
+        <v>574</v>
       </c>
       <c r="B136" t="s">
-        <v>590</v>
+        <v>488</v>
       </c>
       <c r="C136" t="s">
-        <v>519</v>
+        <v>489</v>
       </c>
       <c r="D136" t="s">
-        <v>568</v>
+        <v>490</v>
       </c>
       <c r="E136" t="s">
-        <v>572</v>
+        <v>491</v>
       </c>
     </row>
     <row r="137" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="B137" t="s">
-        <v>550</v>
+        <v>589</v>
       </c>
       <c r="C137" t="s">
-        <v>520</v>
+        <v>539</v>
       </c>
       <c r="D137" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="E137" t="s">
         <v>572</v>
@@ -4623,16 +4650,16 @@
     </row>
     <row r="138" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>543</v>
+        <v>514</v>
       </c>
       <c r="B138" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C138" t="s">
-        <v>540</v>
+        <v>519</v>
       </c>
       <c r="D138" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="E138" t="s">
         <v>572</v>
@@ -4640,16 +4667,16 @@
     </row>
     <row r="139" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>509</v>
+        <v>515</v>
       </c>
       <c r="B139" t="s">
-        <v>595</v>
+        <v>550</v>
       </c>
       <c r="C139" t="s">
-        <v>542</v>
+        <v>520</v>
       </c>
       <c r="D139" t="s">
-        <v>596</v>
+        <v>569</v>
       </c>
       <c r="E139" t="s">
         <v>572</v>
@@ -4657,16 +4684,16 @@
     </row>
     <row r="140" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>511</v>
+        <v>543</v>
       </c>
       <c r="B140" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C140" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="D140" t="s">
-        <v>566</v>
+        <v>571</v>
       </c>
       <c r="E140" t="s">
         <v>572</v>
@@ -4674,16 +4701,16 @@
     </row>
     <row r="141" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="B141" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
       <c r="C141" t="s">
-        <v>538</v>
+        <v>542</v>
       </c>
       <c r="D141" t="s">
-        <v>567</v>
+        <v>596</v>
       </c>
       <c r="E141" t="s">
         <v>572</v>
@@ -4691,16 +4718,16 @@
     </row>
     <row r="142" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="B142" t="s">
-        <v>548</v>
+        <v>592</v>
       </c>
       <c r="C142" t="s">
-        <v>517</v>
+        <v>541</v>
       </c>
       <c r="D142" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="E142" t="s">
         <v>572</v>
@@ -4708,16 +4735,16 @@
     </row>
     <row r="143" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B143" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="C143" t="s">
-        <v>518</v>
+        <v>538</v>
       </c>
       <c r="D143" t="s">
-        <v>549</v>
+        <v>567</v>
       </c>
       <c r="E143" t="s">
         <v>572</v>
@@ -4725,69 +4752,103 @@
     </row>
     <row r="144" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>287</v>
+        <v>510</v>
       </c>
       <c r="B144" t="s">
-        <v>288</v>
+        <v>548</v>
       </c>
       <c r="C144" t="s">
-        <v>289</v>
+        <v>517</v>
       </c>
       <c r="D144" t="s">
-        <v>290</v>
+        <v>565</v>
       </c>
       <c r="E144" t="s">
-        <v>291</v>
+        <v>572</v>
       </c>
     </row>
     <row r="145" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>420</v>
+        <v>513</v>
       </c>
       <c r="B145" t="s">
-        <v>426</v>
+        <v>594</v>
       </c>
       <c r="C145" t="s">
-        <v>423</v>
+        <v>518</v>
       </c>
       <c r="D145" t="s">
-        <v>421</v>
+        <v>549</v>
       </c>
       <c r="E145" t="s">
-        <v>422</v>
+        <v>572</v>
       </c>
     </row>
     <row r="146" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>424</v>
+        <v>287</v>
       </c>
       <c r="B146" t="s">
-        <v>425</v>
+        <v>288</v>
       </c>
       <c r="C146" t="s">
-        <v>427</v>
+        <v>289</v>
       </c>
       <c r="D146" t="s">
-        <v>428</v>
+        <v>290</v>
       </c>
       <c r="E146" t="s">
-        <v>429</v>
+        <v>291</v>
       </c>
     </row>
     <row r="147" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
+        <v>420</v>
+      </c>
+      <c r="B147" t="s">
+        <v>426</v>
+      </c>
+      <c r="C147" t="s">
+        <v>423</v>
+      </c>
+      <c r="D147" t="s">
+        <v>421</v>
+      </c>
+      <c r="E147" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>424</v>
+      </c>
+      <c r="B148" t="s">
+        <v>425</v>
+      </c>
+      <c r="C148" t="s">
+        <v>427</v>
+      </c>
+      <c r="D148" t="s">
+        <v>428</v>
+      </c>
+      <c r="E148" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
         <v>346</v>
       </c>
-      <c r="B147" t="s">
+      <c r="B149" t="s">
         <v>348</v>
       </c>
-      <c r="C147" t="s">
+      <c r="C149" t="s">
         <v>350</v>
       </c>
-      <c r="D147" t="s">
+      <c r="D149" t="s">
         <v>352</v>
       </c>
-      <c r="E147" t="s">
+      <c r="E149" t="s">
         <v>354</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactor sort mode selector & add indicator
</commit_message>
<xml_diff>
--- a/assets/Localizations.xlsx
+++ b/assets/Localizations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Graded\Graded - Flutter\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61DE77DD-91DE-440F-903E-54F08C67CD32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C3244B-4CFF-44A1-B8D2-E63352E32F26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="string" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0">string!$A$1:$B$149</definedName>
+    <definedName name="ExternalData_1" localSheetId="0">string!$A$1:$B$150</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="634">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="638">
   <si>
     <t>keys</t>
   </si>
@@ -1925,6 +1925,18 @@
   </si>
   <si>
     <t>Berühre um aus dem Fach drüber eine Fachgruppe zu machen</t>
+  </si>
+  <si>
+    <t>result</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Résultat</t>
+  </si>
+  <si>
+    <t>Resultat</t>
   </si>
 </sst>
 </file>
@@ -2000,10 +2012,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="string" displayName="string" ref="A1:E149" totalsRowShown="0">
-  <autoFilter ref="A1:E149" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E149">
-    <sortCondition ref="A1:A149"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="string" displayName="string" ref="A1:E150" totalsRowShown="0">
+  <autoFilter ref="A1:E150" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E150">
+    <sortCondition ref="A1:A150"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="keys"/>
@@ -2304,10 +2316,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E149"/>
+  <dimension ref="A1:E150"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="A131" sqref="A131"/>
+      <selection activeCell="C142" sqref="C142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3664,254 +3676,254 @@
     </row>
     <row r="80" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>213</v>
+        <v>634</v>
       </c>
       <c r="B80" t="s">
-        <v>214</v>
+        <v>635</v>
       </c>
       <c r="C80" t="s">
-        <v>215</v>
+        <v>636</v>
       </c>
       <c r="D80" t="s">
-        <v>216</v>
+        <v>637</v>
       </c>
       <c r="E80" t="s">
-        <v>217</v>
+        <v>637</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="B81" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="C81" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="D81" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="E81" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>440</v>
+        <v>218</v>
       </c>
       <c r="B82" t="s">
-        <v>441</v>
+        <v>219</v>
       </c>
       <c r="C82" t="s">
-        <v>442</v>
+        <v>220</v>
       </c>
       <c r="D82" t="s">
-        <v>443</v>
+        <v>221</v>
       </c>
       <c r="E82" t="s">
-        <v>444</v>
+        <v>222</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>223</v>
+        <v>440</v>
       </c>
       <c r="B83" t="s">
-        <v>224</v>
+        <v>441</v>
       </c>
       <c r="C83" t="s">
-        <v>225</v>
+        <v>442</v>
       </c>
       <c r="D83" t="s">
-        <v>226</v>
+        <v>443</v>
       </c>
       <c r="E83" t="s">
-        <v>227</v>
+        <v>444</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>312</v>
+        <v>223</v>
       </c>
       <c r="B84" t="s">
-        <v>313</v>
+        <v>224</v>
       </c>
       <c r="C84" t="s">
-        <v>313</v>
+        <v>225</v>
       </c>
       <c r="D84" t="s">
-        <v>458</v>
+        <v>226</v>
       </c>
       <c r="E84" t="s">
-        <v>314</v>
+        <v>227</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>395</v>
+        <v>312</v>
       </c>
       <c r="B85" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C85" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="D85" t="s">
-        <v>330</v>
+        <v>458</v>
       </c>
       <c r="E85" t="s">
-        <v>339</v>
+        <v>314</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B86" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C86" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D86" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E86" t="s">
-        <v>331</v>
+        <v>339</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B87" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="C87" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D87" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E87" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B88" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="C88" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D88" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E88" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B89" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="C89" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D89" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="E89" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B90" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C90" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D90" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="E90" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B91" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C91" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D91" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E91" t="s">
-        <v>374</v>
+        <v>341</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B92" t="s">
-        <v>409</v>
+        <v>320</v>
       </c>
       <c r="C92" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D92" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E92" t="s">
-        <v>342</v>
+        <v>374</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>494</v>
+        <v>402</v>
       </c>
       <c r="B93" t="s">
-        <v>545</v>
+        <v>409</v>
       </c>
       <c r="C93" t="s">
-        <v>523</v>
+        <v>329</v>
       </c>
       <c r="D93" t="s">
-        <v>552</v>
+        <v>337</v>
       </c>
       <c r="E93" t="s">
-        <v>572</v>
+        <v>342</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="B94" t="s">
-        <v>586</v>
+        <v>545</v>
       </c>
       <c r="C94" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="D94" t="s">
-        <v>587</v>
+        <v>552</v>
       </c>
       <c r="E94" t="s">
         <v>572</v>
@@ -3919,16 +3931,16 @@
     </row>
     <row r="95" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="B95" t="s">
-        <v>575</v>
+        <v>586</v>
       </c>
       <c r="C95" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="D95" t="s">
-        <v>557</v>
+        <v>587</v>
       </c>
       <c r="E95" t="s">
         <v>572</v>
@@ -3936,16 +3948,16 @@
     </row>
     <row r="96" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B96" t="s">
-        <v>531</v>
+        <v>575</v>
       </c>
       <c r="C96" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D96" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E96" t="s">
         <v>572</v>
@@ -3953,16 +3965,16 @@
     </row>
     <row r="97" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="B97" t="s">
-        <v>588</v>
+        <v>531</v>
       </c>
       <c r="C97" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="D97" t="s">
-        <v>588</v>
+        <v>558</v>
       </c>
       <c r="E97" t="s">
         <v>572</v>
@@ -3970,16 +3982,16 @@
     </row>
     <row r="98" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="B98" t="s">
-        <v>576</v>
+        <v>588</v>
       </c>
       <c r="C98" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="D98" t="s">
-        <v>555</v>
+        <v>588</v>
       </c>
       <c r="E98" t="s">
         <v>572</v>
@@ -3987,16 +3999,16 @@
     </row>
     <row r="99" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>504</v>
+        <v>498</v>
       </c>
       <c r="B99" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C99" t="s">
-        <v>533</v>
+        <v>527</v>
       </c>
       <c r="D99" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
       <c r="E99" t="s">
         <v>572</v>
@@ -4004,16 +4016,16 @@
     </row>
     <row r="100" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>492</v>
+        <v>504</v>
       </c>
       <c r="B100" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C100" t="s">
-        <v>521</v>
+        <v>533</v>
       </c>
       <c r="D100" t="s">
-        <v>544</v>
+        <v>560</v>
       </c>
       <c r="E100" t="s">
         <v>572</v>
@@ -4021,16 +4033,16 @@
     </row>
     <row r="101" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="B101" t="s">
-        <v>546</v>
+        <v>578</v>
       </c>
       <c r="C101" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="D101" t="s">
-        <v>553</v>
+        <v>544</v>
       </c>
       <c r="E101" t="s">
         <v>572</v>
@@ -4038,16 +4050,16 @@
     </row>
     <row r="102" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>507</v>
+        <v>495</v>
       </c>
       <c r="B102" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C102" t="s">
-        <v>536</v>
+        <v>524</v>
       </c>
       <c r="D102" t="s">
-        <v>563</v>
+        <v>553</v>
       </c>
       <c r="E102" t="s">
         <v>572</v>
@@ -4055,16 +4067,16 @@
     </row>
     <row r="103" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>503</v>
+        <v>507</v>
       </c>
       <c r="B103" t="s">
-        <v>579</v>
+        <v>547</v>
       </c>
       <c r="C103" t="s">
-        <v>532</v>
+        <v>536</v>
       </c>
       <c r="D103" t="s">
-        <v>559</v>
+        <v>563</v>
       </c>
       <c r="E103" t="s">
         <v>572</v>
@@ -4072,16 +4084,16 @@
     </row>
     <row r="104" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>499</v>
+        <v>503</v>
       </c>
       <c r="B104" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C104" t="s">
-        <v>528</v>
+        <v>532</v>
       </c>
       <c r="D104" t="s">
-        <v>556</v>
+        <v>559</v>
       </c>
       <c r="E104" t="s">
         <v>572</v>
@@ -4089,16 +4101,16 @@
     </row>
     <row r="105" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>508</v>
+        <v>499</v>
       </c>
       <c r="B105" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C105" t="s">
-        <v>537</v>
+        <v>528</v>
       </c>
       <c r="D105" t="s">
-        <v>564</v>
+        <v>556</v>
       </c>
       <c r="E105" t="s">
         <v>572</v>
@@ -4106,16 +4118,16 @@
     </row>
     <row r="106" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="B106" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C106" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="D106" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="E106" t="s">
         <v>572</v>
@@ -4123,16 +4135,16 @@
     </row>
     <row r="107" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="B107" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C107" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="D107" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="E107" t="s">
         <v>572</v>
@@ -4140,16 +4152,16 @@
     </row>
     <row r="108" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>496</v>
+        <v>505</v>
       </c>
       <c r="B108" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C108" t="s">
-        <v>525</v>
+        <v>534</v>
       </c>
       <c r="D108" t="s">
-        <v>554</v>
+        <v>561</v>
       </c>
       <c r="E108" t="s">
         <v>572</v>
@@ -4157,16 +4169,16 @@
     </row>
     <row r="109" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>493</v>
+        <v>496</v>
       </c>
       <c r="B109" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C109" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
       <c r="D109" t="s">
-        <v>551</v>
+        <v>554</v>
       </c>
       <c r="E109" t="s">
         <v>572</v>
@@ -4174,47 +4186,47 @@
     </row>
     <row r="110" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>228</v>
+        <v>493</v>
       </c>
       <c r="B110" t="s">
-        <v>229</v>
+        <v>585</v>
       </c>
       <c r="C110" t="s">
-        <v>230</v>
+        <v>522</v>
       </c>
       <c r="D110" t="s">
-        <v>231</v>
+        <v>551</v>
       </c>
       <c r="E110" t="s">
-        <v>232</v>
+        <v>572</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>461</v>
+        <v>228</v>
       </c>
       <c r="B111" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="C111" t="s">
-        <v>462</v>
+        <v>230</v>
       </c>
       <c r="D111" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="E111" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>233</v>
+        <v>461</v>
       </c>
       <c r="B112" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C112" t="s">
-        <v>235</v>
+        <v>462</v>
       </c>
       <c r="D112" t="s">
         <v>236</v>
@@ -4225,336 +4237,336 @@
     </row>
     <row r="113" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B113" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C113" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="D113" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="E113" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="114" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="B114" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="C114" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="D114" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="E114" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>625</v>
+        <v>242</v>
       </c>
       <c r="B115" t="s">
-        <v>627</v>
+        <v>243</v>
       </c>
       <c r="C115" t="s">
-        <v>629</v>
+        <v>244</v>
       </c>
       <c r="D115" t="s">
-        <v>628</v>
+        <v>245</v>
       </c>
       <c r="E115" t="s">
-        <v>630</v>
+        <v>246</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B116" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="C116" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="D116" t="s">
-        <v>633</v>
+        <v>628</v>
       </c>
       <c r="E116" t="s">
-        <v>572</v>
+        <v>630</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>247</v>
+        <v>626</v>
       </c>
       <c r="B117" t="s">
-        <v>248</v>
+        <v>631</v>
       </c>
       <c r="C117" t="s">
-        <v>249</v>
+        <v>632</v>
       </c>
       <c r="D117" t="s">
-        <v>250</v>
+        <v>633</v>
       </c>
       <c r="E117" t="s">
-        <v>251</v>
+        <v>572</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>415</v>
+        <v>247</v>
       </c>
       <c r="B118" t="s">
-        <v>416</v>
+        <v>248</v>
       </c>
       <c r="C118" t="s">
-        <v>417</v>
+        <v>249</v>
       </c>
       <c r="D118" t="s">
-        <v>418</v>
+        <v>250</v>
       </c>
       <c r="E118" t="s">
-        <v>419</v>
+        <v>251</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>252</v>
+        <v>415</v>
       </c>
       <c r="B119" t="s">
-        <v>253</v>
+        <v>416</v>
       </c>
       <c r="C119" t="s">
-        <v>254</v>
+        <v>417</v>
       </c>
       <c r="D119" t="s">
-        <v>255</v>
+        <v>418</v>
       </c>
       <c r="E119" t="s">
-        <v>255</v>
+        <v>419</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>343</v>
+        <v>252</v>
       </c>
       <c r="B120" t="s">
-        <v>344</v>
+        <v>253</v>
       </c>
       <c r="C120" t="s">
-        <v>345</v>
+        <v>254</v>
       </c>
       <c r="D120" t="s">
-        <v>344</v>
+        <v>255</v>
       </c>
       <c r="E120" t="s">
-        <v>344</v>
+        <v>255</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>410</v>
+        <v>343</v>
       </c>
       <c r="B121" t="s">
-        <v>411</v>
+        <v>344</v>
       </c>
       <c r="C121" t="s">
-        <v>412</v>
+        <v>345</v>
       </c>
       <c r="D121" t="s">
-        <v>413</v>
+        <v>344</v>
       </c>
       <c r="E121" t="s">
-        <v>414</v>
+        <v>344</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>256</v>
+        <v>410</v>
       </c>
       <c r="B122" t="s">
-        <v>257</v>
+        <v>411</v>
       </c>
       <c r="C122" t="s">
-        <v>258</v>
+        <v>412</v>
       </c>
       <c r="D122" t="s">
-        <v>259</v>
+        <v>413</v>
       </c>
       <c r="E122" t="s">
-        <v>259</v>
+        <v>414</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="B123" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="C123" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="D123" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="E123" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>391</v>
+        <v>260</v>
       </c>
       <c r="B124" t="s">
-        <v>392</v>
+        <v>261</v>
       </c>
       <c r="C124" t="s">
-        <v>393</v>
+        <v>262</v>
       </c>
       <c r="D124" t="s">
-        <v>394</v>
+        <v>263</v>
       </c>
       <c r="E124" t="s">
-        <v>394</v>
+        <v>263</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>378</v>
+        <v>391</v>
       </c>
       <c r="B125" t="s">
-        <v>387</v>
+        <v>392</v>
       </c>
       <c r="C125" t="s">
-        <v>388</v>
+        <v>393</v>
       </c>
       <c r="D125" t="s">
-        <v>389</v>
+        <v>394</v>
       </c>
       <c r="E125" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="B126" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="C126" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="D126" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="E126" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="B127" t="s">
-        <v>379</v>
+        <v>384</v>
       </c>
       <c r="C127" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="D127" t="s">
-        <v>382</v>
+        <v>386</v>
       </c>
       <c r="E127" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>264</v>
+        <v>380</v>
       </c>
       <c r="B128" t="s">
-        <v>265</v>
+        <v>379</v>
       </c>
       <c r="C128" t="s">
-        <v>266</v>
+        <v>381</v>
       </c>
       <c r="D128" t="s">
-        <v>267</v>
+        <v>382</v>
       </c>
       <c r="E128" t="s">
-        <v>267</v>
+        <v>383</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="B129" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C129" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="D129" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="E129" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="B130" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="C130" t="s">
-        <v>371</v>
+        <v>270</v>
       </c>
       <c r="D130" t="s">
-        <v>403</v>
+        <v>271</v>
       </c>
       <c r="E130" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>459</v>
+        <v>272</v>
       </c>
       <c r="B131" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="C131" t="s">
-        <v>460</v>
+        <v>371</v>
       </c>
       <c r="D131" t="s">
-        <v>278</v>
+        <v>403</v>
       </c>
       <c r="E131" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>275</v>
+        <v>459</v>
       </c>
       <c r="B132" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="C132" t="s">
-        <v>277</v>
+        <v>460</v>
       </c>
       <c r="D132" t="s">
         <v>278</v>
@@ -4565,101 +4577,101 @@
     </row>
     <row r="133" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="B133" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="C133" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="D133" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="E133" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
     </row>
     <row r="134" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="B134" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="C134" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="D134" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="E134" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>573</v>
+        <v>284</v>
       </c>
       <c r="B135" t="s">
-        <v>485</v>
+        <v>285</v>
       </c>
       <c r="C135" t="s">
-        <v>485</v>
+        <v>286</v>
       </c>
       <c r="D135" t="s">
-        <v>486</v>
+        <v>286</v>
       </c>
       <c r="E135" t="s">
-        <v>487</v>
+        <v>286</v>
       </c>
     </row>
     <row r="136" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B136" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="C136" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="D136" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="E136" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
     </row>
     <row r="137" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>516</v>
+        <v>574</v>
       </c>
       <c r="B137" t="s">
-        <v>589</v>
+        <v>488</v>
       </c>
       <c r="C137" t="s">
-        <v>539</v>
+        <v>489</v>
       </c>
       <c r="D137" t="s">
-        <v>570</v>
+        <v>490</v>
       </c>
       <c r="E137" t="s">
-        <v>572</v>
+        <v>491</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="B138" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C138" t="s">
-        <v>519</v>
+        <v>539</v>
       </c>
       <c r="D138" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c r="E138" t="s">
         <v>572</v>
@@ -4667,16 +4679,16 @@
     </row>
     <row r="139" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B139" t="s">
-        <v>550</v>
+        <v>590</v>
       </c>
       <c r="C139" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D139" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="E139" t="s">
         <v>572</v>
@@ -4684,16 +4696,16 @@
     </row>
     <row r="140" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>543</v>
+        <v>515</v>
       </c>
       <c r="B140" t="s">
-        <v>591</v>
+        <v>550</v>
       </c>
       <c r="C140" t="s">
-        <v>540</v>
+        <v>520</v>
       </c>
       <c r="D140" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="E140" t="s">
         <v>572</v>
@@ -4701,16 +4713,16 @@
     </row>
     <row r="141" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>509</v>
+        <v>543</v>
       </c>
       <c r="B141" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="C141" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="D141" t="s">
-        <v>596</v>
+        <v>571</v>
       </c>
       <c r="E141" t="s">
         <v>572</v>
@@ -4718,16 +4730,16 @@
     </row>
     <row r="142" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="B142" t="s">
-        <v>592</v>
+        <v>595</v>
       </c>
       <c r="C142" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="D142" t="s">
-        <v>566</v>
+        <v>596</v>
       </c>
       <c r="E142" t="s">
         <v>572</v>
@@ -4735,16 +4747,16 @@
     </row>
     <row r="143" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B143" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="C143" t="s">
-        <v>538</v>
+        <v>541</v>
       </c>
       <c r="D143" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="E143" t="s">
         <v>572</v>
@@ -4752,16 +4764,16 @@
     </row>
     <row r="144" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="B144" t="s">
-        <v>548</v>
+        <v>593</v>
       </c>
       <c r="C144" t="s">
-        <v>517</v>
+        <v>538</v>
       </c>
       <c r="D144" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="E144" t="s">
         <v>572</v>
@@ -4769,16 +4781,16 @@
     </row>
     <row r="145" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="B145" t="s">
-        <v>594</v>
+        <v>548</v>
       </c>
       <c r="C145" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D145" t="s">
-        <v>549</v>
+        <v>565</v>
       </c>
       <c r="E145" t="s">
         <v>572</v>
@@ -4786,69 +4798,86 @@
     </row>
     <row r="146" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>287</v>
+        <v>513</v>
       </c>
       <c r="B146" t="s">
-        <v>288</v>
+        <v>594</v>
       </c>
       <c r="C146" t="s">
-        <v>289</v>
+        <v>518</v>
       </c>
       <c r="D146" t="s">
-        <v>290</v>
+        <v>549</v>
       </c>
       <c r="E146" t="s">
-        <v>291</v>
+        <v>572</v>
       </c>
     </row>
     <row r="147" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>420</v>
+        <v>287</v>
       </c>
       <c r="B147" t="s">
-        <v>426</v>
+        <v>288</v>
       </c>
       <c r="C147" t="s">
-        <v>423</v>
+        <v>289</v>
       </c>
       <c r="D147" t="s">
-        <v>421</v>
+        <v>290</v>
       </c>
       <c r="E147" t="s">
-        <v>422</v>
+        <v>291</v>
       </c>
     </row>
     <row r="148" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="B148" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="C148" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="D148" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="E148" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
     </row>
     <row r="149" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
+        <v>424</v>
+      </c>
+      <c r="B149" t="s">
+        <v>425</v>
+      </c>
+      <c r="C149" t="s">
+        <v>427</v>
+      </c>
+      <c r="D149" t="s">
+        <v>428</v>
+      </c>
+      <c r="E149" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
         <v>346</v>
       </c>
-      <c r="B149" t="s">
+      <c r="B150" t="s">
         <v>348</v>
       </c>
-      <c r="C149" t="s">
+      <c r="C150" t="s">
         <v>350</v>
       </c>
-      <c r="D149" t="s">
+      <c r="D150" t="s">
         <v>352</v>
       </c>
-      <c r="E149" t="s">
+      <c r="E150" t="s">
         <v>354</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add oral tests with different weights
</commit_message>
<xml_diff>
--- a/assets/Localizations.xlsx
+++ b/assets/Localizations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Graded\Graded - Flutter\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72EEE449-C848-4F49-B539-D2E51E4CC043}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2AE1D15-BBDC-4DC5-9753-D18AFAC41BE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="string" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0">string!$A$1:$B$151</definedName>
+    <definedName name="ExternalData_1" localSheetId="0">string!$A$1:$B$153</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="643">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="649">
   <si>
     <t>keys</t>
   </si>
@@ -1952,6 +1952,24 @@
   </si>
   <si>
     <t>Feedback ginn</t>
+  </si>
+  <si>
+    <t>oral</t>
+  </si>
+  <si>
+    <t>Oral</t>
+  </si>
+  <si>
+    <t>oral_weight</t>
+  </si>
+  <si>
+    <t>Oral weight</t>
+  </si>
+  <si>
+    <t>Coefficient d'oral</t>
+  </si>
+  <si>
+    <t>Oral Koeffizient</t>
   </si>
 </sst>
 </file>
@@ -2027,10 +2045,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="string" displayName="string" ref="A1:E151" totalsRowShown="0">
-  <autoFilter ref="A1:E151" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E151">
-    <sortCondition ref="A1:A151"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="string" displayName="string" ref="A1:E153" totalsRowShown="0">
+  <autoFilter ref="A1:E153" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E153">
+    <sortCondition ref="A1:A153"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="keys"/>
@@ -2331,10 +2349,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E151"/>
+  <dimension ref="A1:E153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
-      <selection activeCell="E151" sqref="E151"/>
+    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
+      <selection activeCell="E153" sqref="E153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3606,373 +3624,373 @@
     </row>
     <row r="75" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>188</v>
+        <v>643</v>
       </c>
       <c r="B75" t="s">
-        <v>189</v>
+        <v>644</v>
       </c>
       <c r="C75" t="s">
-        <v>190</v>
+        <v>644</v>
       </c>
       <c r="D75" t="s">
-        <v>191</v>
+        <v>644</v>
       </c>
       <c r="E75" t="s">
-        <v>192</v>
+        <v>644</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>193</v>
+        <v>645</v>
       </c>
       <c r="B76" t="s">
-        <v>194</v>
+        <v>646</v>
       </c>
       <c r="C76" t="s">
-        <v>195</v>
+        <v>647</v>
       </c>
       <c r="D76" t="s">
-        <v>196</v>
+        <v>648</v>
       </c>
       <c r="E76" t="s">
-        <v>197</v>
+        <v>648</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="B77" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="C77" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="D77" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="E77" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="B78" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="C78" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="D78" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="E78" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B79" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="C79" t="s">
-        <v>368</v>
+        <v>200</v>
       </c>
       <c r="D79" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="E79" t="s">
-        <v>374</v>
+        <v>202</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>632</v>
+        <v>203</v>
       </c>
       <c r="B80" t="s">
-        <v>633</v>
+        <v>204</v>
       </c>
       <c r="C80" t="s">
-        <v>634</v>
+        <v>205</v>
       </c>
       <c r="D80" t="s">
-        <v>635</v>
+        <v>206</v>
       </c>
       <c r="E80" t="s">
-        <v>635</v>
+        <v>207</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B81" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C81" t="s">
-        <v>213</v>
+        <v>368</v>
       </c>
       <c r="D81" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E81" t="s">
-        <v>215</v>
+        <v>374</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>216</v>
+        <v>632</v>
       </c>
       <c r="B82" t="s">
-        <v>217</v>
+        <v>633</v>
       </c>
       <c r="C82" t="s">
-        <v>218</v>
+        <v>634</v>
       </c>
       <c r="D82" t="s">
-        <v>219</v>
+        <v>635</v>
       </c>
       <c r="E82" t="s">
-        <v>220</v>
+        <v>635</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>438</v>
+        <v>211</v>
       </c>
       <c r="B83" t="s">
-        <v>439</v>
+        <v>212</v>
       </c>
       <c r="C83" t="s">
-        <v>440</v>
+        <v>213</v>
       </c>
       <c r="D83" t="s">
-        <v>441</v>
+        <v>214</v>
       </c>
       <c r="E83" t="s">
-        <v>442</v>
+        <v>215</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="B84" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="C84" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="D84" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="E84" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>310</v>
+        <v>438</v>
       </c>
       <c r="B85" t="s">
-        <v>311</v>
+        <v>439</v>
       </c>
       <c r="C85" t="s">
-        <v>311</v>
+        <v>440</v>
       </c>
       <c r="D85" t="s">
-        <v>456</v>
+        <v>441</v>
       </c>
       <c r="E85" t="s">
-        <v>312</v>
+        <v>442</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>393</v>
+        <v>221</v>
       </c>
       <c r="B86" t="s">
-        <v>313</v>
+        <v>222</v>
       </c>
       <c r="C86" t="s">
-        <v>320</v>
+        <v>223</v>
       </c>
       <c r="D86" t="s">
-        <v>328</v>
+        <v>224</v>
       </c>
       <c r="E86" t="s">
-        <v>337</v>
+        <v>225</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>395</v>
+        <v>310</v>
       </c>
       <c r="B87" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C87" t="s">
-        <v>321</v>
+        <v>311</v>
       </c>
       <c r="D87" t="s">
-        <v>329</v>
+        <v>456</v>
       </c>
       <c r="E87" t="s">
-        <v>329</v>
+        <v>312</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B88" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="C88" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D88" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="E88" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B89" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C89" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D89" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="E89" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="B90" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="C90" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D90" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="E90" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B91" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C91" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D91" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E91" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B92" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C92" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D92" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="E92" t="s">
-        <v>372</v>
+        <v>338</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B93" t="s">
-        <v>407</v>
+        <v>316</v>
       </c>
       <c r="C93" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D93" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E93" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>492</v>
+        <v>399</v>
       </c>
       <c r="B94" t="s">
-        <v>543</v>
+        <v>318</v>
       </c>
       <c r="C94" t="s">
-        <v>521</v>
+        <v>326</v>
       </c>
       <c r="D94" t="s">
-        <v>550</v>
+        <v>334</v>
       </c>
       <c r="E94" t="s">
-        <v>570</v>
+        <v>372</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>495</v>
+        <v>400</v>
       </c>
       <c r="B95" t="s">
-        <v>584</v>
+        <v>407</v>
       </c>
       <c r="C95" t="s">
-        <v>524</v>
+        <v>327</v>
       </c>
       <c r="D95" t="s">
-        <v>585</v>
+        <v>335</v>
       </c>
       <c r="E95" t="s">
-        <v>570</v>
+        <v>340</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>499</v>
+        <v>492</v>
       </c>
       <c r="B96" t="s">
-        <v>573</v>
+        <v>543</v>
       </c>
       <c r="C96" t="s">
-        <v>528</v>
+        <v>521</v>
       </c>
       <c r="D96" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="E96" t="s">
         <v>570</v>
@@ -3980,16 +3998,16 @@
     </row>
     <row r="97" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="B97" t="s">
-        <v>529</v>
+        <v>584</v>
       </c>
       <c r="C97" t="s">
-        <v>529</v>
+        <v>524</v>
       </c>
       <c r="D97" t="s">
-        <v>556</v>
+        <v>585</v>
       </c>
       <c r="E97" t="s">
         <v>570</v>
@@ -3997,16 +4015,16 @@
     </row>
     <row r="98" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B98" t="s">
-        <v>586</v>
+        <v>573</v>
       </c>
       <c r="C98" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="D98" t="s">
-        <v>586</v>
+        <v>555</v>
       </c>
       <c r="E98" t="s">
         <v>570</v>
@@ -4014,16 +4032,16 @@
     </row>
     <row r="99" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>496</v>
+        <v>500</v>
       </c>
       <c r="B99" t="s">
-        <v>574</v>
+        <v>529</v>
       </c>
       <c r="C99" t="s">
-        <v>525</v>
+        <v>529</v>
       </c>
       <c r="D99" t="s">
-        <v>553</v>
+        <v>556</v>
       </c>
       <c r="E99" t="s">
         <v>570</v>
@@ -4031,16 +4049,16 @@
     </row>
     <row r="100" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="B100" t="s">
-        <v>575</v>
+        <v>586</v>
       </c>
       <c r="C100" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="D100" t="s">
-        <v>558</v>
+        <v>586</v>
       </c>
       <c r="E100" t="s">
         <v>570</v>
@@ -4048,16 +4066,16 @@
     </row>
     <row r="101" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>490</v>
+        <v>496</v>
       </c>
       <c r="B101" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="C101" t="s">
-        <v>519</v>
+        <v>525</v>
       </c>
       <c r="D101" t="s">
-        <v>542</v>
+        <v>553</v>
       </c>
       <c r="E101" t="s">
         <v>570</v>
@@ -4065,16 +4083,16 @@
     </row>
     <row r="102" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>493</v>
+        <v>502</v>
       </c>
       <c r="B102" t="s">
-        <v>544</v>
+        <v>575</v>
       </c>
       <c r="C102" t="s">
-        <v>522</v>
+        <v>531</v>
       </c>
       <c r="D102" t="s">
-        <v>551</v>
+        <v>558</v>
       </c>
       <c r="E102" t="s">
         <v>570</v>
@@ -4082,16 +4100,16 @@
     </row>
     <row r="103" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>505</v>
+        <v>490</v>
       </c>
       <c r="B103" t="s">
-        <v>545</v>
+        <v>576</v>
       </c>
       <c r="C103" t="s">
-        <v>534</v>
+        <v>519</v>
       </c>
       <c r="D103" t="s">
-        <v>561</v>
+        <v>542</v>
       </c>
       <c r="E103" t="s">
         <v>570</v>
@@ -4099,16 +4117,16 @@
     </row>
     <row r="104" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>501</v>
+        <v>493</v>
       </c>
       <c r="B104" t="s">
-        <v>577</v>
+        <v>544</v>
       </c>
       <c r="C104" t="s">
-        <v>530</v>
+        <v>522</v>
       </c>
       <c r="D104" t="s">
-        <v>557</v>
+        <v>551</v>
       </c>
       <c r="E104" t="s">
         <v>570</v>
@@ -4116,16 +4134,16 @@
     </row>
     <row r="105" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>497</v>
+        <v>505</v>
       </c>
       <c r="B105" t="s">
-        <v>578</v>
+        <v>545</v>
       </c>
       <c r="C105" t="s">
-        <v>526</v>
+        <v>534</v>
       </c>
       <c r="D105" t="s">
-        <v>554</v>
+        <v>561</v>
       </c>
       <c r="E105" t="s">
         <v>570</v>
@@ -4133,16 +4151,16 @@
     </row>
     <row r="106" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="B106" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="C106" t="s">
-        <v>535</v>
+        <v>530</v>
       </c>
       <c r="D106" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
       <c r="E106" t="s">
         <v>570</v>
@@ -4150,16 +4168,16 @@
     </row>
     <row r="107" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>504</v>
+        <v>497</v>
       </c>
       <c r="B107" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="C107" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
       <c r="D107" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="E107" t="s">
         <v>570</v>
@@ -4167,16 +4185,16 @@
     </row>
     <row r="108" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
       <c r="B108" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="C108" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
       <c r="D108" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="E108" t="s">
         <v>570</v>
@@ -4184,16 +4202,16 @@
     </row>
     <row r="109" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>494</v>
+        <v>504</v>
       </c>
       <c r="B109" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="C109" t="s">
-        <v>523</v>
+        <v>533</v>
       </c>
       <c r="D109" t="s">
-        <v>552</v>
+        <v>560</v>
       </c>
       <c r="E109" t="s">
         <v>570</v>
@@ -4201,16 +4219,16 @@
     </row>
     <row r="110" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>491</v>
+        <v>503</v>
       </c>
       <c r="B110" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="C110" t="s">
-        <v>520</v>
+        <v>532</v>
       </c>
       <c r="D110" t="s">
-        <v>549</v>
+        <v>559</v>
       </c>
       <c r="E110" t="s">
         <v>570</v>
@@ -4218,526 +4236,526 @@
     </row>
     <row r="111" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>226</v>
+        <v>494</v>
       </c>
       <c r="B111" t="s">
-        <v>227</v>
+        <v>582</v>
       </c>
       <c r="C111" t="s">
-        <v>228</v>
+        <v>523</v>
       </c>
       <c r="D111" t="s">
-        <v>229</v>
+        <v>552</v>
       </c>
       <c r="E111" t="s">
-        <v>230</v>
+        <v>570</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>459</v>
+        <v>491</v>
       </c>
       <c r="B112" t="s">
-        <v>234</v>
+        <v>583</v>
       </c>
       <c r="C112" t="s">
-        <v>460</v>
+        <v>520</v>
       </c>
       <c r="D112" t="s">
-        <v>234</v>
+        <v>549</v>
       </c>
       <c r="E112" t="s">
-        <v>234</v>
+        <v>570</v>
       </c>
     </row>
     <row r="113" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="B113" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="C113" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="D113" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="E113" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="114" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>638</v>
+        <v>459</v>
       </c>
       <c r="B114" t="s">
-        <v>640</v>
+        <v>234</v>
       </c>
       <c r="C114" t="s">
-        <v>639</v>
+        <v>460</v>
       </c>
       <c r="D114" t="s">
-        <v>641</v>
+        <v>234</v>
       </c>
       <c r="E114" t="s">
-        <v>642</v>
+        <v>234</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B115" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C115" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="D115" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="E115" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>240</v>
+        <v>638</v>
       </c>
       <c r="B116" t="s">
-        <v>241</v>
+        <v>640</v>
       </c>
       <c r="C116" t="s">
-        <v>242</v>
+        <v>639</v>
       </c>
       <c r="D116" t="s">
-        <v>243</v>
+        <v>641</v>
       </c>
       <c r="E116" t="s">
-        <v>244</v>
+        <v>642</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>623</v>
+        <v>235</v>
       </c>
       <c r="B117" t="s">
-        <v>625</v>
+        <v>236</v>
       </c>
       <c r="C117" t="s">
-        <v>627</v>
+        <v>237</v>
       </c>
       <c r="D117" t="s">
-        <v>626</v>
+        <v>238</v>
       </c>
       <c r="E117" t="s">
-        <v>628</v>
+        <v>239</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>624</v>
+        <v>240</v>
       </c>
       <c r="B118" t="s">
-        <v>629</v>
+        <v>241</v>
       </c>
       <c r="C118" t="s">
-        <v>630</v>
+        <v>242</v>
       </c>
       <c r="D118" t="s">
-        <v>631</v>
+        <v>243</v>
       </c>
       <c r="E118" t="s">
-        <v>570</v>
+        <v>244</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>245</v>
+        <v>623</v>
       </c>
       <c r="B119" t="s">
-        <v>246</v>
+        <v>625</v>
       </c>
       <c r="C119" t="s">
-        <v>247</v>
+        <v>627</v>
       </c>
       <c r="D119" t="s">
-        <v>248</v>
+        <v>626</v>
       </c>
       <c r="E119" t="s">
-        <v>249</v>
+        <v>628</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>413</v>
+        <v>624</v>
       </c>
       <c r="B120" t="s">
-        <v>414</v>
+        <v>629</v>
       </c>
       <c r="C120" t="s">
-        <v>415</v>
+        <v>630</v>
       </c>
       <c r="D120" t="s">
-        <v>416</v>
+        <v>631</v>
       </c>
       <c r="E120" t="s">
-        <v>417</v>
+        <v>570</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="B121" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="C121" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="D121" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="E121" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>341</v>
+        <v>413</v>
       </c>
       <c r="B122" t="s">
-        <v>342</v>
+        <v>414</v>
       </c>
       <c r="C122" t="s">
-        <v>343</v>
+        <v>415</v>
       </c>
       <c r="D122" t="s">
-        <v>342</v>
+        <v>416</v>
       </c>
       <c r="E122" t="s">
-        <v>342</v>
+        <v>417</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>408</v>
+        <v>250</v>
       </c>
       <c r="B123" t="s">
-        <v>409</v>
+        <v>251</v>
       </c>
       <c r="C123" t="s">
-        <v>410</v>
+        <v>252</v>
       </c>
       <c r="D123" t="s">
-        <v>411</v>
+        <v>253</v>
       </c>
       <c r="E123" t="s">
-        <v>412</v>
+        <v>253</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>254</v>
+        <v>341</v>
       </c>
       <c r="B124" t="s">
-        <v>255</v>
+        <v>342</v>
       </c>
       <c r="C124" t="s">
-        <v>256</v>
+        <v>343</v>
       </c>
       <c r="D124" t="s">
-        <v>257</v>
+        <v>342</v>
       </c>
       <c r="E124" t="s">
-        <v>257</v>
+        <v>342</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>258</v>
+        <v>408</v>
       </c>
       <c r="B125" t="s">
-        <v>259</v>
+        <v>409</v>
       </c>
       <c r="C125" t="s">
-        <v>260</v>
+        <v>410</v>
       </c>
       <c r="D125" t="s">
-        <v>261</v>
+        <v>411</v>
       </c>
       <c r="E125" t="s">
-        <v>261</v>
+        <v>412</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>389</v>
+        <v>254</v>
       </c>
       <c r="B126" t="s">
-        <v>390</v>
+        <v>255</v>
       </c>
       <c r="C126" t="s">
-        <v>391</v>
+        <v>256</v>
       </c>
       <c r="D126" t="s">
-        <v>392</v>
+        <v>257</v>
       </c>
       <c r="E126" t="s">
-        <v>392</v>
+        <v>257</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>376</v>
+        <v>258</v>
       </c>
       <c r="B127" t="s">
-        <v>385</v>
+        <v>259</v>
       </c>
       <c r="C127" t="s">
-        <v>386</v>
+        <v>260</v>
       </c>
       <c r="D127" t="s">
-        <v>387</v>
+        <v>261</v>
       </c>
       <c r="E127" t="s">
-        <v>388</v>
+        <v>261</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>375</v>
+        <v>389</v>
       </c>
       <c r="B128" t="s">
-        <v>382</v>
+        <v>390</v>
       </c>
       <c r="C128" t="s">
-        <v>383</v>
+        <v>391</v>
       </c>
       <c r="D128" t="s">
-        <v>384</v>
+        <v>392</v>
       </c>
       <c r="E128" t="s">
-        <v>384</v>
+        <v>392</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B129" t="s">
-        <v>377</v>
+        <v>385</v>
       </c>
       <c r="C129" t="s">
-        <v>379</v>
+        <v>386</v>
       </c>
       <c r="D129" t="s">
-        <v>380</v>
+        <v>387</v>
       </c>
       <c r="E129" t="s">
-        <v>381</v>
+        <v>388</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>262</v>
+        <v>375</v>
       </c>
       <c r="B130" t="s">
-        <v>263</v>
+        <v>382</v>
       </c>
       <c r="C130" t="s">
-        <v>264</v>
+        <v>383</v>
       </c>
       <c r="D130" t="s">
-        <v>265</v>
+        <v>384</v>
       </c>
       <c r="E130" t="s">
-        <v>265</v>
+        <v>384</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>266</v>
+        <v>378</v>
       </c>
       <c r="B131" t="s">
-        <v>267</v>
+        <v>377</v>
       </c>
       <c r="C131" t="s">
-        <v>268</v>
+        <v>379</v>
       </c>
       <c r="D131" t="s">
-        <v>269</v>
+        <v>380</v>
       </c>
       <c r="E131" t="s">
-        <v>269</v>
+        <v>381</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="B132" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="C132" t="s">
-        <v>369</v>
+        <v>264</v>
       </c>
       <c r="D132" t="s">
-        <v>401</v>
+        <v>265</v>
       </c>
       <c r="E132" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>457</v>
+        <v>266</v>
       </c>
       <c r="B133" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="C133" t="s">
-        <v>458</v>
+        <v>268</v>
       </c>
       <c r="D133" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="E133" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
     </row>
     <row r="134" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B134" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C134" t="s">
-        <v>275</v>
+        <v>369</v>
       </c>
       <c r="D134" t="s">
-        <v>276</v>
+        <v>401</v>
       </c>
       <c r="E134" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>277</v>
+        <v>457</v>
       </c>
       <c r="B135" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C135" t="s">
-        <v>279</v>
+        <v>458</v>
       </c>
       <c r="D135" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="E135" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
     </row>
     <row r="136" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="B136" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="C136" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="D136" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="E136" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
     </row>
     <row r="137" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>571</v>
+        <v>277</v>
       </c>
       <c r="B137" t="s">
-        <v>483</v>
+        <v>278</v>
       </c>
       <c r="C137" t="s">
-        <v>483</v>
+        <v>279</v>
       </c>
       <c r="D137" t="s">
-        <v>484</v>
+        <v>280</v>
       </c>
       <c r="E137" t="s">
-        <v>485</v>
+        <v>281</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>572</v>
+        <v>282</v>
       </c>
       <c r="B138" t="s">
-        <v>486</v>
+        <v>283</v>
       </c>
       <c r="C138" t="s">
-        <v>487</v>
+        <v>284</v>
       </c>
       <c r="D138" t="s">
-        <v>488</v>
+        <v>284</v>
       </c>
       <c r="E138" t="s">
-        <v>489</v>
+        <v>284</v>
       </c>
     </row>
     <row r="139" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>514</v>
+        <v>571</v>
       </c>
       <c r="B139" t="s">
-        <v>587</v>
+        <v>483</v>
       </c>
       <c r="C139" t="s">
-        <v>537</v>
+        <v>483</v>
       </c>
       <c r="D139" t="s">
-        <v>568</v>
+        <v>484</v>
       </c>
       <c r="E139" t="s">
-        <v>570</v>
+        <v>485</v>
       </c>
     </row>
     <row r="140" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>512</v>
+        <v>572</v>
       </c>
       <c r="B140" t="s">
-        <v>588</v>
+        <v>486</v>
       </c>
       <c r="C140" t="s">
-        <v>517</v>
+        <v>487</v>
       </c>
       <c r="D140" t="s">
-        <v>566</v>
+        <v>488</v>
       </c>
       <c r="E140" t="s">
-        <v>570</v>
+        <v>489</v>
       </c>
     </row>
     <row r="141" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="B141" t="s">
-        <v>548</v>
+        <v>587</v>
       </c>
       <c r="C141" t="s">
-        <v>518</v>
+        <v>537</v>
       </c>
       <c r="D141" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="E141" t="s">
         <v>570</v>
@@ -4745,16 +4763,16 @@
     </row>
     <row r="142" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>541</v>
+        <v>512</v>
       </c>
       <c r="B142" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C142" t="s">
-        <v>538</v>
+        <v>517</v>
       </c>
       <c r="D142" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="E142" t="s">
         <v>570</v>
@@ -4762,16 +4780,16 @@
     </row>
     <row r="143" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>507</v>
+        <v>513</v>
       </c>
       <c r="B143" t="s">
-        <v>593</v>
+        <v>548</v>
       </c>
       <c r="C143" t="s">
-        <v>540</v>
+        <v>518</v>
       </c>
       <c r="D143" t="s">
-        <v>594</v>
+        <v>567</v>
       </c>
       <c r="E143" t="s">
         <v>570</v>
@@ -4779,16 +4797,16 @@
     </row>
     <row r="144" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>509</v>
+        <v>541</v>
       </c>
       <c r="B144" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C144" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="D144" t="s">
-        <v>564</v>
+        <v>569</v>
       </c>
       <c r="E144" t="s">
         <v>570</v>
@@ -4796,16 +4814,16 @@
     </row>
     <row r="145" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="B145" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
       <c r="C145" t="s">
-        <v>536</v>
+        <v>540</v>
       </c>
       <c r="D145" t="s">
-        <v>565</v>
+        <v>594</v>
       </c>
       <c r="E145" t="s">
         <v>570</v>
@@ -4813,16 +4831,16 @@
     </row>
     <row r="146" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="B146" t="s">
-        <v>546</v>
+        <v>590</v>
       </c>
       <c r="C146" t="s">
-        <v>515</v>
+        <v>539</v>
       </c>
       <c r="D146" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="E146" t="s">
         <v>570</v>
@@ -4830,16 +4848,16 @@
     </row>
     <row r="147" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B147" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C147" t="s">
-        <v>516</v>
+        <v>536</v>
       </c>
       <c r="D147" t="s">
-        <v>547</v>
+        <v>565</v>
       </c>
       <c r="E147" t="s">
         <v>570</v>
@@ -4847,69 +4865,103 @@
     </row>
     <row r="148" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>285</v>
+        <v>508</v>
       </c>
       <c r="B148" t="s">
-        <v>286</v>
+        <v>546</v>
       </c>
       <c r="C148" t="s">
-        <v>287</v>
+        <v>515</v>
       </c>
       <c r="D148" t="s">
-        <v>288</v>
+        <v>563</v>
       </c>
       <c r="E148" t="s">
-        <v>289</v>
+        <v>570</v>
       </c>
     </row>
     <row r="149" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>418</v>
+        <v>511</v>
       </c>
       <c r="B149" t="s">
-        <v>424</v>
+        <v>592</v>
       </c>
       <c r="C149" t="s">
-        <v>421</v>
+        <v>516</v>
       </c>
       <c r="D149" t="s">
-        <v>419</v>
+        <v>547</v>
       </c>
       <c r="E149" t="s">
-        <v>420</v>
+        <v>570</v>
       </c>
     </row>
     <row r="150" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>422</v>
+        <v>285</v>
       </c>
       <c r="B150" t="s">
-        <v>423</v>
+        <v>286</v>
       </c>
       <c r="C150" t="s">
-        <v>425</v>
+        <v>287</v>
       </c>
       <c r="D150" t="s">
-        <v>426</v>
+        <v>288</v>
       </c>
       <c r="E150" t="s">
-        <v>427</v>
+        <v>289</v>
       </c>
     </row>
     <row r="151" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
+        <v>418</v>
+      </c>
+      <c r="B151" t="s">
+        <v>424</v>
+      </c>
+      <c r="C151" t="s">
+        <v>421</v>
+      </c>
+      <c r="D151" t="s">
+        <v>419</v>
+      </c>
+      <c r="E151" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>422</v>
+      </c>
+      <c r="B152" t="s">
+        <v>423</v>
+      </c>
+      <c r="C152" t="s">
+        <v>425</v>
+      </c>
+      <c r="D152" t="s">
+        <v>426</v>
+      </c>
+      <c r="E152" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
         <v>344</v>
       </c>
-      <c r="B151" t="s">
+      <c r="B153" t="s">
         <v>346</v>
       </c>
-      <c r="C151" t="s">
+      <c r="C153" t="s">
         <v>348</v>
       </c>
-      <c r="D151" t="s">
+      <c r="D153" t="s">
         <v>350</v>
       </c>
-      <c r="E151" t="s">
+      <c r="E153" t="s">
         <v>352</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Rename "oral" to "speaking"
</commit_message>
<xml_diff>
--- a/assets/Localizations.xlsx
+++ b/assets/Localizations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Graded\Graded - Flutter\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2AE1D15-BBDC-4DC5-9753-D18AFAC41BE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF0F94C3-6BED-4766-8E6A-F56AC086C7F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="649">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="650">
   <si>
     <t>keys</t>
   </si>
@@ -1954,22 +1954,25 @@
     <t>Feedback ginn</t>
   </si>
   <si>
-    <t>oral</t>
-  </si>
-  <si>
     <t>Oral</t>
   </si>
   <si>
-    <t>oral_weight</t>
-  </si>
-  <si>
-    <t>Oral weight</t>
-  </si>
-  <si>
     <t>Coefficient d'oral</t>
   </si>
   <si>
     <t>Oral Koeffizient</t>
+  </si>
+  <si>
+    <t>speaking</t>
+  </si>
+  <si>
+    <t>Speaking</t>
+  </si>
+  <si>
+    <t>speaking_weight</t>
+  </si>
+  <si>
+    <t>Speaking weight</t>
   </si>
 </sst>
 </file>
@@ -2351,8 +2354,8 @@
   </sheetPr>
   <dimension ref="A1:E153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
-      <selection activeCell="E153" sqref="E153"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3624,373 +3627,373 @@
     </row>
     <row r="75" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>643</v>
+        <v>188</v>
       </c>
       <c r="B75" t="s">
-        <v>644</v>
+        <v>189</v>
       </c>
       <c r="C75" t="s">
-        <v>644</v>
+        <v>190</v>
       </c>
       <c r="D75" t="s">
-        <v>644</v>
+        <v>191</v>
       </c>
       <c r="E75" t="s">
-        <v>644</v>
+        <v>192</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>645</v>
+        <v>193</v>
       </c>
       <c r="B76" t="s">
-        <v>646</v>
+        <v>194</v>
       </c>
       <c r="C76" t="s">
-        <v>647</v>
+        <v>195</v>
       </c>
       <c r="D76" t="s">
-        <v>648</v>
+        <v>196</v>
       </c>
       <c r="E76" t="s">
-        <v>648</v>
+        <v>197</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="B77" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="C77" t="s">
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="D77" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
       <c r="E77" t="s">
-        <v>192</v>
+        <v>202</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>193</v>
+        <v>203</v>
       </c>
       <c r="B78" t="s">
-        <v>194</v>
+        <v>204</v>
       </c>
       <c r="C78" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="D78" t="s">
-        <v>196</v>
+        <v>206</v>
       </c>
       <c r="E78" t="s">
-        <v>197</v>
+        <v>207</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="B79" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="C79" t="s">
-        <v>200</v>
+        <v>368</v>
       </c>
       <c r="D79" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="E79" t="s">
-        <v>202</v>
+        <v>374</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>203</v>
+        <v>632</v>
       </c>
       <c r="B80" t="s">
-        <v>204</v>
+        <v>633</v>
       </c>
       <c r="C80" t="s">
-        <v>205</v>
+        <v>634</v>
       </c>
       <c r="D80" t="s">
-        <v>206</v>
+        <v>635</v>
       </c>
       <c r="E80" t="s">
-        <v>207</v>
+        <v>635</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B81" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="C81" t="s">
-        <v>368</v>
+        <v>213</v>
       </c>
       <c r="D81" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="E81" t="s">
-        <v>374</v>
+        <v>215</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>632</v>
+        <v>216</v>
       </c>
       <c r="B82" t="s">
-        <v>633</v>
+        <v>217</v>
       </c>
       <c r="C82" t="s">
-        <v>634</v>
+        <v>218</v>
       </c>
       <c r="D82" t="s">
-        <v>635</v>
+        <v>219</v>
       </c>
       <c r="E82" t="s">
-        <v>635</v>
+        <v>220</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>211</v>
+        <v>438</v>
       </c>
       <c r="B83" t="s">
-        <v>212</v>
+        <v>439</v>
       </c>
       <c r="C83" t="s">
-        <v>213</v>
+        <v>440</v>
       </c>
       <c r="D83" t="s">
-        <v>214</v>
+        <v>441</v>
       </c>
       <c r="E83" t="s">
-        <v>215</v>
+        <v>442</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="B84" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="C84" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="D84" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="E84" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>438</v>
+        <v>310</v>
       </c>
       <c r="B85" t="s">
-        <v>439</v>
+        <v>311</v>
       </c>
       <c r="C85" t="s">
-        <v>440</v>
+        <v>311</v>
       </c>
       <c r="D85" t="s">
-        <v>441</v>
+        <v>456</v>
       </c>
       <c r="E85" t="s">
-        <v>442</v>
+        <v>312</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>221</v>
+        <v>393</v>
       </c>
       <c r="B86" t="s">
-        <v>222</v>
+        <v>313</v>
       </c>
       <c r="C86" t="s">
-        <v>223</v>
+        <v>320</v>
       </c>
       <c r="D86" t="s">
-        <v>224</v>
+        <v>328</v>
       </c>
       <c r="E86" t="s">
-        <v>225</v>
+        <v>337</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>310</v>
+        <v>395</v>
       </c>
       <c r="B87" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="C87" t="s">
-        <v>311</v>
+        <v>321</v>
       </c>
       <c r="D87" t="s">
-        <v>456</v>
+        <v>329</v>
       </c>
       <c r="E87" t="s">
-        <v>312</v>
+        <v>329</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B88" t="s">
-        <v>313</v>
+        <v>319</v>
       </c>
       <c r="C88" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="D88" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="E88" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B89" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="C89" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="D89" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="E89" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="B90" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="C90" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="D90" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E90" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="B91" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C91" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="D91" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="E91" t="s">
-        <v>332</v>
+        <v>339</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="B92" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="C92" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="D92" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="E92" t="s">
-        <v>338</v>
+        <v>372</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="B93" t="s">
-        <v>316</v>
+        <v>407</v>
       </c>
       <c r="C93" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="D93" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="E93" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>399</v>
+        <v>492</v>
       </c>
       <c r="B94" t="s">
-        <v>318</v>
+        <v>543</v>
       </c>
       <c r="C94" t="s">
-        <v>326</v>
+        <v>521</v>
       </c>
       <c r="D94" t="s">
-        <v>334</v>
+        <v>550</v>
       </c>
       <c r="E94" t="s">
-        <v>372</v>
+        <v>570</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>400</v>
+        <v>495</v>
       </c>
       <c r="B95" t="s">
-        <v>407</v>
+        <v>584</v>
       </c>
       <c r="C95" t="s">
-        <v>327</v>
+        <v>524</v>
       </c>
       <c r="D95" t="s">
-        <v>335</v>
+        <v>585</v>
       </c>
       <c r="E95" t="s">
-        <v>340</v>
+        <v>570</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>492</v>
+        <v>499</v>
       </c>
       <c r="B96" t="s">
-        <v>543</v>
+        <v>573</v>
       </c>
       <c r="C96" t="s">
-        <v>521</v>
+        <v>528</v>
       </c>
       <c r="D96" t="s">
-        <v>550</v>
+        <v>555</v>
       </c>
       <c r="E96" t="s">
         <v>570</v>
@@ -3998,16 +4001,16 @@
     </row>
     <row r="97" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>495</v>
+        <v>500</v>
       </c>
       <c r="B97" t="s">
-        <v>584</v>
+        <v>529</v>
       </c>
       <c r="C97" t="s">
-        <v>524</v>
+        <v>529</v>
       </c>
       <c r="D97" t="s">
-        <v>585</v>
+        <v>556</v>
       </c>
       <c r="E97" t="s">
         <v>570</v>
@@ -4015,16 +4018,16 @@
     </row>
     <row r="98" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B98" t="s">
-        <v>573</v>
+        <v>586</v>
       </c>
       <c r="C98" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D98" t="s">
-        <v>555</v>
+        <v>586</v>
       </c>
       <c r="E98" t="s">
         <v>570</v>
@@ -4032,16 +4035,16 @@
     </row>
     <row r="99" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="B99" t="s">
-        <v>529</v>
+        <v>574</v>
       </c>
       <c r="C99" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="D99" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="E99" t="s">
         <v>570</v>
@@ -4049,16 +4052,16 @@
     </row>
     <row r="100" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>498</v>
+        <v>502</v>
       </c>
       <c r="B100" t="s">
-        <v>586</v>
+        <v>575</v>
       </c>
       <c r="C100" t="s">
-        <v>527</v>
+        <v>531</v>
       </c>
       <c r="D100" t="s">
-        <v>586</v>
+        <v>558</v>
       </c>
       <c r="E100" t="s">
         <v>570</v>
@@ -4066,16 +4069,16 @@
     </row>
     <row r="101" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>496</v>
+        <v>490</v>
       </c>
       <c r="B101" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
       <c r="C101" t="s">
-        <v>525</v>
+        <v>519</v>
       </c>
       <c r="D101" t="s">
-        <v>553</v>
+        <v>542</v>
       </c>
       <c r="E101" t="s">
         <v>570</v>
@@ -4083,16 +4086,16 @@
     </row>
     <row r="102" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>502</v>
+        <v>493</v>
       </c>
       <c r="B102" t="s">
-        <v>575</v>
+        <v>544</v>
       </c>
       <c r="C102" t="s">
-        <v>531</v>
+        <v>522</v>
       </c>
       <c r="D102" t="s">
-        <v>558</v>
+        <v>551</v>
       </c>
       <c r="E102" t="s">
         <v>570</v>
@@ -4100,16 +4103,16 @@
     </row>
     <row r="103" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>490</v>
+        <v>505</v>
       </c>
       <c r="B103" t="s">
-        <v>576</v>
+        <v>545</v>
       </c>
       <c r="C103" t="s">
-        <v>519</v>
+        <v>534</v>
       </c>
       <c r="D103" t="s">
-        <v>542</v>
+        <v>561</v>
       </c>
       <c r="E103" t="s">
         <v>570</v>
@@ -4117,16 +4120,16 @@
     </row>
     <row r="104" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>493</v>
+        <v>501</v>
       </c>
       <c r="B104" t="s">
-        <v>544</v>
+        <v>577</v>
       </c>
       <c r="C104" t="s">
-        <v>522</v>
+        <v>530</v>
       </c>
       <c r="D104" t="s">
-        <v>551</v>
+        <v>557</v>
       </c>
       <c r="E104" t="s">
         <v>570</v>
@@ -4134,16 +4137,16 @@
     </row>
     <row r="105" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>505</v>
+        <v>497</v>
       </c>
       <c r="B105" t="s">
-        <v>545</v>
+        <v>578</v>
       </c>
       <c r="C105" t="s">
-        <v>534</v>
+        <v>526</v>
       </c>
       <c r="D105" t="s">
-        <v>561</v>
+        <v>554</v>
       </c>
       <c r="E105" t="s">
         <v>570</v>
@@ -4151,16 +4154,16 @@
     </row>
     <row r="106" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>501</v>
+        <v>506</v>
       </c>
       <c r="B106" t="s">
-        <v>577</v>
+        <v>579</v>
       </c>
       <c r="C106" t="s">
-        <v>530</v>
+        <v>535</v>
       </c>
       <c r="D106" t="s">
-        <v>557</v>
+        <v>562</v>
       </c>
       <c r="E106" t="s">
         <v>570</v>
@@ -4168,16 +4171,16 @@
     </row>
     <row r="107" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>497</v>
+        <v>504</v>
       </c>
       <c r="B107" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="C107" t="s">
-        <v>526</v>
+        <v>533</v>
       </c>
       <c r="D107" t="s">
-        <v>554</v>
+        <v>560</v>
       </c>
       <c r="E107" t="s">
         <v>570</v>
@@ -4185,16 +4188,16 @@
     </row>
     <row r="108" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="B108" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
       <c r="C108" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="D108" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="E108" t="s">
         <v>570</v>
@@ -4202,16 +4205,16 @@
     </row>
     <row r="109" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>504</v>
+        <v>494</v>
       </c>
       <c r="B109" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="C109" t="s">
-        <v>533</v>
+        <v>523</v>
       </c>
       <c r="D109" t="s">
-        <v>560</v>
+        <v>552</v>
       </c>
       <c r="E109" t="s">
         <v>570</v>
@@ -4219,16 +4222,16 @@
     </row>
     <row r="110" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>503</v>
+        <v>491</v>
       </c>
       <c r="B110" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
       <c r="C110" t="s">
-        <v>532</v>
+        <v>520</v>
       </c>
       <c r="D110" t="s">
-        <v>559</v>
+        <v>549</v>
       </c>
       <c r="E110" t="s">
         <v>570</v>
@@ -4236,189 +4239,189 @@
     </row>
     <row r="111" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>494</v>
+        <v>226</v>
       </c>
       <c r="B111" t="s">
-        <v>582</v>
+        <v>227</v>
       </c>
       <c r="C111" t="s">
-        <v>523</v>
+        <v>228</v>
       </c>
       <c r="D111" t="s">
-        <v>552</v>
+        <v>229</v>
       </c>
       <c r="E111" t="s">
-        <v>570</v>
+        <v>230</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>491</v>
+        <v>459</v>
       </c>
       <c r="B112" t="s">
-        <v>583</v>
+        <v>234</v>
       </c>
       <c r="C112" t="s">
-        <v>520</v>
+        <v>460</v>
       </c>
       <c r="D112" t="s">
-        <v>549</v>
+        <v>234</v>
       </c>
       <c r="E112" t="s">
-        <v>570</v>
+        <v>234</v>
       </c>
     </row>
     <row r="113" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="B113" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="C113" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="D113" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="E113" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
     </row>
     <row r="114" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>459</v>
+        <v>638</v>
       </c>
       <c r="B114" t="s">
-        <v>234</v>
+        <v>640</v>
       </c>
       <c r="C114" t="s">
-        <v>460</v>
+        <v>639</v>
       </c>
       <c r="D114" t="s">
-        <v>234</v>
+        <v>641</v>
       </c>
       <c r="E114" t="s">
-        <v>234</v>
+        <v>642</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="B115" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="C115" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="D115" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="E115" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>638</v>
+        <v>240</v>
       </c>
       <c r="B116" t="s">
-        <v>640</v>
+        <v>241</v>
       </c>
       <c r="C116" t="s">
-        <v>639</v>
+        <v>242</v>
       </c>
       <c r="D116" t="s">
-        <v>641</v>
+        <v>243</v>
       </c>
       <c r="E116" t="s">
-        <v>642</v>
+        <v>244</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>235</v>
+        <v>623</v>
       </c>
       <c r="B117" t="s">
-        <v>236</v>
+        <v>625</v>
       </c>
       <c r="C117" t="s">
-        <v>237</v>
+        <v>627</v>
       </c>
       <c r="D117" t="s">
-        <v>238</v>
+        <v>626</v>
       </c>
       <c r="E117" t="s">
-        <v>239</v>
+        <v>628</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>240</v>
+        <v>624</v>
       </c>
       <c r="B118" t="s">
-        <v>241</v>
+        <v>629</v>
       </c>
       <c r="C118" t="s">
-        <v>242</v>
+        <v>630</v>
       </c>
       <c r="D118" t="s">
-        <v>243</v>
+        <v>631</v>
       </c>
       <c r="E118" t="s">
-        <v>244</v>
+        <v>570</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>623</v>
+        <v>245</v>
       </c>
       <c r="B119" t="s">
-        <v>625</v>
+        <v>246</v>
       </c>
       <c r="C119" t="s">
-        <v>627</v>
+        <v>247</v>
       </c>
       <c r="D119" t="s">
-        <v>626</v>
+        <v>248</v>
       </c>
       <c r="E119" t="s">
-        <v>628</v>
+        <v>249</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>624</v>
+        <v>646</v>
       </c>
       <c r="B120" t="s">
-        <v>629</v>
+        <v>647</v>
       </c>
       <c r="C120" t="s">
-        <v>630</v>
+        <v>643</v>
       </c>
       <c r="D120" t="s">
-        <v>631</v>
+        <v>643</v>
       </c>
       <c r="E120" t="s">
-        <v>570</v>
+        <v>643</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>245</v>
+        <v>648</v>
       </c>
       <c r="B121" t="s">
-        <v>246</v>
+        <v>649</v>
       </c>
       <c r="C121" t="s">
-        <v>247</v>
+        <v>644</v>
       </c>
       <c r="D121" t="s">
-        <v>248</v>
+        <v>645</v>
       </c>
       <c r="E121" t="s">
-        <v>249</v>
+        <v>645</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>